<commit_message>
Restructured Definitions - better access to data
Restructured Definitions - better access to data
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="All Topics" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="191">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -571,12 +569,45 @@
   <si>
     <t>Bootstrap</t>
   </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Excel Sheet Name</t>
+  </si>
+  <si>
+    <t>2_Definitions.xlsx</t>
+  </si>
+  <si>
+    <t>3_Definitions.xlsx</t>
+  </si>
+  <si>
+    <t>Ionic</t>
+  </si>
+  <si>
+    <t>Phone Gap</t>
+  </si>
+  <si>
+    <t>Node JS</t>
+  </si>
+  <si>
+    <t>Spring REST</t>
+  </si>
+  <si>
+    <t>SPA</t>
+  </si>
+  <si>
+    <t>Cordova</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,8 +637,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,8 +665,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -676,25 +733,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -718,14 +762,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,701 +1072,849 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" customWidth="1"/>
-    <col min="2" max="2" width="96.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="60">
-      <c r="A10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="45">
-      <c r="A11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="45">
-      <c r="A18" s="1" t="s">
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" ht="45">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45">
+      <c r="A22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="30">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" ht="60">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60">
+      <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="6" t="s">
+      <c r="C32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="6" t="s">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="6" t="s">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="6" t="s">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="6" t="s">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="6" t="s">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="6" t="s">
+      <c r="C39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="6" t="s">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="6" t="s">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="6" t="s">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="6" t="s">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="6" t="s">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="6" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="6" t="s">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="6" t="s">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="6" t="s">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="6" t="s">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="6" t="s">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30">
-      <c r="A52" s="6" t="s">
+    <row r="53" spans="1:3" ht="30">
+      <c r="A53" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="75">
-      <c r="A53" s="6" t="s">
+    <row r="54" spans="1:3" ht="75">
+      <c r="A54" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="6" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="6" t="s">
+      <c r="C55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="6" t="s">
+      <c r="C56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="6" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="6" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="6" t="s">
+      <c r="C59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="6" t="s">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="6" t="s">
+      <c r="C61" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="6" t="s">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="6" t="s">
+      <c r="C63" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="6" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="6" t="s">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" ht="30">
-      <c r="A66" s="6" t="s">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="6" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="6" t="s">
+      <c r="B68" s="2"/>
+      <c r="C68" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="6" t="s">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="6" t="s">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="6" t="s">
+      <c r="B71" s="2"/>
+      <c r="C71" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="6" t="s">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="6" t="s">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="6" t="s">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="6" t="s">
+    <row r="76" spans="1:3">
+      <c r="A76" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="6" t="s">
+    <row r="77" spans="1:3">
+      <c r="A77" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="6" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="6" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="6" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="6" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="6" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="6" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="9" t="s">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="10"/>
-      <c r="B85" s="3" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" s="13"/>
+      <c r="B86" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="6" t="s">
+    <row r="87" spans="1:3">
+      <c r="A87" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="6" t="s">
+      <c r="C87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="6" t="s">
+      <c r="C88" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="6" t="s">
+    <row r="90" spans="1:3">
+      <c r="A90" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="30">
-      <c r="A90" s="6" t="s">
+    <row r="91" spans="1:3" ht="30">
+      <c r="A91" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="6" t="s">
+    <row r="92" spans="1:3">
+      <c r="A92" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="6" t="s">
+      <c r="C92" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:3">
+      <c r="A94" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="6" t="s">
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B94" s="2"/>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="6" t="s">
+      <c r="B95" s="2"/>
+      <c r="C95" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B95" s="2"/>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="6" t="s">
+      <c r="B96" s="2"/>
+      <c r="C96" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="6" t="s">
+      <c r="B97" s="2"/>
+      <c r="C97" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B97" s="2"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="6" t="s">
         <v>143</v>
       </c>
@@ -1724,43 +1922,43 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:3">
       <c r="A100" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:3">
       <c r="A101" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:3">
       <c r="A102" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:3">
       <c r="A103" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:3">
       <c r="A104" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:3">
       <c r="A105" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B105" s="2"/>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:3">
       <c r="A106" s="6" t="s">
         <v>149</v>
       </c>
@@ -1768,7 +1966,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="30">
+    <row r="107" spans="1:3" ht="30">
       <c r="A107" s="6" t="s">
         <v>151</v>
       </c>
@@ -1776,208 +1974,231 @@
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:3">
       <c r="A108" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:3">
       <c r="A109" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:3">
       <c r="A110" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:3">
       <c r="A111" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="11" t="s">
+    <row r="112" spans="1:3">
+      <c r="A112" s="6" t="s">
         <v>157</v>
       </c>
       <c r="B112" s="3"/>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="11" t="s">
+    <row r="113" spans="1:3">
+      <c r="A113" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B113" s="3"/>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="11" t="s">
+    <row r="114" spans="1:3">
+      <c r="A114" s="6" t="s">
         <v>159</v>
       </c>
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="11" t="s">
+    <row r="115" spans="1:3">
+      <c r="A115" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="11" t="s">
+    <row r="116" spans="1:3">
+      <c r="A116" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B116" s="3"/>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="11" t="s">
+    <row r="117" spans="1:3">
+      <c r="A117" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B117" s="3"/>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="11" t="s">
+    <row r="118" spans="1:3">
+      <c r="A118" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="11" t="s">
+      <c r="C118" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B119" s="3"/>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="11" t="s">
+    <row r="120" spans="1:3">
+      <c r="A120" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="11" t="s">
+    <row r="121" spans="1:3">
+      <c r="A121" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B121" s="2"/>
     </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="11" t="s">
+    <row r="122" spans="1:3">
+      <c r="A122" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="11" t="s">
+    <row r="123" spans="1:3">
+      <c r="A123" s="6" t="s">
         <v>169</v>
       </c>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="11" t="s">
+    <row r="124" spans="1:3">
+      <c r="A124" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="11" t="s">
+    <row r="125" spans="1:3">
+      <c r="A125" s="6" t="s">
         <v>171</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="11" t="s">
+    <row r="126" spans="1:3">
+      <c r="A126" s="6" t="s">
         <v>173</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="11" t="s">
+    <row r="127" spans="1:3">
+      <c r="A127" s="6" t="s">
         <v>175</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="11" t="s">
+      <c r="C127" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="11" t="s">
+    <row r="129" spans="1:3">
+      <c r="A129" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130" s="2"/>
+      <c r="C130" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B131" s="2"/>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="6" t="s">
+        <v>189</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A85:A86"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B84" r:id="rId2"/>
-    <hyperlink ref="B87" r:id="rId3"/>
-    <hyperlink ref="B88" r:id="rId4"/>
-    <hyperlink ref="B89" r:id="rId5"/>
-    <hyperlink ref="B90" r:id="rId6"/>
-    <hyperlink ref="B91" r:id="rId7"/>
-    <hyperlink ref="B66" r:id="rId8"/>
-    <hyperlink ref="B76" r:id="rId9"/>
-    <hyperlink ref="B62" r:id="rId10"/>
-    <hyperlink ref="B55" r:id="rId11"/>
-    <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B57" r:id="rId13"/>
-    <hyperlink ref="B92" r:id="rId14"/>
-    <hyperlink ref="B86" r:id="rId15"/>
-    <hyperlink ref="B79" r:id="rId16"/>
-    <hyperlink ref="B31" r:id="rId17"/>
-    <hyperlink ref="B52" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
-    <hyperlink ref="B51" r:id="rId19"/>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B85" r:id="rId2"/>
+    <hyperlink ref="B88" r:id="rId3"/>
+    <hyperlink ref="B89" r:id="rId4"/>
+    <hyperlink ref="B90" r:id="rId5"/>
+    <hyperlink ref="B91" r:id="rId6"/>
+    <hyperlink ref="B92" r:id="rId7"/>
+    <hyperlink ref="B67" r:id="rId8"/>
+    <hyperlink ref="B77" r:id="rId9"/>
+    <hyperlink ref="B63" r:id="rId10"/>
+    <hyperlink ref="B56" r:id="rId11"/>
+    <hyperlink ref="B18" r:id="rId12"/>
+    <hyperlink ref="B58" r:id="rId13"/>
+    <hyperlink ref="B93" r:id="rId14"/>
+    <hyperlink ref="B87" r:id="rId15"/>
+    <hyperlink ref="B80" r:id="rId16"/>
+    <hyperlink ref="B32" r:id="rId17"/>
+    <hyperlink ref="B53" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
+    <hyperlink ref="B52" r:id="rId19"/>
     <hyperlink ref="B106" r:id="rId20"/>
     <hyperlink ref="B107" r:id="rId21"/>
-    <hyperlink ref="B45" r:id="rId22"/>
-    <hyperlink ref="B41" r:id="rId23"/>
+    <hyperlink ref="B46" r:id="rId22"/>
+    <hyperlink ref="B42" r:id="rId23"/>
     <hyperlink ref="B120" r:id="rId24"/>
-    <hyperlink ref="B75" r:id="rId25"/>
+    <hyperlink ref="B76" r:id="rId25"/>
     <hyperlink ref="B125" r:id="rId26"/>
     <hyperlink ref="B126" r:id="rId27" location="commandLine"/>
     <hyperlink ref="B127" r:id="rId28"/>
-    <hyperlink ref="B85" r:id="rId29"/>
+    <hyperlink ref="B86" r:id="rId29"/>
     <hyperlink ref="B128" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JAXB, Rest web services
JAXB, Rest web services
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1135,8 +1135,8 @@
   <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Spring Java Based Configuration, Cassandra
Spring Java Based Configuration, Cassandra
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="214">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -668,6 +668,9 @@
   </si>
   <si>
     <t>Mockito</t>
+  </si>
+  <si>
+    <t>Apache Cassandra</t>
   </si>
 </sst>
 </file>
@@ -805,7 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +841,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1149,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C109" sqref="C109"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1464,7 +1468,7 @@
       <c r="B31" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="24" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1475,7 +1479,7 @@
       <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="23"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
@@ -1859,7 +1863,7 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="21" t="s">
+      <c r="A87" s="22" t="s">
         <v>119</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -1867,7 +1871,7 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="22"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="3" t="s">
         <v>121</v>
       </c>
@@ -1982,331 +1986,340 @@
         <v>143</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" s="21" customFormat="1">
       <c r="A102" s="5" t="s">
-        <v>144</v>
+        <v>213</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="21" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" s="15" customFormat="1">
-      <c r="A104" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:3" s="15" customFormat="1">
       <c r="A105" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:3" s="15" customFormat="1">
       <c r="A106" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:3" s="15" customFormat="1">
       <c r="A107" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="1:3" s="15" customFormat="1">
+      <c r="A108" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C108" s="14" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C109" s="20" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
-        <v>60</v>
+        <v>146</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="30">
-      <c r="A113" s="5" t="s">
+    <row r="114" spans="1:3" ht="30">
+      <c r="A114" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B115" s="3"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B116" s="3"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B117" s="3"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B119" s="3"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B123" s="3"/>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B124" s="3"/>
-      <c r="C124" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B125" s="3"/>
+      <c r="C125" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>164</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B126" s="3"/>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C135" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
-        <v>185</v>
+        <v>141</v>
+      </c>
+      <c r="C136" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C143" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="30">
-      <c r="A144" s="5" t="s">
+      <c r="C144" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="30">
+      <c r="A145" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C145" s="10" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C146" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C146" s="10" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C147" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C147" s="12" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C148" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C148" s="13" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C149" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C149" s="16" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C150" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C150" s="17" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C151" s="19" t="s">
+      <c r="C152" s="19" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2335,24 +2348,24 @@
     <hyperlink ref="B35" r:id="rId17"/>
     <hyperlink ref="B56" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
     <hyperlink ref="B55" r:id="rId19"/>
-    <hyperlink ref="B112" r:id="rId20"/>
-    <hyperlink ref="B113" r:id="rId21"/>
+    <hyperlink ref="B113" r:id="rId20"/>
+    <hyperlink ref="B114" r:id="rId21"/>
     <hyperlink ref="B49" r:id="rId22"/>
     <hyperlink ref="B45" r:id="rId23"/>
-    <hyperlink ref="B126" r:id="rId24"/>
+    <hyperlink ref="B127" r:id="rId24"/>
     <hyperlink ref="B79" r:id="rId25"/>
-    <hyperlink ref="B131" r:id="rId26"/>
-    <hyperlink ref="B132" r:id="rId27" location="commandLine"/>
+    <hyperlink ref="B132" r:id="rId26"/>
+    <hyperlink ref="B133" r:id="rId27" location="commandLine"/>
     <hyperlink ref="B30" r:id="rId28"/>
     <hyperlink ref="B88" r:id="rId29"/>
-    <hyperlink ref="B133" r:id="rId30"/>
+    <hyperlink ref="B134" r:id="rId30"/>
     <hyperlink ref="B78" r:id="rId31"/>
-    <hyperlink ref="B142" r:id="rId32"/>
+    <hyperlink ref="B143" r:id="rId32"/>
     <hyperlink ref="B31" r:id="rId33"/>
     <hyperlink ref="B29" r:id="rId34"/>
     <hyperlink ref="B33" r:id="rId35"/>
-    <hyperlink ref="B144" r:id="rId36"/>
-    <hyperlink ref="B107" r:id="rId37"/>
+    <hyperlink ref="B145" r:id="rId36"/>
+    <hyperlink ref="B108" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>

</xml_diff>

<commit_message>
Web Services - SOAP and REST
Web Services - SOAP and REST
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -194,12 +194,6 @@
   </si>
   <si>
     <t>RESTful web service</t>
-  </si>
-  <si>
-    <t>http://www.tutorialspoint.com/restful/index.htm</t>
-  </si>
-  <si>
-    <t>SOAP Web Services Advanced topics</t>
   </si>
   <si>
     <t>Clustering</t>
@@ -588,9 +582,6 @@
     <t>Node JS</t>
   </si>
   <si>
-    <t>Spring REST</t>
-  </si>
-  <si>
     <t>SPA</t>
   </si>
   <si>
@@ -661,9 +652,6 @@
     <t>MongoDB</t>
   </si>
   <si>
-    <t xml:space="preserve">Jersey - RESTful web services implementation </t>
-  </si>
-  <si>
     <t>Junit</t>
   </si>
   <si>
@@ -683,6 +671,9 @@
   </si>
   <si>
     <t>8_Definitions_Angular_JS.xlsx</t>
+  </si>
+  <si>
+    <t>9_Definitions_Web_Services.xlsx</t>
   </si>
 </sst>
 </file>
@@ -820,7 +811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -853,6 +844,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1171,11 +1163,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1187,13 +1179,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1204,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
@@ -1215,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1226,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1234,7 +1226,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1245,7 +1237,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1256,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1267,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -1275,7 +1267,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
@@ -1286,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="60">
@@ -1297,7 +1289,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45">
@@ -1308,7 +1300,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1319,924 +1311,914 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="28" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>216</v>
+        <v>56</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="28" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>181</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="45">
-      <c r="A19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="45">
-      <c r="A22" s="4" t="s">
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30">
-      <c r="A27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30">
+      <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="60">
-      <c r="A28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="60">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="B30" s="3" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
-        <v>197</v>
+      <c r="A31" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>182</v>
+        <v>172</v>
+      </c>
+      <c r="C31" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="30"/>
+        <v>194</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="A33" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C35" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="3"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>215</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="A47" s="5"/>
+      <c r="C47" s="28"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>182</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30">
+      <c r="A57" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="30">
-      <c r="A56" s="5" t="s">
+    <row r="58" spans="1:3" ht="75">
+      <c r="A58" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B58" s="6" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="75">
-      <c r="A57" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="C60" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" t="s">
-        <v>181</v>
+        <v>76</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C63" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>214</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" t="s">
-        <v>181</v>
+        <v>90</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C71" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="C74" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="30">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C78" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>98</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="30">
       <c r="A79" s="5" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>103</v>
+        <v>186</v>
+      </c>
+      <c r="C79" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="28" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" s="30"/>
+      <c r="B89" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="29"/>
-      <c r="B88" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C90" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="C91" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30">
+      <c r="A94" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="30">
-      <c r="A93" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C94" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="C95" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C97" t="s">
-        <v>181</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C98" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C99" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C100" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" s="20" customFormat="1">
+        <v>138</v>
+      </c>
+      <c r="C101" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>140</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" s="20" customFormat="1">
       <c r="A103" s="5" t="s">
-        <v>144</v>
+        <v>209</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="20" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" s="14" customFormat="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B105" s="2"/>
+        <v>143</v>
+      </c>
     </row>
     <row r="106" spans="1:3" s="14" customFormat="1">
       <c r="A106" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:3" s="14" customFormat="1">
       <c r="A107" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:3" s="14" customFormat="1">
       <c r="A108" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B108" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C108" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:3" s="14" customFormat="1">
       <c r="A109" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C110" s="19" t="s">
-        <v>182</v>
+        <v>199</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
-        <v>60</v>
+        <v>144</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30">
+      <c r="A115" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="30">
-      <c r="A114" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B115" s="3"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B116" s="3"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B117" s="3"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B119" s="3"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B123" s="3"/>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B124" s="3"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B125" s="3"/>
-      <c r="C125" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B126" s="3"/>
+      <c r="C126" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>164</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B127" s="3"/>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C136" s="27" t="s">
-        <v>217</v>
+        <v>175</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
-        <v>185</v>
+        <v>139</v>
+      </c>
+      <c r="C137" s="27" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2246,147 +2228,147 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C145" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="30">
+      <c r="A146" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C144" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="30">
-      <c r="A145" s="5" t="s">
+      <c r="B146" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C146" s="10" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C147" s="12" t="s">
-        <v>182</v>
+        <v>196</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C148" s="24" t="s">
-        <v>214</v>
+        <v>197</v>
+      </c>
+      <c r="C148" s="12" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>182</v>
+        <v>198</v>
+      </c>
+      <c r="C149" s="24" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>182</v>
+        <v>205</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C151" s="17" t="s">
-        <v>182</v>
+        <v>206</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C152" s="18" t="s">
-        <v>182</v>
+        <v>207</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C153" s="18" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B87" r:id="rId2"/>
-    <hyperlink ref="B90" r:id="rId3"/>
-    <hyperlink ref="B91" r:id="rId4"/>
-    <hyperlink ref="B92" r:id="rId5"/>
-    <hyperlink ref="B93" r:id="rId6"/>
-    <hyperlink ref="B94" r:id="rId7"/>
-    <hyperlink ref="B69" r:id="rId8"/>
-    <hyperlink ref="B80" r:id="rId9"/>
-    <hyperlink ref="B65" r:id="rId10"/>
-    <hyperlink ref="B58" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B60" r:id="rId13"/>
-    <hyperlink ref="B95" r:id="rId14"/>
-    <hyperlink ref="B89" r:id="rId15"/>
-    <hyperlink ref="B83" r:id="rId16"/>
-    <hyperlink ref="B35" r:id="rId17"/>
-    <hyperlink ref="B56" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
-    <hyperlink ref="B55" r:id="rId19"/>
-    <hyperlink ref="B113" r:id="rId20"/>
-    <hyperlink ref="B114" r:id="rId21"/>
-    <hyperlink ref="B49" r:id="rId22"/>
-    <hyperlink ref="B45" r:id="rId23"/>
-    <hyperlink ref="B127" r:id="rId24"/>
-    <hyperlink ref="B79" r:id="rId25"/>
-    <hyperlink ref="B132" r:id="rId26"/>
-    <hyperlink ref="B133" r:id="rId27" location="commandLine"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B88" r:id="rId29"/>
-    <hyperlink ref="B134" r:id="rId30"/>
-    <hyperlink ref="B78" r:id="rId31"/>
-    <hyperlink ref="B143" r:id="rId32"/>
-    <hyperlink ref="B31" r:id="rId33"/>
-    <hyperlink ref="B29" r:id="rId34"/>
-    <hyperlink ref="B33" r:id="rId35"/>
-    <hyperlink ref="B145" r:id="rId36"/>
-    <hyperlink ref="B108" r:id="rId37"/>
+    <hyperlink ref="B88" r:id="rId2"/>
+    <hyperlink ref="B91" r:id="rId3"/>
+    <hyperlink ref="B92" r:id="rId4"/>
+    <hyperlink ref="B93" r:id="rId5"/>
+    <hyperlink ref="B94" r:id="rId6"/>
+    <hyperlink ref="B95" r:id="rId7"/>
+    <hyperlink ref="B70" r:id="rId8"/>
+    <hyperlink ref="B81" r:id="rId9"/>
+    <hyperlink ref="B66" r:id="rId10"/>
+    <hyperlink ref="B59" r:id="rId11"/>
+    <hyperlink ref="B19" r:id="rId12"/>
+    <hyperlink ref="B61" r:id="rId13"/>
+    <hyperlink ref="B96" r:id="rId14"/>
+    <hyperlink ref="B90" r:id="rId15"/>
+    <hyperlink ref="B84" r:id="rId16"/>
+    <hyperlink ref="B36" r:id="rId17"/>
+    <hyperlink ref="B57" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
+    <hyperlink ref="B56" r:id="rId19"/>
+    <hyperlink ref="B114" r:id="rId20"/>
+    <hyperlink ref="B115" r:id="rId21"/>
+    <hyperlink ref="B50" r:id="rId22"/>
+    <hyperlink ref="B15" r:id="rId23" display="http://www.tutorialspoint.com/restful/index.htm"/>
+    <hyperlink ref="B128" r:id="rId24"/>
+    <hyperlink ref="B80" r:id="rId25"/>
+    <hyperlink ref="B133" r:id="rId26"/>
+    <hyperlink ref="B134" r:id="rId27" location="commandLine"/>
+    <hyperlink ref="B31" r:id="rId28"/>
+    <hyperlink ref="B89" r:id="rId29"/>
+    <hyperlink ref="B135" r:id="rId30"/>
+    <hyperlink ref="B79" r:id="rId31"/>
+    <hyperlink ref="B144" r:id="rId32"/>
+    <hyperlink ref="B32" r:id="rId33"/>
+    <hyperlink ref="B30" r:id="rId34"/>
+    <hyperlink ref="B34" r:id="rId35"/>
+    <hyperlink ref="B146" r:id="rId36"/>
+    <hyperlink ref="B109" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>

</xml_diff>

<commit_message>
REST Web Services, SQL
REST Web Services, SQL
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="219">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -674,6 +674,18 @@
   </si>
   <si>
     <t>9_Definitions_Web_Services.xlsx</t>
+  </si>
+  <si>
+    <t>Togglz</t>
+  </si>
+  <si>
+    <t>7_Definitions_Design_Patterns.xlsx</t>
+  </si>
+  <si>
+    <t>Utils</t>
+  </si>
+  <si>
+    <t>a_Definitions_Util.xlsx</t>
   </si>
 </sst>
 </file>
@@ -811,7 +823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -844,6 +856,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1166,8 +1180,8 @@
   <dimension ref="A1:C153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1487,7 +1501,7 @@
       <c r="B32" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="33" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1498,7 +1512,7 @@
       <c r="B33" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="33"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
@@ -1876,7 +1890,7 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="29" t="s">
+      <c r="A88" s="31" t="s">
         <v>117</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -1884,7 +1898,7 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="30"/>
+      <c r="A89" s="32"/>
       <c r="B89" s="3" t="s">
         <v>119</v>
       </c>
@@ -2047,6 +2061,14 @@
         <v>180</v>
       </c>
     </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C110" s="29" t="s">
+        <v>216</v>
+      </c>
+    </row>
     <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
         <v>144</v>
@@ -2241,9 +2263,17 @@
         <v>185</v>
       </c>
     </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
     <row r="143" spans="1:3">
       <c r="A143" s="5" t="s">
         <v>184</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="144" spans="1:3">

</xml_diff>

<commit_message>
Apache Camel, SAML 2.0
Apache Camel, SAML 2.0
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1303,8 +1303,8 @@
   <dimension ref="A1:D184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A180" sqref="A180"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Spring Boot, Spring Annotations, Linux
Spring Boot, Spring Annotations, Linux
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="248">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -726,9 +726,6 @@
     <t>JVM and JDK Tools - c_Definitions_JVM.xlsx</t>
   </si>
   <si>
-    <t>Jmeter</t>
-  </si>
-  <si>
     <t>Docker Hub</t>
   </si>
   <si>
@@ -739,6 +736,42 @@
   </si>
   <si>
     <t>Authentication/Autherization - i_Definitions_Authentication.xlsx</t>
+  </si>
+  <si>
+    <t>Linux - j_Definitions_Linux.xlsx</t>
+  </si>
+  <si>
+    <t>Ecl Emma</t>
+  </si>
+  <si>
+    <t>Coburtura</t>
+  </si>
+  <si>
+    <t>Jacoco</t>
+  </si>
+  <si>
+    <t>Jcov</t>
+  </si>
+  <si>
+    <t>Clover</t>
+  </si>
+  <si>
+    <t>Wiki</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Java_Code_Coverage_Tools</t>
+  </si>
+  <si>
+    <t>Code coverage tools - b_Definitions_Tools.xlsx</t>
+  </si>
+  <si>
+    <t>Apache Jmeter</t>
+  </si>
+  <si>
+    <t>Load and performance testing tool by Apache</t>
+  </si>
+  <si>
+    <t>Performance testing tools - b_Definitions_Tools.xlsx</t>
   </si>
 </sst>
 </file>
@@ -945,7 +978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1005,10 +1038,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1326,18 +1362,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="48.875" customWidth="1"/>
+    <col min="2" max="2" width="88.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1">
@@ -1355,11 +1391,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
@@ -1372,7 +1408,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1435,7 +1471,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1454,7 +1490,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60">
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1501,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1557,7 +1593,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -1635,8 +1671,8 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="34" t="s">
-        <v>233</v>
+      <c r="A33" s="33" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1909,7 +1945,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="38" t="s">
+      <c r="A73" s="41" t="s">
         <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1917,7 +1953,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="39"/>
+      <c r="A74" s="42"/>
       <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
@@ -1993,8 +2029,8 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="34" t="s">
-        <v>234</v>
+      <c r="A83" s="33" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2067,8 +2103,8 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="34" t="s">
-        <v>235</v>
+      <c r="A94" s="33" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2288,11 +2324,11 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A130" s="35" t="s">
+      <c r="A130" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="B130" s="36"/>
-      <c r="C130" s="37"/>
+      <c r="B130" s="39"/>
+      <c r="C130" s="40"/>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="29" t="s">
@@ -2320,11 +2356,11 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="136" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A136" s="35" t="s">
+      <c r="A136" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B136" s="36"/>
-      <c r="C136" s="37"/>
+      <c r="B136" s="39"/>
+      <c r="C136" s="40"/>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
@@ -2348,11 +2384,11 @@
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="142" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A142" s="35" t="s">
+      <c r="A142" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="B142" s="36"/>
-      <c r="C142" s="37"/>
+      <c r="B142" s="39"/>
+      <c r="C142" s="40"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
@@ -2381,11 +2417,11 @@
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="147" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A147" s="35" t="s">
+      <c r="A147" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="B147" s="36"/>
-      <c r="C147" s="37"/>
+      <c r="B147" s="39"/>
+      <c r="C147" s="40"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
@@ -2424,11 +2460,11 @@
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="155" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A155" s="35" t="s">
+      <c r="A155" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B155" s="36"/>
-      <c r="C155" s="37"/>
+      <c r="B155" s="39"/>
+      <c r="C155" s="40"/>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
@@ -2481,11 +2517,11 @@
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="165" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A165" s="35" t="s">
+      <c r="A165" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="B165" s="36"/>
-      <c r="C165" s="37"/>
+      <c r="B165" s="39"/>
+      <c r="C165" s="40"/>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
@@ -2496,20 +2532,20 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="30">
-      <c r="A167" s="40" t="s">
+      <c r="A167" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C167" s="42"/>
+      <c r="C167" s="45"/>
     </row>
     <row r="168" spans="1:3" s="26" customFormat="1">
-      <c r="A168" s="41"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C168" s="42"/>
+      <c r="C168" s="45"/>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
@@ -2518,11 +2554,11 @@
     </row>
     <row r="171" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="172" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A172" s="35" t="s">
+      <c r="A172" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="B172" s="36"/>
-      <c r="C172" s="37"/>
+      <c r="B172" s="39"/>
+      <c r="C172" s="40"/>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="26" t="s">
@@ -2541,9 +2577,7 @@
       </c>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="1:3" s="30" customFormat="1">
-      <c r="B176" s="2"/>
-    </row>
+    <row r="176" spans="1:3" s="30" customFormat="1"/>
     <row r="177" spans="1:3" s="30" customFormat="1">
       <c r="A177" s="5" t="s">
         <v>210</v>
@@ -2559,11 +2593,11 @@
     </row>
     <row r="179" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="180" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A180" s="35" t="s">
+      <c r="A180" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B180" s="36"/>
-      <c r="C180" s="37"/>
+      <c r="B180" s="39"/>
+      <c r="C180" s="40"/>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
@@ -2579,16 +2613,11 @@
     </row>
     <row r="184" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="185" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A185" s="35" t="s">
+      <c r="A185" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B185" s="36"/>
-      <c r="C185" s="37"/>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="33" t="s">
-        <v>232</v>
-      </c>
+      <c r="B185" s="39"/>
+      <c r="C185" s="40"/>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
@@ -2606,11 +2635,11 @@
     </row>
     <row r="189" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="190" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A190" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="B190" s="36"/>
-      <c r="C190" s="37"/>
+      <c r="A190" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="B190" s="39"/>
+      <c r="C190" s="40"/>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="5" t="s">
@@ -2623,16 +2652,105 @@
         <v>230</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:3">
       <c r="A193" s="31" t="s">
         <v>208</v>
       </c>
     </row>
+    <row r="194" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A194" s="31"/>
+      <c r="B194" s="2"/>
+    </row>
+    <row r="195" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A195" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="B195" s="39"/>
+      <c r="C195" s="40"/>
+    </row>
+    <row r="196" spans="1:3" s="34" customFormat="1">
+      <c r="A196" s="31"/>
+      <c r="B196" s="2"/>
+    </row>
+    <row r="197" spans="1:3" s="34" customFormat="1">
+      <c r="A197" s="31"/>
+      <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="1:3" s="34" customFormat="1">
+      <c r="A198" s="31"/>
+      <c r="B198" s="2"/>
+    </row>
+    <row r="199" spans="1:3" s="34" customFormat="1">
+      <c r="A199" s="31"/>
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="201" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A201" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="B201" s="39"/>
+      <c r="C201" s="40"/>
+    </row>
+    <row r="202" spans="1:3" s="34" customFormat="1">
+      <c r="A202" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B202" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="34" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="209" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A209" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B209" s="39"/>
+      <c r="C209" s="40"/>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="37" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A190:C190"/>
+  <mergeCells count="17">
     <mergeCell ref="A185:C185"/>
     <mergeCell ref="A180:C180"/>
+    <mergeCell ref="A209:C209"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A130:C130"/>
     <mergeCell ref="A136:C136"/>
@@ -2644,6 +2762,9 @@
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="A167:A168"/>
     <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A201:C201"/>
+    <mergeCell ref="A195:C195"/>
+    <mergeCell ref="A190:C190"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>
@@ -2680,8 +2801,9 @@
     <hyperlink ref="B122" r:id="rId32"/>
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
     <hyperlink ref="B168" r:id="rId33"/>
+    <hyperlink ref="B202" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spring Boot, Spring Boot + Junit
Spring Boot, Spring Boot + Junit
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1365,14 +1365,14 @@
   <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A196" sqref="A196"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.875" customWidth="1"/>
-    <col min="2" max="2" width="88.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="71.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2748,6 +2748,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A190:C190"/>
     <mergeCell ref="A185:C185"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A209:C209"/>
@@ -2764,7 +2765,6 @@
     <mergeCell ref="C167:C168"/>
     <mergeCell ref="A201:C201"/>
     <mergeCell ref="A195:C195"/>
-    <mergeCell ref="A190:C190"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>

</xml_diff>

<commit_message>
Spring MVC, component-scan tag
Spring MVC, component-scan tag
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="252">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -775,6 +775,15 @@
   </si>
   <si>
     <t>Docker</t>
+  </si>
+  <si>
+    <t>Code quality tools - b_Definitions_Tools.xlsx</t>
+  </si>
+  <si>
+    <t>Sonarqube</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
   </si>
 </sst>
 </file>
@@ -981,7 +990,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1047,6 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1360,11 +1370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,11 +1399,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
@@ -1943,7 +1953,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="43" t="s">
         <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1951,7 +1961,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="43"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
@@ -2322,11 +2332,11 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A130" s="39" t="s">
+      <c r="A130" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="B130" s="40"/>
-      <c r="C130" s="41"/>
+      <c r="B130" s="41"/>
+      <c r="C130" s="42"/>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="29" t="s">
@@ -2354,11 +2364,11 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="136" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A136" s="39" t="s">
+      <c r="A136" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="B136" s="40"/>
-      <c r="C136" s="41"/>
+      <c r="B136" s="41"/>
+      <c r="C136" s="42"/>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
@@ -2382,11 +2392,11 @@
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="142" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A142" s="39" t="s">
+      <c r="A142" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="B142" s="40"/>
-      <c r="C142" s="41"/>
+      <c r="B142" s="41"/>
+      <c r="C142" s="42"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
@@ -2415,11 +2425,11 @@
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="147" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A147" s="39" t="s">
+      <c r="A147" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="B147" s="40"/>
-      <c r="C147" s="41"/>
+      <c r="B147" s="41"/>
+      <c r="C147" s="42"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
@@ -2458,11 +2468,11 @@
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="155" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A155" s="39" t="s">
+      <c r="A155" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="B155" s="40"/>
-      <c r="C155" s="41"/>
+      <c r="B155" s="41"/>
+      <c r="C155" s="42"/>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
@@ -2515,11 +2525,11 @@
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="165" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A165" s="39" t="s">
+      <c r="A165" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="B165" s="40"/>
-      <c r="C165" s="41"/>
+      <c r="B165" s="41"/>
+      <c r="C165" s="42"/>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="38" t="s">
@@ -2536,14 +2546,14 @@
       <c r="B167" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C167" s="44"/>
+      <c r="C167" s="45"/>
     </row>
     <row r="168" spans="1:3" s="26" customFormat="1">
       <c r="A168" s="38"/>
       <c r="B168" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C168" s="44"/>
+      <c r="C168" s="45"/>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="38" t="s">
@@ -2552,11 +2562,11 @@
     </row>
     <row r="171" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="172" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A172" s="39" t="s">
+      <c r="A172" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="B172" s="40"/>
-      <c r="C172" s="41"/>
+      <c r="B172" s="41"/>
+      <c r="C172" s="42"/>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="26" t="s">
@@ -2593,162 +2603,180 @@
       </c>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" thickBot="1">
+    <row r="179" spans="1:3">
       <c r="A179" s="38" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A180" s="39" t="s">
+    <row r="180" spans="1:3" s="39" customFormat="1">
+      <c r="B180" s="2"/>
+    </row>
+    <row r="181" spans="1:3" s="39" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A182" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="B180" s="40"/>
-      <c r="C180" s="41"/>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="38" t="s">
+      <c r="B182" s="41"/>
+      <c r="C182" s="42"/>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C181" s="26"/>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="38" t="s">
+      <c r="C183" s="26"/>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C182" s="24"/>
-    </row>
-    <row r="184" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="185" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A185" s="39" t="s">
+      <c r="C184" s="24"/>
+    </row>
+    <row r="186" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="187" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A187" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="B185" s="40"/>
-      <c r="C185" s="41"/>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="38" t="s">
+      <c r="B187" s="41"/>
+      <c r="C187" s="42"/>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="38" t="s">
+      <c r="B188" s="3"/>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B189" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="189" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A189" s="39" t="s">
+    <row r="190" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="191" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A191" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="B189" s="40"/>
-      <c r="C189" s="41"/>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="38" t="s">
+      <c r="B191" s="41"/>
+      <c r="C191" s="42"/>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="C190" s="14"/>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="31" t="s">
+      <c r="C192" s="14"/>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="31" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="31" t="s">
+    <row r="194" spans="1:3">
+      <c r="A194" s="31" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="193" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A193" s="31"/>
-      <c r="B193" s="2"/>
-    </row>
-    <row r="194" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A194" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="B194" s="40"/>
-      <c r="C194" s="41"/>
-    </row>
-    <row r="195" spans="1:3" s="34" customFormat="1">
+    <row r="195" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
       <c r="A195" s="31"/>
       <c r="B195" s="2"/>
     </row>
-    <row r="196" spans="1:3" s="34" customFormat="1">
-      <c r="A196" s="31"/>
-      <c r="B196" s="2"/>
-    </row>
-    <row r="197" spans="1:3" s="34" customFormat="1">
+    <row r="196" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A196" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="B196" s="41"/>
+      <c r="C196" s="42"/>
+    </row>
+    <row r="197" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
       <c r="A197" s="31"/>
       <c r="B197" s="2"/>
     </row>
-    <row r="198" spans="1:3" s="34" customFormat="1">
-      <c r="A198" s="31"/>
-      <c r="B198" s="2"/>
-    </row>
-    <row r="199" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="200" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A200" s="39" t="s">
+    <row r="198" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A198" s="40" t="s">
         <v>244</v>
       </c>
-      <c r="B200" s="40"/>
-      <c r="C200" s="41"/>
-    </row>
-    <row r="201" spans="1:3" s="34" customFormat="1">
+      <c r="B198" s="41"/>
+      <c r="C198" s="42"/>
+    </row>
+    <row r="199" spans="1:3" s="34" customFormat="1">
+      <c r="A199" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B199" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
       <c r="A201" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="B201" s="36" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="34" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="34" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="A205" s="34" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" s="34" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="208" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A208" s="39" t="s">
+    <row r="205" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="206" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A206" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="B208" s="40"/>
-      <c r="C208" s="41"/>
-    </row>
-    <row r="209" spans="1:2">
-      <c r="A209" s="35" t="s">
+      <c r="B206" s="41"/>
+      <c r="C206" s="42"/>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B207" s="2" t="s">
         <v>246</v>
       </c>
     </row>
+    <row r="208" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="209" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A209" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="B209" s="41"/>
+      <c r="C209" s="42"/>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="39" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="39" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="A209:C209"/>
+    <mergeCell ref="A196:C196"/>
+    <mergeCell ref="A191:C191"/>
+    <mergeCell ref="A187:C187"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A198:C198"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A130:C130"/>
     <mergeCell ref="A136:C136"/>
@@ -2759,12 +2787,6 @@
     <mergeCell ref="A165:C165"/>
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A194:C194"/>
-    <mergeCell ref="A189:C189"/>
-    <mergeCell ref="A185:C185"/>
-    <mergeCell ref="A180:C180"/>
-    <mergeCell ref="A208:C208"/>
-    <mergeCell ref="A200:C200"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>
@@ -2801,7 +2823,7 @@
     <hyperlink ref="B122" r:id="rId32"/>
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
     <hyperlink ref="B168" r:id="rId33"/>
-    <hyperlink ref="B201" r:id="rId34"/>
+    <hyperlink ref="B199" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
AWS, Groovy, Spring, Maven, RegEx
AWS, Groovy, Spring, Maven, RegEx
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="All Topics" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="A">'All Topics'!$A$232</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="263">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -808,6 +811,15 @@
   </si>
   <si>
     <t>Logging - 2_Definitions.xlsx</t>
+  </si>
+  <si>
+    <t>Regular Expression</t>
+  </si>
+  <si>
+    <t>Core Java - 2_Definitions.xlsx</t>
+  </si>
+  <si>
+    <t>Groovy - k_Definitions_Groovy.xlsx</t>
   </si>
 </sst>
 </file>
@@ -912,7 +924,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1009,12 +1021,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1088,6 +1109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1096,6 +1118,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1399,11 +1427,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D229"/>
+  <dimension ref="A1:D237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A180" sqref="A180"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A238" sqref="A238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1428,33 +1456,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>173</v>
-      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
@@ -1963,7 +1969,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="48" t="s">
+      <c r="A73" s="51" t="s">
         <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1971,7 +1977,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="49"/>
+      <c r="A74" s="52"/>
       <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
@@ -2326,11 +2332,11 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A130" s="45" t="s">
+      <c r="A130" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="B130" s="46"/>
-      <c r="C130" s="47"/>
+      <c r="B130" s="47"/>
+      <c r="C130" s="48"/>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="29" t="s">
@@ -2358,11 +2364,11 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="136" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A136" s="45" t="s">
+      <c r="A136" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="B136" s="46"/>
-      <c r="C136" s="47"/>
+      <c r="B136" s="47"/>
+      <c r="C136" s="48"/>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
@@ -2412,11 +2418,11 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A143" s="45" t="s">
+      <c r="A143" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="B143" s="46"/>
-      <c r="C143" s="47"/>
+      <c r="B143" s="47"/>
+      <c r="C143" s="48"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
@@ -2445,11 +2451,11 @@
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="148" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A148" s="45" t="s">
+      <c r="A148" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="B148" s="46"/>
-      <c r="C148" s="47"/>
+      <c r="B148" s="47"/>
+      <c r="C148" s="48"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
@@ -2488,11 +2494,11 @@
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="156" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A156" s="45" t="s">
+      <c r="A156" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="B156" s="46"/>
-      <c r="C156" s="47"/>
+      <c r="B156" s="47"/>
+      <c r="C156" s="48"/>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
@@ -2545,11 +2551,11 @@
     </row>
     <row r="165" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="166" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A166" s="45" t="s">
+      <c r="A166" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="B166" s="46"/>
-      <c r="C166" s="47"/>
+      <c r="B166" s="47"/>
+      <c r="C166" s="48"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="38" t="s">
@@ -2566,14 +2572,14 @@
       <c r="B168" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C168" s="50"/>
+      <c r="C168" s="53"/>
     </row>
     <row r="169" spans="1:3" s="26" customFormat="1">
       <c r="A169" s="38"/>
       <c r="B169" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C169" s="50"/>
+      <c r="C169" s="53"/>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="38" t="s">
@@ -2582,11 +2588,11 @@
     </row>
     <row r="172" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="173" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A173" s="45" t="s">
+      <c r="A173" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="B173" s="46"/>
-      <c r="C173" s="47"/>
+      <c r="B173" s="47"/>
+      <c r="C173" s="48"/>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="26" t="s">
@@ -2633,11 +2639,11 @@
       <c r="B182" s="2"/>
     </row>
     <row r="183" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A183" s="45" t="s">
+      <c r="A183" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="B183" s="46"/>
-      <c r="C183" s="47"/>
+      <c r="B183" s="47"/>
+      <c r="C183" s="48"/>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="38" t="s">
@@ -2653,11 +2659,11 @@
     </row>
     <row r="187" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="188" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A188" s="45" t="s">
+      <c r="A188" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="B188" s="46"/>
-      <c r="C188" s="47"/>
+      <c r="B188" s="47"/>
+      <c r="C188" s="48"/>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="38" t="s">
@@ -2675,11 +2681,11 @@
     </row>
     <row r="191" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="45" t="s">
+      <c r="A192" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="B192" s="46"/>
-      <c r="C192" s="47"/>
+      <c r="B192" s="47"/>
+      <c r="C192" s="48"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="38" t="s">
@@ -2702,22 +2708,22 @@
       <c r="B196" s="2"/>
     </row>
     <row r="197" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A197" s="45" t="s">
+      <c r="A197" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="B197" s="46"/>
-      <c r="C197" s="47"/>
+      <c r="B197" s="47"/>
+      <c r="C197" s="48"/>
     </row>
     <row r="198" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
       <c r="A198" s="31"/>
       <c r="B198" s="2"/>
     </row>
     <row r="199" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A199" s="45" t="s">
+      <c r="A199" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="B199" s="46"/>
-      <c r="C199" s="47"/>
+      <c r="B199" s="47"/>
+      <c r="C199" s="48"/>
     </row>
     <row r="200" spans="1:3" s="34" customFormat="1">
       <c r="A200" s="34" t="s">
@@ -2754,11 +2760,11 @@
     </row>
     <row r="206" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="207" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A207" s="45" t="s">
+      <c r="A207" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="B207" s="46"/>
-      <c r="C207" s="47"/>
+      <c r="B207" s="47"/>
+      <c r="C207" s="48"/>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="35" t="s">
@@ -2770,11 +2776,11 @@
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="210" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A210" s="45" t="s">
+      <c r="A210" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="B210" s="46"/>
-      <c r="C210" s="47"/>
+      <c r="B210" s="47"/>
+      <c r="C210" s="48"/>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="39" t="s">
@@ -2788,11 +2794,11 @@
     </row>
     <row r="214" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="215" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A215" s="45" t="s">
+      <c r="A215" s="46" t="s">
         <v>252</v>
       </c>
-      <c r="B215" s="46"/>
-      <c r="C215" s="47"/>
+      <c r="B215" s="47"/>
+      <c r="C215" s="48"/>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="40" t="s">
@@ -2811,11 +2817,11 @@
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="45" t="s">
+      <c r="A221" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="B221" s="46"/>
-      <c r="C221" s="47"/>
+      <c r="B221" s="47"/>
+      <c r="C221" s="48"/>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="44" t="s">
@@ -2844,11 +2850,11 @@
     </row>
     <row r="226" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="227" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A227" s="45" t="s">
+      <c r="A227" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="B227" s="46"/>
-      <c r="C227" s="47"/>
+      <c r="B227" s="47"/>
+      <c r="C227" s="48"/>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="44" t="s">
@@ -2858,8 +2864,47 @@
     <row r="229" spans="1:3">
       <c r="A229" s="44"/>
     </row>
+    <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="231" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A231" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="B231" s="47"/>
+      <c r="C231" s="48"/>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="45" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B234" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C234" s="50"/>
+    </row>
+    <row r="236" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="237" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A237" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="B237" s="47"/>
+      <c r="C237" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="A237:C237"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A130:C130"/>
     <mergeCell ref="A136:C136"/>
@@ -2870,6 +2915,8 @@
     <mergeCell ref="A166:C166"/>
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="C168:C169"/>
+    <mergeCell ref="A231:C231"/>
+    <mergeCell ref="B234:C234"/>
     <mergeCell ref="A183:C183"/>
     <mergeCell ref="A207:C207"/>
     <mergeCell ref="A199:C199"/>

</xml_diff>

<commit_message>
Mockito, Swagger, Apiary, Junit
Mockito, Swagger, Apiary, Junit
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -10,14 +10,14 @@
     <sheet name="All Topics" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="A">'All Topics'!$A$232</definedName>
+    <definedName name="A">'All Topics'!$A$229</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="267">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -825,7 +825,13 @@
     <t>Apache Benchmark</t>
   </si>
   <si>
-    <t>Jmock</t>
+    <t>DBUnit</t>
+  </si>
+  <si>
+    <t>JMock</t>
+  </si>
+  <si>
+    <t>Splunk</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1095,9 +1101,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1116,6 +1119,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1434,11 +1445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D237"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A133" sqref="A133"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1463,11 +1474,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
@@ -1721,7 +1732,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="32" t="s">
         <v>230</v>
       </c>
     </row>
@@ -1976,7 +1987,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="50" t="s">
+      <c r="A73" s="53" t="s">
         <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1984,7 +1995,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="51"/>
+      <c r="A74" s="54"/>
       <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
@@ -2060,7 +2071,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="33" t="s">
+      <c r="A83" s="32" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2121,12 +2132,12 @@
         <v>190</v>
       </c>
       <c r="B93" s="3"/>
-      <c r="C93" s="32" t="s">
+      <c r="C93" s="31" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="33" t="s">
+      <c r="A94" s="32" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2322,626 +2333,631 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="5" t="s">
+    <row r="125" spans="1:3">
+      <c r="A125" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C127" s="26" t="s">
+      <c r="C125" s="26" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A129" s="28" t="s">
+    <row r="126" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A126" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C129" s="26" t="s">
+      <c r="C126" s="26" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15.75" thickBot="1">
+    <row r="127" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A127" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="B127" s="51"/>
+      <c r="C127" s="52"/>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="C128" s="26"/>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="C129" s="26"/>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="47" t="s">
-        <v>226</v>
-      </c>
-      <c r="B130" s="48"/>
-      <c r="C130" s="49"/>
+        <v>210</v>
+      </c>
+      <c r="C130" s="26"/>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="29" t="s">
-        <v>197</v>
+      <c r="A131" s="47" t="s">
+        <v>211</v>
       </c>
       <c r="C131" s="26"/>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C132" s="26"/>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C133" s="26"/>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C134" s="26"/>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A135" s="5" t="s">
+      <c r="A132" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" s="46" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A133" s="47" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A136" s="47" t="s">
+      <c r="B133" s="47"/>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A134" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="B136" s="48"/>
-      <c r="C136" s="49"/>
+      <c r="B134" s="51"/>
+      <c r="C134" s="52"/>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C135" s="15"/>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C137" s="15"/>
+        <v>199</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C137" s="16"/>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>182</v>
+        <v>256</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C139" s="16"/>
-    </row>
-    <row r="140" spans="1:3">
+    </row>
+    <row r="140" spans="1:3" s="42" customFormat="1" ht="15.75" thickBot="1">
       <c r="A140" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" s="43" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A142" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A143" s="47" t="s">
+    <row r="141" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A141" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="B143" s="48"/>
-      <c r="C143" s="49"/>
+      <c r="B141" s="51"/>
+      <c r="C141" s="52"/>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C142" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B143" s="3"/>
+      <c r="C143" s="23" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C144" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B145" s="3"/>
-      <c r="C145" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="5" t="s">
+      <c r="A144" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C146" s="26" t="s">
+      <c r="C144" s="26" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="148" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A148" s="47" t="s">
+    <row r="145" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="146" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A146" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B148" s="48"/>
-      <c r="C148" s="49"/>
+      <c r="B146" s="51"/>
+      <c r="C146" s="52"/>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C149" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="1" t="s">
-        <v>26</v>
+      <c r="A150" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C150" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C151" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C152" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="156" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A156" s="47" t="s">
+    <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="154" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A154" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="B156" s="48"/>
-      <c r="C156" s="49"/>
+      <c r="B154" s="51"/>
+      <c r="C154" s="52"/>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C155" s="26"/>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C156" s="26"/>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>24</v>
+      <c r="A157" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C157" s="26"/>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="5" t="s">
-        <v>146</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B158" s="3"/>
       <c r="C158" s="26"/>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
-        <v>147</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="B159" s="3"/>
       <c r="C159" s="26"/>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="26"/>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="26"/>
     </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="26"/>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B163" s="3"/>
-      <c r="C163" s="26"/>
-    </row>
-    <row r="165" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="166" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A166" s="47" t="s">
+    <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="164" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A164" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="B166" s="48"/>
-      <c r="C166" s="49"/>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="38" t="s">
+      <c r="B164" s="51"/>
+      <c r="C164" s="52"/>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B167" s="7" t="s">
+      <c r="B165" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="30">
-      <c r="A168" s="38" t="s">
+    <row r="166" spans="1:3" ht="30">
+      <c r="A166" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C168" s="52"/>
-    </row>
-    <row r="169" spans="1:3" s="26" customFormat="1">
-      <c r="A169" s="38"/>
-      <c r="B169" s="3" t="s">
+      <c r="C166" s="55"/>
+    </row>
+    <row r="167" spans="1:3" s="26" customFormat="1">
+      <c r="A167" s="37"/>
+      <c r="B167" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C169" s="52"/>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="38" t="s">
+      <c r="C167" s="55"/>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="173" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A173" s="47" t="s">
+    <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="171" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A171" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B173" s="48"/>
-      <c r="C173" s="49"/>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="26" t="s">
+      <c r="B171" s="51"/>
+      <c r="C171" s="52"/>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C174" s="26"/>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="38" t="s">
+      <c r="C172" s="26"/>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="176" spans="1:3" s="26" customFormat="1">
+    <row r="174" spans="1:3" s="29" customFormat="1">
+      <c r="A174" s="37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" s="29" customFormat="1">
+      <c r="A175" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="26"/>
+    </row>
+    <row r="176" spans="1:3" s="29" customFormat="1">
+      <c r="A176" s="36" t="s">
+        <v>232</v>
+      </c>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" spans="1:3" s="30" customFormat="1">
-      <c r="A177" s="38" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" s="30" customFormat="1">
-      <c r="A178" s="31" t="s">
-        <v>209</v>
+    <row r="177" spans="1:3">
+      <c r="A177" s="37" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" s="38" customFormat="1">
+      <c r="A178" s="49" t="s">
+        <v>266</v>
       </c>
       <c r="B178" s="2"/>
-      <c r="C178" s="26"/>
-    </row>
-    <row r="179" spans="1:3" s="30" customFormat="1">
-      <c r="A179" s="37" t="s">
-        <v>232</v>
-      </c>
+    </row>
+    <row r="179" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
       <c r="B179" s="2"/>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="38" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" s="39" customFormat="1">
-      <c r="A181" s="40"/>
-      <c r="B181" s="2"/>
-    </row>
-    <row r="182" spans="1:3" s="39" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B182" s="2"/>
-    </row>
-    <row r="183" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A183" s="47" t="s">
+    <row r="180" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A180" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B183" s="48"/>
-      <c r="C183" s="49"/>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="38" t="s">
+      <c r="B180" s="51"/>
+      <c r="C180" s="52"/>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C184" s="26"/>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="38" t="s">
+      <c r="C181" s="26"/>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="C185" s="24"/>
-    </row>
-    <row r="187" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="188" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A188" s="47" t="s">
+      <c r="C182" s="24"/>
+    </row>
+    <row r="184" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="185" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A185" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="B188" s="48"/>
-      <c r="C188" s="49"/>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="38" t="s">
+      <c r="B185" s="51"/>
+      <c r="C185" s="52"/>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B189" s="3"/>
+      <c r="B186" s="3"/>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="189" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A189" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="B189" s="51"/>
+      <c r="C189" s="52"/>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="47" t="s">
-        <v>233</v>
-      </c>
-      <c r="B192" s="48"/>
-      <c r="C192" s="49"/>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="38" t="s">
+      <c r="A190" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="C193" s="14"/>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" s="31" t="s">
+      <c r="C190" s="14"/>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
-      <c r="A195" s="31" t="s">
+    <row r="192" spans="1:3">
+      <c r="A192" s="30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="196" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A196" s="31"/>
-      <c r="B196" s="2"/>
-    </row>
-    <row r="197" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A197" s="47" t="s">
+    <row r="193" spans="1:3" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A193" s="30"/>
+      <c r="B193" s="2"/>
+    </row>
+    <row r="194" spans="1:3" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A194" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="B197" s="48"/>
-      <c r="C197" s="49"/>
-    </row>
-    <row r="198" spans="1:3" s="34" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A198" s="31"/>
-      <c r="B198" s="2"/>
-    </row>
-    <row r="199" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A199" s="47" t="s">
+      <c r="B194" s="51"/>
+      <c r="C194" s="52"/>
+    </row>
+    <row r="195" spans="1:3" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A195" s="30"/>
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A196" s="50" t="s">
         <v>242</v>
       </c>
-      <c r="B199" s="48"/>
-      <c r="C199" s="49"/>
-    </row>
-    <row r="200" spans="1:3" s="34" customFormat="1">
-      <c r="A200" s="34" t="s">
+      <c r="B196" s="51"/>
+      <c r="C196" s="52"/>
+    </row>
+    <row r="197" spans="1:3" s="33" customFormat="1">
+      <c r="A197" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="B200" s="36" t="s">
+      <c r="B197" s="35" t="s">
         <v>241</v>
       </c>
     </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="34" t="s">
-        <v>235</v>
+      <c r="A201" s="33" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="34" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="A203" s="34" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
-      <c r="A204" s="34" t="s">
-        <v>238</v>
-      </c>
+      <c r="A202" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="204" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A204" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="B204" s="51"/>
+      <c r="C204" s="52"/>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="15.75" thickBot="1"/>
+        <v>243</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A206" s="45" t="s">
+        <v>263</v>
+      </c>
+    </row>
     <row r="207" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A207" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="B207" s="48"/>
-      <c r="C207" s="49"/>
+      <c r="A207" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="B207" s="51"/>
+      <c r="C207" s="52"/>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="46" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A210" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="B210" s="48"/>
-      <c r="C210" s="49"/>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="A211" s="39" t="s">
+      <c r="A208" s="38" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
-      <c r="A212" s="39" t="s">
+    <row r="209" spans="1:3">
+      <c r="A209" s="38" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="215" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A215" s="47" t="s">
+    <row r="211" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="212" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A212" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="B215" s="48"/>
-      <c r="C215" s="49"/>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" s="40" t="s">
+      <c r="B212" s="51"/>
+      <c r="C212" s="52"/>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="39" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
-      <c r="A217" s="40" t="s">
+    <row r="214" spans="1:3">
+      <c r="A214" s="39" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
-      <c r="A218" s="40" t="s">
+    <row r="215" spans="1:3">
+      <c r="A215" s="39" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="47" t="s">
+    <row r="217" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="218" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A218" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="B221" s="48"/>
-      <c r="C221" s="49"/>
+      <c r="B218" s="51"/>
+      <c r="C218" s="52"/>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C219" s="19"/>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C220" s="20"/>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="40" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C222" s="19"/>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="C223" s="20"/>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="41" t="s">
-        <v>254</v>
-      </c>
+      <c r="A222" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="224" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A224" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="B224" s="51"/>
+      <c r="C224" s="52"/>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="42" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="227" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A227" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="B227" s="48"/>
-      <c r="C227" s="49"/>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="44" t="s">
+      <c r="A225" s="43" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="43"/>
+    </row>
+    <row r="227" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="228" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A228" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="B228" s="51"/>
+      <c r="C228" s="52"/>
+    </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="44"/>
-    </row>
-    <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="231" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A231" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="B231" s="48"/>
-      <c r="C231" s="49"/>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" s="45" t="s">
+      <c r="A229" s="44" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="45" t="s">
+    <row r="230" spans="1:3">
+      <c r="A230" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B230" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
-      <c r="A234" s="45" t="s">
+    <row r="231" spans="1:3">
+      <c r="A231" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B234" s="53" t="s">
+      <c r="B231" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C234" s="54"/>
-    </row>
-    <row r="236" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="47" t="s">
+      <c r="C231" s="57"/>
+    </row>
+    <row r="233" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="234" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A234" s="50" t="s">
         <v>262</v>
       </c>
-      <c r="B237" s="48"/>
-      <c r="C237" s="49"/>
+      <c r="B234" s="51"/>
+      <c r="C234" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A234:C234"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="A173:C173"/>
-    <mergeCell ref="A143:C143"/>
-    <mergeCell ref="A148:C148"/>
-    <mergeCell ref="A156:C156"/>
-    <mergeCell ref="A166:C166"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A171:C171"/>
+    <mergeCell ref="A141:C141"/>
+    <mergeCell ref="A146:C146"/>
+    <mergeCell ref="A154:C154"/>
+    <mergeCell ref="A164:C164"/>
     <mergeCell ref="A73:A74"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="A231:C231"/>
-    <mergeCell ref="B234:C234"/>
-    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="C166:C167"/>
+    <mergeCell ref="A228:C228"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="A180:C180"/>
+    <mergeCell ref="A204:C204"/>
+    <mergeCell ref="A196:C196"/>
+    <mergeCell ref="A189:C189"/>
+    <mergeCell ref="A185:C185"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A218:C218"/>
+    <mergeCell ref="A212:C212"/>
     <mergeCell ref="A207:C207"/>
-    <mergeCell ref="A199:C199"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="A227:C227"/>
-    <mergeCell ref="A221:C221"/>
-    <mergeCell ref="A215:C215"/>
-    <mergeCell ref="A210:C210"/>
-    <mergeCell ref="A197:C197"/>
+    <mergeCell ref="A194:C194"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>
@@ -2953,8 +2969,8 @@
     <hyperlink ref="B80" r:id="rId7"/>
     <hyperlink ref="B56" r:id="rId8"/>
     <hyperlink ref="B66" r:id="rId9"/>
-    <hyperlink ref="B222" r:id="rId10"/>
-    <hyperlink ref="B152" r:id="rId11"/>
+    <hyperlink ref="B219" r:id="rId10"/>
+    <hyperlink ref="B150" r:id="rId11"/>
     <hyperlink ref="B15" r:id="rId12"/>
     <hyperlink ref="B48" r:id="rId13"/>
     <hyperlink ref="B81" r:id="rId14"/>
@@ -2966,7 +2982,7 @@
     <hyperlink ref="B97" r:id="rId20"/>
     <hyperlink ref="B98" r:id="rId21"/>
     <hyperlink ref="B38" r:id="rId22"/>
-    <hyperlink ref="B145" r:id="rId23" display="http://www.tutorialspoint.com/restful/index.htm"/>
+    <hyperlink ref="B143" r:id="rId23" display="http://www.tutorialspoint.com/restful/index.htm"/>
     <hyperlink ref="B105" r:id="rId24"/>
     <hyperlink ref="B65" r:id="rId25"/>
     <hyperlink ref="B110" r:id="rId26"/>
@@ -2974,11 +2990,11 @@
     <hyperlink ref="B74" r:id="rId28"/>
     <hyperlink ref="B112" r:id="rId29"/>
     <hyperlink ref="B64" r:id="rId30"/>
-    <hyperlink ref="B138" r:id="rId31"/>
+    <hyperlink ref="B136" r:id="rId31"/>
     <hyperlink ref="B122" r:id="rId32"/>
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
-    <hyperlink ref="B169" r:id="rId33"/>
-    <hyperlink ref="B200" r:id="rId34"/>
+    <hyperlink ref="B167" r:id="rId33"/>
+    <hyperlink ref="B197" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
AWS, Web Services, DB, Enum
AWS, Web Services, DB, Enum
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1157,19 +1157,19 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1468,8 +1468,8 @@
   <dimension ref="A1:D248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A243" sqref="A243"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2007,7 +2007,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="57" t="s">
+      <c r="A73" s="55" t="s">
         <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="58"/>
+      <c r="A74" s="56"/>
       <c r="B74" s="3" t="s">
         <v>116</v>
       </c>
@@ -2604,14 +2604,14 @@
       <c r="B166" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C166" s="59"/>
+      <c r="C166" s="57"/>
     </row>
     <row r="167" spans="1:3" s="26" customFormat="1">
       <c r="A167" s="37"/>
       <c r="B167" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C167" s="59"/>
+      <c r="C167" s="57"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="37" t="s">
@@ -2924,10 +2924,10 @@
       <c r="A231" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B231" s="55" t="s">
+      <c r="B231" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C231" s="56"/>
+      <c r="C231" s="59"/>
     </row>
     <row r="233" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="234" spans="1:3" ht="15.75" thickBot="1">
@@ -2991,6 +2991,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A234:C234"/>
+    <mergeCell ref="A228:C228"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="A185:C185"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A218:C218"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A207:C207"/>
+    <mergeCell ref="A194:C194"/>
     <mergeCell ref="A247:C247"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A204:C204"/>
@@ -3007,15 +3016,6 @@
     <mergeCell ref="C166:C167"/>
     <mergeCell ref="A242:C242"/>
     <mergeCell ref="A189:C189"/>
-    <mergeCell ref="A185:C185"/>
-    <mergeCell ref="A224:C224"/>
-    <mergeCell ref="A218:C218"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A207:C207"/>
-    <mergeCell ref="A194:C194"/>
-    <mergeCell ref="A234:C234"/>
-    <mergeCell ref="A228:C228"/>
-    <mergeCell ref="B231:C231"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>

</xml_diff>

<commit_message>
Web Services, Mockito, Servers
Web Services, Mockito, Servers
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -10,14 +10,14 @@
     <sheet name="All Topics" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="A">'All Topics'!$A$228</definedName>
+    <definedName name="A">'All Topics'!$A$241</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="285">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -860,6 +860,30 @@
   </si>
   <si>
     <t>Logging - b_Definitions_Tools.xlsx</t>
+  </si>
+  <si>
+    <t>RAML</t>
+  </si>
+  <si>
+    <t>REST API Documentation Tools - b_Definitions_Tools.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST API Debugger Tools - </t>
+  </si>
+  <si>
+    <t>Burp</t>
+  </si>
+  <si>
+    <t>Fiddler</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>REST API - Packet Sniffers - To see Network traffic</t>
+  </si>
+  <si>
+    <t>Wire shark</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1083,6 +1107,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1092,7 +1120,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1105,6 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1400,11 +1428,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D260"/>
+  <dimension ref="A1:D273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2232,11 +2260,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="40" t="s">
+      <c r="A124" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="B124" s="41"/>
-      <c r="C124" s="42"/>
+      <c r="B124" s="43"/>
+      <c r="C124" s="44"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="37" t="s">
@@ -2274,11 +2302,11 @@
       <c r="B130" s="31"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="40" t="s">
+      <c r="A131" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B131" s="41"/>
-      <c r="C131" s="42"/>
+      <c r="B131" s="43"/>
+      <c r="C131" s="44"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="37" t="s">
@@ -2334,11 +2362,11 @@
       <c r="B138" s="37"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="40" t="s">
+      <c r="A139" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B139" s="41"/>
-      <c r="C139" s="42"/>
+      <c r="B139" s="43"/>
+      <c r="C139" s="44"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="37" t="s">
@@ -2374,11 +2402,11 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A144" s="40" t="s">
+      <c r="A144" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="B144" s="41"/>
-      <c r="C144" s="42"/>
+      <c r="B144" s="43"/>
+      <c r="C144" s="44"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="37" t="s">
@@ -2417,11 +2445,11 @@
     </row>
     <row r="151" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="152" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A152" s="40" t="s">
+      <c r="A152" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="B152" s="41"/>
-      <c r="C152" s="42"/>
+      <c r="B152" s="43"/>
+      <c r="C152" s="44"/>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="37" t="s">
@@ -2474,11 +2502,11 @@
     </row>
     <row r="161" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="162" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A162" s="40" t="s">
+      <c r="A162" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="B162" s="41"/>
-      <c r="C162" s="42"/>
+      <c r="B162" s="43"/>
+      <c r="C162" s="44"/>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="37" t="s">
@@ -2495,14 +2523,14 @@
       <c r="B164" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C164" s="43"/>
+      <c r="C164" s="49"/>
     </row>
     <row r="165" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A165" s="37"/>
       <c r="B165" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C165" s="43"/>
+      <c r="C165" s="49"/>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="37" t="s">
@@ -2511,11 +2539,11 @@
     </row>
     <row r="168" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="169" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A169" s="40" t="s">
+      <c r="A169" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B169" s="41"/>
-      <c r="C169" s="42"/>
+      <c r="B169" s="43"/>
+      <c r="C169" s="44"/>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="37" t="s">
@@ -2530,451 +2558,507 @@
     </row>
     <row r="172" spans="1:3" s="24" customFormat="1">
       <c r="A172" s="37" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="173" spans="1:3" s="24" customFormat="1">
-      <c r="A173" s="39" t="s">
-        <v>202</v>
+      <c r="A173" s="37" t="s">
+        <v>238</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="22"/>
     </row>
     <row r="174" spans="1:3" s="24" customFormat="1">
       <c r="A174" s="37" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="B174" s="1"/>
     </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="37" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" s="28" customFormat="1">
-      <c r="A176" s="37" t="s">
-        <v>257</v>
-      </c>
+    <row r="176" spans="1:3" s="28" customFormat="1" ht="15.75" thickBot="1">
       <c r="B176" s="1"/>
     </row>
-    <row r="177" spans="1:3" s="28" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A177" s="37"/>
-      <c r="B177" s="1"/>
-    </row>
-    <row r="178" spans="1:3" ht="15.75" thickBot="1">
+    <row r="177" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A177" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="B177" s="43"/>
+      <c r="C177" s="44"/>
+    </row>
+    <row r="178" spans="1:3" s="41" customFormat="1">
       <c r="A178" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="B178" s="40"/>
+    </row>
+    <row r="179" spans="1:3" s="41" customFormat="1">
+      <c r="A179" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B179" s="40"/>
+    </row>
+    <row r="180" spans="1:3" s="41" customFormat="1">
+      <c r="A180" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="B180" s="40"/>
+    </row>
+    <row r="181" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A181" s="40"/>
+      <c r="B181" s="40"/>
+    </row>
+    <row r="182" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A182" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="B182" s="43"/>
+      <c r="C182" s="44"/>
+    </row>
+    <row r="183" spans="1:3" s="41" customFormat="1">
+      <c r="A183" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="B183" s="40"/>
+    </row>
+    <row r="184" spans="1:3" s="41" customFormat="1">
+      <c r="A184" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B184" s="40"/>
+    </row>
+    <row r="185" spans="1:3" s="28" customFormat="1">
+      <c r="A185" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A186" s="40"/>
+      <c r="B186" s="40"/>
+    </row>
+    <row r="187" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A187" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="B187" s="43"/>
+      <c r="C187" s="44"/>
+    </row>
+    <row r="188" spans="1:3" s="41" customFormat="1">
+      <c r="A188" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B188" s="40"/>
+    </row>
+    <row r="189" spans="1:3" s="41" customFormat="1">
+      <c r="A189" s="40"/>
+      <c r="B189" s="40"/>
+    </row>
+    <row r="190" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A190" s="40"/>
+      <c r="B190" s="40"/>
+    </row>
+    <row r="191" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A191" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="B178" s="41"/>
-      <c r="C178" s="42"/>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="37" t="s">
+      <c r="B191" s="43"/>
+      <c r="C191" s="44"/>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C179" s="22"/>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="37" t="s">
+      <c r="C192" s="22"/>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="C180" s="20"/>
-    </row>
-    <row r="182" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="183" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A183" s="40" t="s">
+      <c r="C193" s="20"/>
+    </row>
+    <row r="195" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="196" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A196" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="B183" s="41"/>
-      <c r="C183" s="42"/>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="B184" s="2"/>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="B186" s="2"/>
-    </row>
-    <row r="187" spans="1:3" s="36" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A187" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="B187" s="2"/>
-    </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A188" s="40" t="s">
-        <v>225</v>
-      </c>
-      <c r="B188" s="41"/>
-      <c r="C188" s="42"/>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="C189" s="10"/>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="39" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="39" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A192" s="39"/>
-      <c r="B192" s="1"/>
-    </row>
-    <row r="193" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A193" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="B193" s="41"/>
-      <c r="C193" s="42"/>
-    </row>
-    <row r="194" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A194" s="39"/>
-      <c r="B194" s="1"/>
-    </row>
-    <row r="195" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A195" s="40" t="s">
-        <v>234</v>
-      </c>
-      <c r="B195" s="41"/>
-      <c r="C195" s="42"/>
-    </row>
-    <row r="196" spans="1:3" s="26" customFormat="1">
-      <c r="A196" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B196" s="27" t="s">
-        <v>233</v>
-      </c>
+      <c r="B196" s="43"/>
+      <c r="C196" s="44"/>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="37" t="s">
-        <v>227</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="B197" s="2"/>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="37" t="s">
-        <v>228</v>
+        <v>38</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="37" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
+        <v>274</v>
+      </c>
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="1:3" s="36" customFormat="1" ht="15.75" thickBot="1">
       <c r="A200" s="37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201" s="37" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="203" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A203" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="B203" s="41"/>
-      <c r="C203" s="42"/>
+        <v>273</v>
+      </c>
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A201" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="B201" s="43"/>
+      <c r="C201" s="44"/>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C202" s="10"/>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="39" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A205" s="37" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A206" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="B206" s="41"/>
-      <c r="C206" s="42"/>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="A207" s="37" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" s="37" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="211" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A211" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="B211" s="41"/>
-      <c r="C211" s="42"/>
+      <c r="A204" s="39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A205" s="39"/>
+      <c r="B205" s="1"/>
+    </row>
+    <row r="206" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A206" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B206" s="43"/>
+      <c r="C206" s="44"/>
+    </row>
+    <row r="207" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A207" s="39"/>
+      <c r="B207" s="1"/>
+    </row>
+    <row r="208" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A208" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="B208" s="43"/>
+      <c r="C208" s="44"/>
+    </row>
+    <row r="209" spans="1:3" s="26" customFormat="1">
+      <c r="A209" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B209" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="37" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="37" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="37" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="37" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A217" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="B217" s="41"/>
-      <c r="C217" s="42"/>
-    </row>
-    <row r="218" spans="1:3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="216" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A216" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B216" s="43"/>
+      <c r="C216" s="44"/>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="15.75" thickBot="1">
       <c r="A218" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C218" s="15"/>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="C219" s="16"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A219" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="B219" s="43"/>
+      <c r="C219" s="44"/>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="37" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="37" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="223" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A223" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="B223" s="41"/>
-      <c r="C223" s="42"/>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="37" t="s">
-        <v>70</v>
-      </c>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="224" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A224" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="B224" s="43"/>
+      <c r="C224" s="44"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B225" s="2"/>
-    </row>
-    <row r="226" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="227" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A227" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="B227" s="34"/>
-      <c r="C227" s="35"/>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="37" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B230" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C230" s="47"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="37" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A230" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B230" s="43"/>
+      <c r="C230" s="44"/>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C231" s="13"/>
-    </row>
-    <row r="232" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="233" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A233" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="B233" s="34"/>
-      <c r="C233" s="35"/>
+        <v>79</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C231" s="15"/>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C232" s="16"/>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="37" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="37" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="37" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="B241" s="34"/>
-      <c r="C241" s="35"/>
-    </row>
-    <row r="242" spans="1:3" ht="30">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="236" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A236" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="B236" s="43"/>
+      <c r="C236" s="44"/>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="240" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A240" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B240" s="34"/>
+      <c r="C240" s="35"/>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="37" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
       <c r="A242" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>154</v>
+        <v>0</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="37" t="s">
-        <v>260</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B243" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C243" s="48"/>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="37" t="s">
-        <v>261</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C244" s="13"/>
     </row>
     <row r="245" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="246" spans="1:3" ht="15.75" thickBot="1">
       <c r="A246" s="33" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B246" s="34"/>
       <c r="C246" s="35"/>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="C247" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B250" s="34"/>
-      <c r="C250" s="35"/>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B251" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C251" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252" s="45"/>
-      <c r="B252" s="32" t="s">
-        <v>264</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="37" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="254" spans="1:3" ht="15.75" thickBot="1">
       <c r="A254" s="33" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B254" s="34"/>
       <c r="C254" s="35"/>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" ht="30">
       <c r="A255" s="37" t="s">
-        <v>265</v>
+        <v>153</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="37" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="259" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A259" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B259" s="34"/>
+      <c r="C259" s="35"/>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C260" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="263" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A263" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B263" s="34"/>
+      <c r="C263" s="35"/>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C264" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="46"/>
+      <c r="B265" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="267" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A267" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B267" s="34"/>
+      <c r="C267" s="35"/>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="37" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="37" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="257" spans="1:1">
-      <c r="A257" s="37" t="s">
+    <row r="270" spans="1:3">
+      <c r="A270" s="37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="258" spans="1:1">
-      <c r="A258" s="37" t="s">
+    <row r="271" spans="1:3">
+      <c r="A271" s="37" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="259" spans="1:1">
-      <c r="A259" s="37" t="s">
+    <row r="272" spans="1:3">
+      <c r="A272" s="37" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="260" spans="1:1">
-      <c r="A260" s="37" t="s">
+    <row r="273" spans="1:1">
+      <c r="A273" s="37" t="s">
         <v>269</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A251:A252"/>
-    <mergeCell ref="B230:C230"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="A193:C193"/>
-    <mergeCell ref="A195:C195"/>
-    <mergeCell ref="A203:C203"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="A211:C211"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A223:C223"/>
-    <mergeCell ref="A178:C178"/>
+  <mergeCells count="23">
+    <mergeCell ref="A191:C191"/>
     <mergeCell ref="A124:C124"/>
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="A169:C169"/>
@@ -2983,6 +3067,20 @@
     <mergeCell ref="A152:C152"/>
     <mergeCell ref="A162:C162"/>
     <mergeCell ref="C164:C165"/>
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="A187:C187"/>
+    <mergeCell ref="A196:C196"/>
+    <mergeCell ref="A264:A265"/>
+    <mergeCell ref="B243:C243"/>
+    <mergeCell ref="A201:C201"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A208:C208"/>
+    <mergeCell ref="A216:C216"/>
+    <mergeCell ref="A219:C219"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A230:C230"/>
+    <mergeCell ref="A236:C236"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
@@ -2994,20 +3092,20 @@
     <hyperlink ref="B77" r:id="rId7"/>
     <hyperlink ref="B53" r:id="rId8"/>
     <hyperlink ref="B63" r:id="rId9"/>
-    <hyperlink ref="B218" r:id="rId10"/>
+    <hyperlink ref="B231" r:id="rId10"/>
     <hyperlink ref="B148" r:id="rId11"/>
     <hyperlink ref="B45" r:id="rId12"/>
     <hyperlink ref="B78" r:id="rId13"/>
     <hyperlink ref="B72" r:id="rId14"/>
     <hyperlink ref="B66" r:id="rId15"/>
-    <hyperlink ref="B251" r:id="rId16"/>
+    <hyperlink ref="B264" r:id="rId16"/>
     <hyperlink ref="B42" r:id="rId17" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
     <hyperlink ref="B41" r:id="rId18"/>
     <hyperlink ref="B94" r:id="rId19"/>
     <hyperlink ref="B95" r:id="rId20"/>
     <hyperlink ref="B35" r:id="rId21"/>
     <hyperlink ref="B141" r:id="rId22" display="http://www.tutorialspoint.com/restful/index.htm"/>
-    <hyperlink ref="B242" r:id="rId23"/>
+    <hyperlink ref="B255" r:id="rId23"/>
     <hyperlink ref="B62" r:id="rId24"/>
     <hyperlink ref="B107" r:id="rId25"/>
     <hyperlink ref="B108" r:id="rId26" location="commandLine"/>
@@ -3017,7 +3115,7 @@
     <hyperlink ref="B119" r:id="rId30"/>
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
     <hyperlink ref="B165" r:id="rId31"/>
-    <hyperlink ref="B196" r:id="rId32"/>
+    <hyperlink ref="B209" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>

</xml_diff>

<commit_message>
Spring Boot, AWS, REST
Spring Boot, AWS, REST
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="288">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -887,6 +887,12 @@
   </si>
   <si>
     <t>cURL</t>
+  </si>
+  <si>
+    <t>Beanio</t>
+  </si>
+  <si>
+    <t>http://www.beanio.org/2.0/docs/reference/index.html</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1091,15 +1097,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1118,6 +1115,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1127,7 +1127,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1140,6 +1139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1435,22 +1435,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D274"/>
+  <dimension ref="A1:D272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A273" sqref="A273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" style="37" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="35" t="s">
         <v>166</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1464,7 +1464,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1475,7 +1475,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1494,7 +1494,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1505,7 +1505,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="34" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1535,7 +1535,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1546,7 +1546,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="45">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="34" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1557,7 +1557,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="34" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="34" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="45">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1587,7 +1587,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C15" t="s">
@@ -1595,7 +1595,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="34" t="s">
         <v>35</v>
       </c>
       <c r="C17" t="s">
@@ -1611,7 +1611,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C18" t="s">
@@ -1619,7 +1619,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C19" t="s">
@@ -1627,11 +1627,11 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="B20" s="37"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="34" t="s">
         <v>39</v>
       </c>
       <c r="C21" t="s">
@@ -1639,43 +1639,43 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="34" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="34" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="34" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1686,12 +1686,12 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="34" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="34" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1699,17 +1699,17 @@
       <c r="C32" s="19"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="34" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1717,27 +1717,27 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1745,7 +1745,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="45">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="75">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="34" t="s">
         <v>66</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="34" t="s">
         <v>71</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1769,12 +1769,12 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="34" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1785,12 +1785,12 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="34" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="34" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1798,17 +1798,17 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="34" t="s">
         <v>87</v>
       </c>
       <c r="C54" t="s">
@@ -1824,17 +1824,17 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="34" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="34" t="s">
         <v>89</v>
       </c>
       <c r="C57" t="s">
@@ -1842,17 +1842,17 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="34" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="34" t="s">
         <v>93</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1860,7 +1860,7 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="34" t="s">
         <v>95</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -1876,7 +1876,7 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="34" t="s">
         <v>99</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1884,7 +1884,7 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="34" t="s">
         <v>101</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1892,7 +1892,7 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="34" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -1900,7 +1900,7 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="34" t="s">
         <v>105</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1908,7 +1908,7 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="34" t="s">
         <v>107</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1916,12 +1916,12 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="37" t="s">
+      <c r="A69" s="34" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="34" t="s">
         <v>110</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -1934,7 +1934,7 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="37" t="s">
+      <c r="A72" s="34" t="s">
         <v>113</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="37" t="s">
+      <c r="A73" s="34" t="s">
         <v>115</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="37" t="s">
+      <c r="A74" s="34" t="s">
         <v>117</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -1964,7 +1964,7 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="37" t="s">
+      <c r="A75" s="34" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -1972,7 +1972,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="30">
-      <c r="A76" s="37" t="s">
+      <c r="A76" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="37" t="s">
+      <c r="A77" s="34" t="s">
         <v>123</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -1991,7 +1991,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="30">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="34" t="s">
         <v>125</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -1999,17 +1999,17 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="37" t="s">
+      <c r="A79" s="34" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="37" t="s">
+      <c r="A80" s="34" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="37" t="s">
+      <c r="A81" s="34" t="s">
         <v>129</v>
       </c>
       <c r="C81" t="s">
@@ -2017,7 +2017,7 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="37" t="s">
+      <c r="A82" s="34" t="s">
         <v>130</v>
       </c>
       <c r="C82" t="s">
@@ -2025,7 +2025,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="37" t="s">
+      <c r="A83" s="34" t="s">
         <v>131</v>
       </c>
       <c r="C83" t="s">
@@ -2033,35 +2033,35 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="34" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="37" t="s">
+      <c r="A86" s="34" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="9" customFormat="1">
-      <c r="A87" s="37" t="s">
+      <c r="A87" s="34" t="s">
         <v>185</v>
       </c>
       <c r="B87" s="1"/>
     </row>
     <row r="88" spans="1:3" s="9" customFormat="1">
-      <c r="A88" s="37" t="s">
+      <c r="A88" s="34" t="s">
         <v>186</v>
       </c>
       <c r="B88" s="1"/>
     </row>
     <row r="89" spans="1:3" s="9" customFormat="1">
-      <c r="A89" s="37" t="s">
+      <c r="A89" s="34" t="s">
         <v>187</v>
       </c>
       <c r="B89" s="1"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1">
-      <c r="A90" s="37" t="s">
+      <c r="A90" s="34" t="s">
         <v>184</v>
       </c>
       <c r="B90" s="2"/>
@@ -2070,22 +2070,22 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="34" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="37" t="s">
+      <c r="A92" s="34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="37" t="s">
+      <c r="A93" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="37" t="s">
+      <c r="A94" s="34" t="s">
         <v>137</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="30">
-      <c r="A95" s="37" t="s">
+      <c r="A95" s="34" t="s">
         <v>139</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -2101,63 +2101,63 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A96" s="37" t="s">
+      <c r="A96" s="34" t="s">
         <v>141</v>
       </c>
       <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="37" t="s">
+      <c r="A97" s="34" t="s">
         <v>144</v>
       </c>
       <c r="B97" s="2"/>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="37" t="s">
+      <c r="A98" s="34" t="s">
         <v>145</v>
       </c>
       <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="37" t="s">
+      <c r="A99" s="34" t="s">
         <v>146</v>
       </c>
       <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="37" t="s">
+      <c r="A100" s="34" t="s">
         <v>147</v>
       </c>
       <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="37" t="s">
+      <c r="A101" s="34" t="s">
         <v>148</v>
       </c>
       <c r="B101" s="2"/>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="37" t="s">
+      <c r="A103" s="34" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="37" t="s">
+      <c r="A104" s="34" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="37" t="s">
+      <c r="A105" s="34" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="37" t="s">
+      <c r="A106" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="37" t="s">
+      <c r="A107" s="34" t="s">
         <v>159</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="37" t="s">
+      <c r="A108" s="34" t="s">
         <v>161</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="34" t="s">
         <v>163</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -2181,37 +2181,37 @@
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="37" t="s">
+      <c r="A110" s="34" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="34" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="37" t="s">
+      <c r="A113" s="34" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="37" t="s">
+      <c r="A114" s="34" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="37" t="s">
+      <c r="A115" s="34" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="37" t="s">
+      <c r="A116" s="34" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="37" t="s">
+      <c r="A117" s="34" t="s">
         <v>174</v>
       </c>
       <c r="C117" s="21" t="s">
@@ -2219,7 +2219,7 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="37" t="s">
+      <c r="A118" s="34" t="s">
         <v>178</v>
       </c>
       <c r="C118" t="s">
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="30">
-      <c r="A119" s="37" t="s">
+      <c r="A119" s="34" t="s">
         <v>179</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -2235,7 +2235,7 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="37" t="s">
+      <c r="A120" s="34" t="s">
         <v>181</v>
       </c>
       <c r="C120" s="6" t="s">
@@ -2243,7 +2243,7 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="37" t="s">
+      <c r="A121" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -2251,7 +2251,7 @@
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="37" t="s">
+      <c r="A122" s="34" t="s">
         <v>199</v>
       </c>
       <c r="C122" s="22" t="s">
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A123" s="37" t="s">
+      <c r="A123" s="34" t="s">
         <v>202</v>
       </c>
       <c r="C123" s="22" t="s">
@@ -2267,62 +2267,62 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="44" t="s">
+      <c r="A124" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="B124" s="45"/>
-      <c r="C124" s="46"/>
+      <c r="B124" s="43"/>
+      <c r="C124" s="44"/>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="37" t="s">
+      <c r="A125" s="34" t="s">
         <v>190</v>
       </c>
       <c r="C125" s="22"/>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="37" t="s">
+      <c r="A126" s="34" t="s">
         <v>191</v>
       </c>
       <c r="C126" s="22"/>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="37" t="s">
+      <c r="A127" s="34" t="s">
         <v>203</v>
       </c>
       <c r="C127" s="22"/>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="37" t="s">
+      <c r="A128" s="34" t="s">
         <v>204</v>
       </c>
       <c r="C128" s="22"/>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="37" t="s">
+      <c r="A129" s="34" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="30" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A130" s="37" t="s">
+      <c r="A130" s="34" t="s">
         <v>255</v>
       </c>
       <c r="B130" s="31"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="44" t="s">
+      <c r="A131" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B131" s="45"/>
-      <c r="C131" s="46"/>
+      <c r="B131" s="43"/>
+      <c r="C131" s="44"/>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="34" t="s">
         <v>189</v>
       </c>
       <c r="C132" s="11"/>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="37" t="s">
+      <c r="A133" s="34" t="s">
         <v>176</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -2330,7 +2330,7 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="37" t="s">
+      <c r="A134" s="34" t="s">
         <v>192</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -2339,7 +2339,7 @@
       <c r="C134" s="12"/>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="37" t="s">
+      <c r="A135" s="34" t="s">
         <v>248</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="37" t="s">
+      <c r="A136" s="34" t="s">
         <v>249</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -2355,28 +2355,28 @@
       </c>
     </row>
     <row r="137" spans="1:3" s="29" customFormat="1">
-      <c r="A137" s="37" t="s">
+      <c r="A137" s="34" t="s">
         <v>250</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="36" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A138" s="37" t="s">
+    <row r="138" spans="1:3" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A138" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="B138" s="37"/>
+      <c r="B138" s="34"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="44" t="s">
+      <c r="A139" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B139" s="45"/>
-      <c r="C139" s="46"/>
+      <c r="B139" s="43"/>
+      <c r="C139" s="44"/>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="37" t="s">
+      <c r="A140" s="34" t="s">
         <v>22</v>
       </c>
       <c r="C140" s="19" t="s">
@@ -2384,7 +2384,7 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="37" t="s">
+      <c r="A141" s="34" t="s">
         <v>52</v>
       </c>
       <c r="B141" s="2"/>
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="37" t="s">
+      <c r="A142" s="34" t="s">
         <v>136</v>
       </c>
       <c r="C142" s="22" t="s">
@@ -2401,31 +2401,31 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="37" t="s">
+      <c r="A143" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="C143" s="36" t="s">
+      <c r="C143" s="33" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="144" spans="1:3" s="43" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A144" s="42" t="s">
+    <row r="144" spans="1:3" s="40" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A144" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="B144" s="42"/>
-      <c r="C144" s="43" t="s">
+      <c r="B144" s="39"/>
+      <c r="C144" s="40" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="44" t="s">
+      <c r="A145" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="B145" s="45"/>
-      <c r="C145" s="46"/>
+      <c r="B145" s="43"/>
+      <c r="C145" s="44"/>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="37" t="s">
+      <c r="A146" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C146" t="s">
@@ -2433,7 +2433,7 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="37" t="s">
+      <c r="A147" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C147" t="s">
@@ -2441,7 +2441,7 @@
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="37" t="s">
+      <c r="A148" s="34" t="s">
         <v>30</v>
       </c>
       <c r="C148" t="s">
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="37" t="s">
+      <c r="A149" s="34" t="s">
         <v>68</v>
       </c>
       <c r="B149" s="2" t="s">
@@ -2461,14 +2461,14 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="44" t="s">
+      <c r="A153" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="B153" s="45"/>
-      <c r="C153" s="46"/>
+      <c r="B153" s="43"/>
+      <c r="C153" s="44"/>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="37" t="s">
+      <c r="A154" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -2477,40 +2477,40 @@
       <c r="C154" s="22"/>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="37" t="s">
+      <c r="A155" s="34" t="s">
         <v>142</v>
       </c>
       <c r="C155" s="22"/>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="37" t="s">
+      <c r="A156" s="34" t="s">
         <v>143</v>
       </c>
       <c r="C156" s="22"/>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="37" t="s">
+      <c r="A157" s="34" t="s">
         <v>149</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" s="22"/>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="37" t="s">
+      <c r="A158" s="34" t="s">
         <v>150</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="22"/>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="37" t="s">
+      <c r="A159" s="34" t="s">
         <v>151</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="22"/>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="37" t="s">
+      <c r="A160" s="34" t="s">
         <v>152</v>
       </c>
       <c r="B160" s="2"/>
@@ -2518,14 +2518,14 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="44" t="s">
+      <c r="A163" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="B163" s="45"/>
-      <c r="C163" s="46"/>
+      <c r="B163" s="43"/>
+      <c r="C163" s="44"/>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="37" t="s">
+      <c r="A164" s="34" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="4" t="s">
@@ -2533,59 +2533,59 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="30">
-      <c r="A165" s="37" t="s">
+      <c r="A165" s="34" t="s">
         <v>28</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C165" s="47"/>
+      <c r="C165" s="49"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
-      <c r="A166" s="37"/>
+      <c r="A166" s="34"/>
       <c r="B166" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C166" s="47"/>
+      <c r="C166" s="49"/>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="37" t="s">
+      <c r="A167" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="44" t="s">
+      <c r="A170" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B170" s="45"/>
-      <c r="C170" s="46"/>
+      <c r="B170" s="43"/>
+      <c r="C170" s="44"/>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" s="37" t="s">
+      <c r="A171" s="34" t="s">
         <v>209</v>
       </c>
       <c r="C171" s="22"/>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="37" t="s">
+      <c r="A172" s="34" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="173" spans="1:3" s="24" customFormat="1">
-      <c r="A173" s="37" t="s">
+      <c r="A173" s="34" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="174" spans="1:3" s="24" customFormat="1">
-      <c r="A174" s="37" t="s">
+      <c r="A174" s="34" t="s">
         <v>238</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="22"/>
     </row>
     <row r="175" spans="1:3" s="24" customFormat="1">
-      <c r="A175" s="37" t="s">
+      <c r="A175" s="34" t="s">
         <v>257</v>
       </c>
       <c r="B175" s="1"/>
@@ -2593,182 +2593,182 @@
     <row r="177" spans="1:3" s="28" customFormat="1" ht="15.75" thickBot="1">
       <c r="B177" s="1"/>
     </row>
-    <row r="178" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="44" t="s">
+    <row r="178" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A178" s="42" t="s">
         <v>278</v>
       </c>
-      <c r="B178" s="45"/>
-      <c r="C178" s="46"/>
-    </row>
-    <row r="179" spans="1:3" s="41" customFormat="1">
-      <c r="A179" s="40" t="s">
+      <c r="B178" s="43"/>
+      <c r="C178" s="44"/>
+    </row>
+    <row r="179" spans="1:3" s="38" customFormat="1">
+      <c r="A179" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="B179" s="40"/>
-    </row>
-    <row r="180" spans="1:3" s="41" customFormat="1">
-      <c r="A180" s="40" t="s">
+      <c r="B179" s="37"/>
+    </row>
+    <row r="180" spans="1:3" s="38" customFormat="1">
+      <c r="A180" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B180" s="40"/>
-    </row>
-    <row r="181" spans="1:3" s="41" customFormat="1">
-      <c r="A181" s="40" t="s">
+      <c r="B180" s="37"/>
+    </row>
+    <row r="181" spans="1:3" s="38" customFormat="1">
+      <c r="A181" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="B181" s="40"/>
-    </row>
-    <row r="182" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A182" s="40"/>
-      <c r="B182" s="40"/>
-    </row>
-    <row r="183" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="44" t="s">
+      <c r="B181" s="37"/>
+    </row>
+    <row r="182" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A182" s="37"/>
+      <c r="B182" s="37"/>
+    </row>
+    <row r="183" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A183" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="B183" s="45"/>
-      <c r="C183" s="46"/>
-    </row>
-    <row r="184" spans="1:3" s="41" customFormat="1">
-      <c r="A184" s="40" t="s">
+      <c r="B183" s="43"/>
+      <c r="C183" s="44"/>
+    </row>
+    <row r="184" spans="1:3" s="38" customFormat="1">
+      <c r="A184" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="B184" s="40"/>
-    </row>
-    <row r="185" spans="1:3" s="41" customFormat="1">
-      <c r="A185" s="40" t="s">
+      <c r="B184" s="37"/>
+    </row>
+    <row r="185" spans="1:3" s="38" customFormat="1">
+      <c r="A185" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="B185" s="40"/>
+      <c r="B185" s="37"/>
     </row>
     <row r="186" spans="1:3" s="28" customFormat="1">
-      <c r="A186" s="40" t="s">
+      <c r="A186" s="37" t="s">
         <v>282</v>
       </c>
       <c r="B186" s="1"/>
     </row>
-    <row r="187" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A187" s="40"/>
-      <c r="B187" s="40"/>
-    </row>
-    <row r="188" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="44" t="s">
+    <row r="187" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A187" s="37"/>
+      <c r="B187" s="37"/>
+    </row>
+    <row r="188" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A188" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="B188" s="45"/>
-      <c r="C188" s="46"/>
-    </row>
-    <row r="189" spans="1:3" s="41" customFormat="1">
-      <c r="A189" s="40" t="s">
+      <c r="B188" s="43"/>
+      <c r="C188" s="44"/>
+    </row>
+    <row r="189" spans="1:3" s="38" customFormat="1">
+      <c r="A189" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B189" s="40"/>
-    </row>
-    <row r="190" spans="1:3" s="41" customFormat="1">
-      <c r="A190" s="40"/>
-      <c r="B190" s="40"/>
-    </row>
-    <row r="191" spans="1:3" s="41" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A191" s="40"/>
-      <c r="B191" s="40"/>
+      <c r="B189" s="37"/>
+    </row>
+    <row r="190" spans="1:3" s="38" customFormat="1">
+      <c r="A190" s="37"/>
+      <c r="B190" s="37"/>
+    </row>
+    <row r="191" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A191" s="37"/>
+      <c r="B191" s="37"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="44" t="s">
+      <c r="A192" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="B192" s="45"/>
-      <c r="C192" s="46"/>
+      <c r="B192" s="43"/>
+      <c r="C192" s="44"/>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="37" t="s">
+      <c r="A193" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C193" s="22"/>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="37" t="s">
+      <c r="A194" s="34" t="s">
         <v>196</v>
       </c>
       <c r="C194" s="20"/>
     </row>
     <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="44" t="s">
+      <c r="A197" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="B197" s="45"/>
-      <c r="C197" s="46"/>
+      <c r="B197" s="43"/>
+      <c r="C197" s="44"/>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="37" t="s">
+      <c r="A198" s="34" t="s">
         <v>275</v>
       </c>
       <c r="B198" s="2"/>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="37" t="s">
+      <c r="A199" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="37" t="s">
+      <c r="A200" s="34" t="s">
         <v>274</v>
       </c>
       <c r="B200" s="2"/>
     </row>
-    <row r="201" spans="1:3" s="36" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A201" s="37" t="s">
+    <row r="201" spans="1:3" s="33" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A201" s="34" t="s">
         <v>273</v>
       </c>
       <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A202" s="44" t="s">
+      <c r="A202" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="B202" s="45"/>
-      <c r="C202" s="46"/>
+      <c r="B202" s="43"/>
+      <c r="C202" s="44"/>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="37" t="s">
+      <c r="A203" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C203" s="10"/>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="39" t="s">
+      <c r="A204" s="36" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="39" t="s">
+      <c r="A205" s="36" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="206" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A206" s="39"/>
+      <c r="A206" s="36"/>
       <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A207" s="44" t="s">
+      <c r="A207" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="B207" s="45"/>
-      <c r="C207" s="46"/>
+      <c r="B207" s="43"/>
+      <c r="C207" s="44"/>
     </row>
     <row r="208" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A208" s="39"/>
+      <c r="A208" s="36"/>
       <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="44" t="s">
+      <c r="A209" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="B209" s="45"/>
-      <c r="C209" s="46"/>
+      <c r="B209" s="43"/>
+      <c r="C209" s="44"/>
     </row>
     <row r="210" spans="1:3" s="26" customFormat="1">
-      <c r="A210" s="37" t="s">
+      <c r="A210" s="34" t="s">
         <v>232</v>
       </c>
       <c r="B210" s="27" t="s">
@@ -2776,40 +2776,40 @@
       </c>
     </row>
     <row r="211" spans="1:3">
-      <c r="A211" s="37" t="s">
+      <c r="A211" s="34" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="37" t="s">
+      <c r="A212" s="34" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="37" t="s">
+      <c r="A213" s="34" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="37" t="s">
+      <c r="A214" s="34" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="37" t="s">
+      <c r="A215" s="34" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="217" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A217" s="44" t="s">
+      <c r="A217" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="B217" s="45"/>
-      <c r="C217" s="46"/>
+      <c r="B217" s="43"/>
+      <c r="C217" s="44"/>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="37" t="s">
+      <c r="A218" s="34" t="s">
         <v>235</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -2817,60 +2817,60 @@
       </c>
     </row>
     <row r="219" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A219" s="37" t="s">
+      <c r="A219" s="34" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="44" t="s">
+      <c r="A220" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="B220" s="45"/>
-      <c r="C220" s="46"/>
+      <c r="B220" s="43"/>
+      <c r="C220" s="44"/>
     </row>
     <row r="221" spans="1:3">
-      <c r="A221" s="37" t="s">
+      <c r="A221" s="34" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="37" t="s">
+      <c r="A222" s="34" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="225" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A225" s="44" t="s">
+      <c r="A225" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="B225" s="45"/>
-      <c r="C225" s="46"/>
+      <c r="B225" s="43"/>
+      <c r="C225" s="44"/>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="37" t="s">
+      <c r="A226" s="34" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="37" t="s">
+      <c r="A227" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="37" t="s">
+      <c r="A228" s="34" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A231" s="44" t="s">
+      <c r="A231" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="B231" s="45"/>
-      <c r="C231" s="46"/>
+      <c r="B231" s="43"/>
+      <c r="C231" s="44"/>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="37" t="s">
+      <c r="A232" s="34" t="s">
         <v>79</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -2879,55 +2879,55 @@
       <c r="C232" s="15"/>
     </row>
     <row r="233" spans="1:3">
-      <c r="A233" s="37" t="s">
+      <c r="A233" s="34" t="s">
         <v>183</v>
       </c>
       <c r="C233" s="16"/>
     </row>
     <row r="234" spans="1:3">
-      <c r="A234" s="37" t="s">
+      <c r="A234" s="34" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="235" spans="1:3">
-      <c r="A235" s="37" t="s">
+      <c r="A235" s="34" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="44" t="s">
+      <c r="A237" s="42" t="s">
         <v>276</v>
       </c>
-      <c r="B237" s="45"/>
-      <c r="C237" s="46"/>
+      <c r="B237" s="43"/>
+      <c r="C237" s="44"/>
     </row>
     <row r="238" spans="1:3">
-      <c r="A238" s="37" t="s">
+      <c r="A238" s="34" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="239" spans="1:3">
-      <c r="A239" s="37" t="s">
+      <c r="A239" s="34" t="s">
         <v>27</v>
       </c>
       <c r="B239" s="2"/>
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="44" t="s">
+      <c r="A241" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="B241" s="45"/>
-      <c r="C241" s="46"/>
+      <c r="B241" s="43"/>
+      <c r="C241" s="44"/>
     </row>
     <row r="242" spans="1:3">
-      <c r="A242" s="37" t="s">
+      <c r="A242" s="34" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="37" t="s">
+      <c r="A243" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B243" s="1" t="s">
@@ -2935,158 +2935,163 @@
       </c>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="37" t="s">
+      <c r="A244" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B244" s="50" t="s">
+      <c r="B244" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C244" s="51"/>
+      <c r="C244" s="48"/>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="37" t="s">
+      <c r="A245" s="34" t="s">
         <v>58</v>
       </c>
       <c r="C245" s="13"/>
     </row>
     <row r="246" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A247" s="44" t="s">
+      <c r="A247" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B247" s="45"/>
-      <c r="C247" s="46"/>
+      <c r="B247" s="43"/>
+      <c r="C247" s="44"/>
     </row>
     <row r="248" spans="1:3">
-      <c r="A248" s="37" t="s">
+      <c r="A248" s="34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
-      <c r="A249" s="37" t="s">
+    <row r="249" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A249" s="34" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A250" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="B250" s="43"/>
+      <c r="C250" s="44"/>
+    </row>
+    <row r="251" spans="1:3" ht="30">
+      <c r="A251" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="34" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="255" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A255" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="B255" s="34"/>
-      <c r="C255" s="35"/>
-    </row>
-    <row r="256" spans="1:3" ht="30">
-      <c r="A256" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="B256" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="A257" s="37" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258" s="37" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="260" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A260" s="33" t="s">
+      <c r="A255" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="B260" s="34"/>
-      <c r="C260" s="35"/>
+      <c r="B255" s="43"/>
+      <c r="C255" s="44"/>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C256" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="259" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A259" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B259" s="43"/>
+      <c r="C259" s="44"/>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C260" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="C261" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="264" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A264" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B264" s="34"/>
-      <c r="C264" s="35"/>
+      <c r="A261" s="46"/>
+      <c r="B261" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="263" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A263" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="B263" s="43"/>
+      <c r="C263" s="44"/>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="34" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="265" spans="1:3">
-      <c r="A265" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C265" t="s">
-        <v>169</v>
+      <c r="A265" s="34" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="266" spans="1:3">
-      <c r="A266" s="49"/>
-      <c r="B266" s="32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="268" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A268" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="B268" s="34"/>
-      <c r="C268" s="35"/>
+      <c r="A266" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="34" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="269" spans="1:3">
-      <c r="A269" s="37" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" s="37" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271" s="37" t="s">
-        <v>267</v>
-      </c>
+      <c r="A269" s="34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="271" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A271" s="42"/>
+      <c r="B271" s="43"/>
+      <c r="C271" s="44"/>
     </row>
     <row r="272" spans="1:3">
-      <c r="A272" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1">
-      <c r="A273" s="37" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1">
-      <c r="A274" s="37" t="s">
-        <v>269</v>
+      <c r="A272" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A197:C197"/>
-    <mergeCell ref="A265:A266"/>
-    <mergeCell ref="B244:C244"/>
-    <mergeCell ref="A202:C202"/>
-    <mergeCell ref="A207:C207"/>
-    <mergeCell ref="A209:C209"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A220:C220"/>
-    <mergeCell ref="A225:C225"/>
-    <mergeCell ref="A231:C231"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A241:C241"/>
-    <mergeCell ref="A247:C247"/>
+  <mergeCells count="30">
+    <mergeCell ref="A263:C263"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A271:C271"/>
     <mergeCell ref="A192:C192"/>
     <mergeCell ref="A124:C124"/>
     <mergeCell ref="A131:C131"/>
@@ -3099,6 +3104,19 @@
     <mergeCell ref="A178:C178"/>
     <mergeCell ref="A183:C183"/>
     <mergeCell ref="A188:C188"/>
+    <mergeCell ref="A197:C197"/>
+    <mergeCell ref="A260:A261"/>
+    <mergeCell ref="B244:C244"/>
+    <mergeCell ref="A202:C202"/>
+    <mergeCell ref="A207:C207"/>
+    <mergeCell ref="A209:C209"/>
+    <mergeCell ref="A217:C217"/>
+    <mergeCell ref="A220:C220"/>
+    <mergeCell ref="A225:C225"/>
+    <mergeCell ref="A231:C231"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A241:C241"/>
+    <mergeCell ref="A247:C247"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
@@ -3116,14 +3134,14 @@
     <hyperlink ref="B78" r:id="rId13"/>
     <hyperlink ref="B72" r:id="rId14"/>
     <hyperlink ref="B66" r:id="rId15"/>
-    <hyperlink ref="B265" r:id="rId16"/>
+    <hyperlink ref="B260" r:id="rId16"/>
     <hyperlink ref="B42" r:id="rId17" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
     <hyperlink ref="B41" r:id="rId18"/>
     <hyperlink ref="B94" r:id="rId19"/>
     <hyperlink ref="B95" r:id="rId20"/>
     <hyperlink ref="B35" r:id="rId21"/>
     <hyperlink ref="B141" r:id="rId22" display="http://www.tutorialspoint.com/restful/index.htm"/>
-    <hyperlink ref="B256" r:id="rId23"/>
+    <hyperlink ref="B251" r:id="rId23"/>
     <hyperlink ref="B62" r:id="rId24"/>
     <hyperlink ref="B107" r:id="rId25"/>
     <hyperlink ref="B108" r:id="rId26" location="commandLine"/>
@@ -3134,8 +3152,9 @@
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
     <hyperlink ref="B166" r:id="rId31"/>
     <hyperlink ref="B210" r:id="rId32"/>
+    <hyperlink ref="B272" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scala, Gradle, Spring MVC
Scala, Gradle, Spring MVC
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="290">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -896,6 +896,9 @@
   </si>
   <si>
     <t>JWT (JSON WEB TOKENS)</t>
+  </si>
+  <si>
+    <t>n_scala.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1051,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1121,6 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1130,6 +1134,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1142,7 +1147,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1441,8 +1445,8 @@
   <dimension ref="A1:D272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A207" sqref="A207:C207"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2109,57 +2113,60 @@
       </c>
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:3">
       <c r="A97" s="34" t="s">
         <v>144</v>
       </c>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:3">
       <c r="A98" s="34" t="s">
         <v>145</v>
       </c>
       <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" s="42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="34" t="s">
         <v>146</v>
       </c>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:3">
       <c r="A100" s="34" t="s">
         <v>147</v>
       </c>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:3">
       <c r="A101" s="34" t="s">
         <v>148</v>
       </c>
       <c r="B101" s="2"/>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:3">
       <c r="A103" s="34" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:3">
       <c r="A104" s="34" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:3">
       <c r="A105" s="34" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:3">
       <c r="A106" s="34" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:3">
       <c r="A107" s="34" t="s">
         <v>159</v>
       </c>
@@ -2167,7 +2174,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:3">
       <c r="A108" s="34" t="s">
         <v>161</v>
       </c>
@@ -2175,7 +2182,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:3">
       <c r="A109" s="34" t="s">
         <v>163</v>
       </c>
@@ -2183,12 +2190,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:3">
       <c r="A110" s="34" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:3">
       <c r="A112" s="34" t="s">
         <v>173</v>
       </c>
@@ -2270,11 +2277,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="42" t="s">
+      <c r="A124" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="B124" s="43"/>
-      <c r="C124" s="44"/>
+      <c r="B124" s="44"/>
+      <c r="C124" s="45"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="34" t="s">
@@ -2312,11 +2319,11 @@
       <c r="B130" s="31"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="42" t="s">
+      <c r="A131" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="B131" s="43"/>
-      <c r="C131" s="44"/>
+      <c r="B131" s="44"/>
+      <c r="C131" s="45"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="34" t="s">
@@ -2372,11 +2379,11 @@
       <c r="B138" s="34"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="42" t="s">
+      <c r="A139" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="B139" s="43"/>
-      <c r="C139" s="44"/>
+      <c r="B139" s="44"/>
+      <c r="C139" s="45"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="34" t="s">
@@ -2421,11 +2428,11 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="42" t="s">
+      <c r="A145" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="B145" s="43"/>
-      <c r="C145" s="44"/>
+      <c r="B145" s="44"/>
+      <c r="C145" s="45"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="34" t="s">
@@ -2464,11 +2471,11 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="42" t="s">
+      <c r="A153" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="B153" s="43"/>
-      <c r="C153" s="44"/>
+      <c r="B153" s="44"/>
+      <c r="C153" s="45"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="34" t="s">
@@ -2521,11 +2528,11 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="42" t="s">
+      <c r="A163" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="B163" s="43"/>
-      <c r="C163" s="44"/>
+      <c r="B163" s="44"/>
+      <c r="C163" s="45"/>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="34" t="s">
@@ -2542,14 +2549,14 @@
       <c r="B165" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C165" s="49"/>
+      <c r="C165" s="46"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A166" s="34"/>
       <c r="B166" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C166" s="49"/>
+      <c r="C166" s="46"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="34" t="s">
@@ -2558,11 +2565,11 @@
     </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="42" t="s">
+      <c r="A170" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="B170" s="43"/>
-      <c r="C170" s="44"/>
+      <c r="B170" s="44"/>
+      <c r="C170" s="45"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="34" t="s">
@@ -2597,11 +2604,11 @@
       <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="42" t="s">
+      <c r="A178" s="43" t="s">
         <v>278</v>
       </c>
-      <c r="B178" s="43"/>
-      <c r="C178" s="44"/>
+      <c r="B178" s="44"/>
+      <c r="C178" s="45"/>
     </row>
     <row r="179" spans="1:3" s="38" customFormat="1">
       <c r="A179" s="37" t="s">
@@ -2626,11 +2633,11 @@
       <c r="B182" s="37"/>
     </row>
     <row r="183" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="42" t="s">
+      <c r="A183" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="B183" s="43"/>
-      <c r="C183" s="44"/>
+      <c r="B183" s="44"/>
+      <c r="C183" s="45"/>
     </row>
     <row r="184" spans="1:3" s="38" customFormat="1">
       <c r="A184" s="37" t="s">
@@ -2655,11 +2662,11 @@
       <c r="B187" s="37"/>
     </row>
     <row r="188" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="42" t="s">
+      <c r="A188" s="43" t="s">
         <v>283</v>
       </c>
-      <c r="B188" s="43"/>
-      <c r="C188" s="44"/>
+      <c r="B188" s="44"/>
+      <c r="C188" s="45"/>
     </row>
     <row r="189" spans="1:3" s="38" customFormat="1">
       <c r="A189" s="37" t="s">
@@ -2676,11 +2683,11 @@
       <c r="B191" s="37"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="42" t="s">
+      <c r="A192" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="B192" s="43"/>
-      <c r="C192" s="44"/>
+      <c r="B192" s="44"/>
+      <c r="C192" s="45"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="34" t="s">
@@ -2696,11 +2703,11 @@
     </row>
     <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="42" t="s">
+      <c r="A197" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B197" s="43"/>
-      <c r="C197" s="44"/>
+      <c r="B197" s="44"/>
+      <c r="C197" s="45"/>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="34" t="s">
@@ -2726,11 +2733,11 @@
       <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A202" s="42" t="s">
+      <c r="A202" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="B202" s="43"/>
-      <c r="C202" s="44"/>
+      <c r="B202" s="44"/>
+      <c r="C202" s="45"/>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="34" t="s">
@@ -2755,22 +2762,22 @@
       <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A207" s="42" t="s">
+      <c r="A207" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="B207" s="43"/>
-      <c r="C207" s="44"/>
+      <c r="B207" s="44"/>
+      <c r="C207" s="45"/>
     </row>
     <row r="208" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
       <c r="A208" s="36"/>
       <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="42" t="s">
+      <c r="A209" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="B209" s="43"/>
-      <c r="C209" s="44"/>
+      <c r="B209" s="44"/>
+      <c r="C209" s="45"/>
     </row>
     <row r="210" spans="1:3" s="26" customFormat="1">
       <c r="A210" s="34" t="s">
@@ -2807,11 +2814,11 @@
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="217" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A217" s="42" t="s">
+      <c r="A217" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="B217" s="43"/>
-      <c r="C217" s="44"/>
+      <c r="B217" s="44"/>
+      <c r="C217" s="45"/>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="34" t="s">
@@ -2827,11 +2834,11 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="42" t="s">
+      <c r="A220" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="B220" s="43"/>
-      <c r="C220" s="44"/>
+      <c r="B220" s="44"/>
+      <c r="C220" s="45"/>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="34" t="s">
@@ -2845,11 +2852,11 @@
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="225" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A225" s="42" t="s">
+      <c r="A225" s="43" t="s">
         <v>244</v>
       </c>
-      <c r="B225" s="43"/>
-      <c r="C225" s="44"/>
+      <c r="B225" s="44"/>
+      <c r="C225" s="45"/>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="34" t="s">
@@ -2868,11 +2875,11 @@
     </row>
     <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A231" s="42" t="s">
+      <c r="A231" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="B231" s="43"/>
-      <c r="C231" s="44"/>
+      <c r="B231" s="44"/>
+      <c r="C231" s="45"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="34" t="s">
@@ -2901,11 +2908,11 @@
     </row>
     <row r="236" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="42" t="s">
+      <c r="A237" s="43" t="s">
         <v>276</v>
       </c>
-      <c r="B237" s="43"/>
-      <c r="C237" s="44"/>
+      <c r="B237" s="44"/>
+      <c r="C237" s="45"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="34" t="s">
@@ -2920,11 +2927,11 @@
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="42" t="s">
+      <c r="A241" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B241" s="43"/>
-      <c r="C241" s="44"/>
+      <c r="B241" s="44"/>
+      <c r="C241" s="45"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="34" t="s">
@@ -2943,10 +2950,10 @@
       <c r="A244" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B244" s="47" t="s">
+      <c r="B244" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C244" s="48"/>
+      <c r="C244" s="50"/>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="34" t="s">
@@ -2956,11 +2963,11 @@
     </row>
     <row r="246" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A247" s="42" t="s">
+      <c r="A247" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="B247" s="43"/>
-      <c r="C247" s="44"/>
+      <c r="B247" s="44"/>
+      <c r="C247" s="45"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="34" t="s">
@@ -2973,11 +2980,11 @@
       </c>
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="42" t="s">
+      <c r="A250" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="B250" s="43"/>
-      <c r="C250" s="44"/>
+      <c r="B250" s="44"/>
+      <c r="C250" s="45"/>
     </row>
     <row r="251" spans="1:3" ht="30">
       <c r="A251" s="34" t="s">
@@ -2999,11 +3006,11 @@
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="255" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A255" s="42" t="s">
+      <c r="A255" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="B255" s="43"/>
-      <c r="C255" s="44"/>
+      <c r="B255" s="44"/>
+      <c r="C255" s="45"/>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="34" t="s">
@@ -3015,14 +3022,14 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="42" t="s">
+      <c r="A259" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B259" s="43"/>
-      <c r="C259" s="44"/>
+      <c r="B259" s="44"/>
+      <c r="C259" s="45"/>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" s="45" t="s">
+      <c r="A260" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B260" s="2" t="s">
@@ -3033,18 +3040,18 @@
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="46"/>
+      <c r="A261" s="48"/>
       <c r="B261" s="32" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="263" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A263" s="42" t="s">
+      <c r="A263" s="43" t="s">
         <v>270</v>
       </c>
-      <c r="B263" s="43"/>
-      <c r="C263" s="44"/>
+      <c r="B263" s="44"/>
+      <c r="C263" s="45"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="34" t="s">
@@ -3078,9 +3085,9 @@
     </row>
     <row r="270" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="271" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A271" s="42"/>
-      <c r="B271" s="43"/>
-      <c r="C271" s="44"/>
+      <c r="A271" s="43"/>
+      <c r="B271" s="44"/>
+      <c r="C271" s="45"/>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="41" t="s">
@@ -3092,23 +3099,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A263:C263"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A271:C271"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A260:A261"/>
     <mergeCell ref="B244:C244"/>
@@ -3122,6 +3112,23 @@
     <mergeCell ref="A237:C237"/>
     <mergeCell ref="A241:C241"/>
     <mergeCell ref="A247:C247"/>
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="A263:C263"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A271:C271"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
Junit, Apache Kafka, Spring
Junit, Apache Kafka, Spring
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="293">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -902,6 +902,12 @@
   </si>
   <si>
     <t>Dozer</t>
+  </si>
+  <si>
+    <t>Bean tools</t>
+  </si>
+  <si>
+    <t>Apache Kafka</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1131,6 +1137,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1140,6 +1149,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1152,7 +1162,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1451,8 +1460,8 @@
   <dimension ref="A1:D273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A274" sqref="A274"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A237" sqref="A237:C237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2283,11 +2292,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="44" t="s">
+      <c r="A124" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="B124" s="45"/>
-      <c r="C124" s="46"/>
+      <c r="B124" s="46"/>
+      <c r="C124" s="47"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="34" t="s">
@@ -2325,11 +2334,11 @@
       <c r="B130" s="31"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="44" t="s">
+      <c r="A131" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="B131" s="45"/>
-      <c r="C131" s="46"/>
+      <c r="B131" s="46"/>
+      <c r="C131" s="47"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="34" t="s">
@@ -2385,11 +2394,11 @@
       <c r="B138" s="34"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="44" t="s">
+      <c r="A139" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="B139" s="45"/>
-      <c r="C139" s="46"/>
+      <c r="B139" s="46"/>
+      <c r="C139" s="47"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="34" t="s">
@@ -2434,11 +2443,11 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="44" t="s">
+      <c r="A145" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="B145" s="45"/>
-      <c r="C145" s="46"/>
+      <c r="B145" s="46"/>
+      <c r="C145" s="47"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="34" t="s">
@@ -2477,11 +2486,11 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="44" t="s">
+      <c r="A153" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="B153" s="45"/>
-      <c r="C153" s="46"/>
+      <c r="B153" s="46"/>
+      <c r="C153" s="47"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="34" t="s">
@@ -2534,11 +2543,11 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="44" t="s">
+      <c r="A163" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="45"/>
-      <c r="C163" s="46"/>
+      <c r="B163" s="46"/>
+      <c r="C163" s="47"/>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="34" t="s">
@@ -2555,14 +2564,14 @@
       <c r="B165" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C165" s="51"/>
+      <c r="C165" s="48"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A166" s="34"/>
       <c r="B166" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C166" s="51"/>
+      <c r="C166" s="48"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="43" t="s">
@@ -2571,11 +2580,11 @@
     </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="44" t="s">
+      <c r="A170" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="B170" s="45"/>
-      <c r="C170" s="46"/>
+      <c r="B170" s="46"/>
+      <c r="C170" s="47"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="34" t="s">
@@ -2610,11 +2619,11 @@
       <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="44" t="s">
+      <c r="A178" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="B178" s="45"/>
-      <c r="C178" s="46"/>
+      <c r="B178" s="46"/>
+      <c r="C178" s="47"/>
     </row>
     <row r="179" spans="1:3" s="38" customFormat="1">
       <c r="A179" s="37" t="s">
@@ -2639,11 +2648,11 @@
       <c r="B182" s="37"/>
     </row>
     <row r="183" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="44" t="s">
+      <c r="A183" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="B183" s="45"/>
-      <c r="C183" s="46"/>
+      <c r="B183" s="46"/>
+      <c r="C183" s="47"/>
     </row>
     <row r="184" spans="1:3" s="38" customFormat="1">
       <c r="A184" s="37" t="s">
@@ -2668,11 +2677,11 @@
       <c r="B187" s="37"/>
     </row>
     <row r="188" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="44" t="s">
+      <c r="A188" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="B188" s="45"/>
-      <c r="C188" s="46"/>
+      <c r="B188" s="46"/>
+      <c r="C188" s="47"/>
     </row>
     <row r="189" spans="1:3" s="38" customFormat="1">
       <c r="A189" s="37" t="s">
@@ -2689,11 +2698,11 @@
       <c r="B191" s="37"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="44" t="s">
+      <c r="A192" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="B192" s="45"/>
-      <c r="C192" s="46"/>
+      <c r="B192" s="46"/>
+      <c r="C192" s="47"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="34" t="s">
@@ -2709,11 +2718,11 @@
     </row>
     <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="44" t="s">
+      <c r="A197" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="B197" s="45"/>
-      <c r="C197" s="46"/>
+      <c r="B197" s="46"/>
+      <c r="C197" s="47"/>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="34" t="s">
@@ -2739,11 +2748,11 @@
       <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A202" s="44" t="s">
+      <c r="A202" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="B202" s="45"/>
-      <c r="C202" s="46"/>
+      <c r="B202" s="46"/>
+      <c r="C202" s="47"/>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="34" t="s">
@@ -2768,22 +2777,22 @@
       <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A207" s="44" t="s">
+      <c r="A207" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="B207" s="45"/>
-      <c r="C207" s="46"/>
+      <c r="B207" s="46"/>
+      <c r="C207" s="47"/>
     </row>
     <row r="208" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
       <c r="A208" s="36"/>
       <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="44" t="s">
+      <c r="A209" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="B209" s="45"/>
-      <c r="C209" s="46"/>
+      <c r="B209" s="46"/>
+      <c r="C209" s="47"/>
     </row>
     <row r="210" spans="1:3" s="26" customFormat="1">
       <c r="A210" s="34" t="s">
@@ -2820,11 +2829,11 @@
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="217" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A217" s="44" t="s">
+      <c r="A217" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="B217" s="45"/>
-      <c r="C217" s="46"/>
+      <c r="B217" s="46"/>
+      <c r="C217" s="47"/>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="34" t="s">
@@ -2840,11 +2849,11 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="44" t="s">
+      <c r="A220" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="B220" s="45"/>
-      <c r="C220" s="46"/>
+      <c r="B220" s="46"/>
+      <c r="C220" s="47"/>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="34" t="s">
@@ -2858,11 +2867,11 @@
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="225" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A225" s="44" t="s">
+      <c r="A225" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="B225" s="45"/>
-      <c r="C225" s="46"/>
+      <c r="B225" s="46"/>
+      <c r="C225" s="47"/>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="34" t="s">
@@ -2881,11 +2890,11 @@
     </row>
     <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A231" s="44" t="s">
+      <c r="A231" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="B231" s="45"/>
-      <c r="C231" s="46"/>
+      <c r="B231" s="46"/>
+      <c r="C231" s="47"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="34" t="s">
@@ -2912,13 +2921,17 @@
         <v>246</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="236" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A236" s="44" t="s">
+        <v>292</v>
+      </c>
+    </row>
     <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="44" t="s">
+      <c r="A237" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="B237" s="45"/>
-      <c r="C237" s="46"/>
+      <c r="B237" s="46"/>
+      <c r="C237" s="47"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="34" t="s">
@@ -2933,11 +2946,11 @@
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="44" t="s">
+      <c r="A241" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="B241" s="45"/>
-      <c r="C241" s="46"/>
+      <c r="B241" s="46"/>
+      <c r="C241" s="47"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="34" t="s">
@@ -2956,10 +2969,10 @@
       <c r="A244" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B244" s="49" t="s">
+      <c r="B244" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C244" s="50"/>
+      <c r="C244" s="52"/>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="34" t="s">
@@ -2969,11 +2982,11 @@
     </row>
     <row r="246" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A247" s="44" t="s">
+      <c r="A247" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="B247" s="45"/>
-      <c r="C247" s="46"/>
+      <c r="B247" s="46"/>
+      <c r="C247" s="47"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="34" t="s">
@@ -2986,11 +2999,11 @@
       </c>
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="44" t="s">
+      <c r="A250" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="B250" s="45"/>
-      <c r="C250" s="46"/>
+      <c r="B250" s="46"/>
+      <c r="C250" s="47"/>
     </row>
     <row r="251" spans="1:3" ht="30">
       <c r="A251" s="34" t="s">
@@ -3012,11 +3025,11 @@
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="255" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A255" s="44" t="s">
+      <c r="A255" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="B255" s="45"/>
-      <c r="C255" s="46"/>
+      <c r="B255" s="46"/>
+      <c r="C255" s="47"/>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="34" t="s">
@@ -3028,14 +3041,14 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="44" t="s">
+      <c r="A259" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B259" s="45"/>
-      <c r="C259" s="46"/>
+      <c r="B259" s="46"/>
+      <c r="C259" s="47"/>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" s="47" t="s">
+      <c r="A260" s="49" t="s">
         <v>40</v>
       </c>
       <c r="B260" s="2" t="s">
@@ -3046,18 +3059,18 @@
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="48"/>
+      <c r="A261" s="50"/>
       <c r="B261" s="32" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="263" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A263" s="44" t="s">
+      <c r="A263" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="B263" s="45"/>
-      <c r="C263" s="46"/>
+      <c r="B263" s="46"/>
+      <c r="C263" s="47"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="34" t="s">
@@ -3091,9 +3104,11 @@
     </row>
     <row r="270" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="271" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A271" s="44"/>
-      <c r="B271" s="45"/>
-      <c r="C271" s="46"/>
+      <c r="A271" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="B271" s="46"/>
+      <c r="C271" s="47"/>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="41" t="s">
@@ -3110,23 +3125,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A263:C263"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A271:C271"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A260:A261"/>
     <mergeCell ref="B244:C244"/>
@@ -3140,6 +3138,23 @@
     <mergeCell ref="A237:C237"/>
     <mergeCell ref="A241:C241"/>
     <mergeCell ref="A247:C247"/>
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="A263:C263"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A271:C271"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
Available 3rd party JSON Frameworks
Available 3rd party JSON Frameworks
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="300">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -908,6 +908,27 @@
   </si>
   <si>
     <t>Apache Kafka</t>
+  </si>
+  <si>
+    <t>JSON Frameworks - Cerebro</t>
+  </si>
+  <si>
+    <t>Jackson JSON</t>
+  </si>
+  <si>
+    <t>GSON</t>
+  </si>
+  <si>
+    <t>Boon</t>
+  </si>
+  <si>
+    <t>Simple JSON</t>
+  </si>
+  <si>
+    <t>Json.org</t>
+  </si>
+  <si>
+    <t>JSONP</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1081,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1140,6 +1161,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1149,7 +1173,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1162,6 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1457,11 +1481,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D273"/>
+  <dimension ref="A1:D281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A274" sqref="A274"/>
+      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2292,11 +2316,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="45" t="s">
+      <c r="A124" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="B124" s="46"/>
-      <c r="C124" s="47"/>
+      <c r="B124" s="47"/>
+      <c r="C124" s="48"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="34" t="s">
@@ -2334,11 +2358,11 @@
       <c r="B130" s="31"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="45" t="s">
+      <c r="A131" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="B131" s="46"/>
-      <c r="C131" s="47"/>
+      <c r="B131" s="47"/>
+      <c r="C131" s="48"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="34" t="s">
@@ -2394,11 +2418,11 @@
       <c r="B138" s="34"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="45" t="s">
+      <c r="A139" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="B139" s="46"/>
-      <c r="C139" s="47"/>
+      <c r="B139" s="47"/>
+      <c r="C139" s="48"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="34" t="s">
@@ -2443,11 +2467,11 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="45" t="s">
+      <c r="A145" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="B145" s="46"/>
-      <c r="C145" s="47"/>
+      <c r="B145" s="47"/>
+      <c r="C145" s="48"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="34" t="s">
@@ -2486,11 +2510,11 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="45" t="s">
+      <c r="A153" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="B153" s="46"/>
-      <c r="C153" s="47"/>
+      <c r="B153" s="47"/>
+      <c r="C153" s="48"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="34" t="s">
@@ -2543,11 +2567,11 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="45" t="s">
+      <c r="A163" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="46"/>
-      <c r="C163" s="47"/>
+      <c r="B163" s="47"/>
+      <c r="C163" s="48"/>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="34" t="s">
@@ -2564,14 +2588,14 @@
       <c r="B165" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C165" s="48"/>
+      <c r="C165" s="53"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A166" s="34"/>
       <c r="B166" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C166" s="48"/>
+      <c r="C166" s="53"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="43" t="s">
@@ -2580,11 +2604,11 @@
     </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="45" t="s">
+      <c r="A170" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="B170" s="46"/>
-      <c r="C170" s="47"/>
+      <c r="B170" s="47"/>
+      <c r="C170" s="48"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="34" t="s">
@@ -2619,11 +2643,11 @@
       <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="45" t="s">
+      <c r="A178" s="46" t="s">
         <v>277</v>
       </c>
-      <c r="B178" s="46"/>
-      <c r="C178" s="47"/>
+      <c r="B178" s="47"/>
+      <c r="C178" s="48"/>
     </row>
     <row r="179" spans="1:3" s="38" customFormat="1">
       <c r="A179" s="37" t="s">
@@ -2648,11 +2672,11 @@
       <c r="B182" s="37"/>
     </row>
     <row r="183" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="45" t="s">
+      <c r="A183" s="46" t="s">
         <v>278</v>
       </c>
-      <c r="B183" s="46"/>
-      <c r="C183" s="47"/>
+      <c r="B183" s="47"/>
+      <c r="C183" s="48"/>
     </row>
     <row r="184" spans="1:3" s="38" customFormat="1">
       <c r="A184" s="37" t="s">
@@ -2677,11 +2701,11 @@
       <c r="B187" s="37"/>
     </row>
     <row r="188" spans="1:3" s="38" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="45" t="s">
+      <c r="A188" s="46" t="s">
         <v>282</v>
       </c>
-      <c r="B188" s="46"/>
-      <c r="C188" s="47"/>
+      <c r="B188" s="47"/>
+      <c r="C188" s="48"/>
     </row>
     <row r="189" spans="1:3" s="38" customFormat="1">
       <c r="A189" s="37" t="s">
@@ -2698,11 +2722,11 @@
       <c r="B191" s="37"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="45" t="s">
+      <c r="A192" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="B192" s="46"/>
-      <c r="C192" s="47"/>
+      <c r="B192" s="47"/>
+      <c r="C192" s="48"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="34" t="s">
@@ -2718,11 +2742,11 @@
     </row>
     <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="45" t="s">
+      <c r="A197" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="B197" s="46"/>
-      <c r="C197" s="47"/>
+      <c r="B197" s="47"/>
+      <c r="C197" s="48"/>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="34" t="s">
@@ -2748,11 +2772,11 @@
       <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A202" s="45" t="s">
+      <c r="A202" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="B202" s="46"/>
-      <c r="C202" s="47"/>
+      <c r="B202" s="47"/>
+      <c r="C202" s="48"/>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="34" t="s">
@@ -2777,22 +2801,22 @@
       <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A207" s="45" t="s">
+      <c r="A207" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="B207" s="46"/>
-      <c r="C207" s="47"/>
+      <c r="B207" s="47"/>
+      <c r="C207" s="48"/>
     </row>
     <row r="208" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1">
       <c r="A208" s="36"/>
       <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="45" t="s">
+      <c r="A209" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="B209" s="46"/>
-      <c r="C209" s="47"/>
+      <c r="B209" s="47"/>
+      <c r="C209" s="48"/>
     </row>
     <row r="210" spans="1:3" s="26" customFormat="1">
       <c r="A210" s="34" t="s">
@@ -2829,11 +2853,11 @@
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="217" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A217" s="45" t="s">
+      <c r="A217" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="B217" s="46"/>
-      <c r="C217" s="47"/>
+      <c r="B217" s="47"/>
+      <c r="C217" s="48"/>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="34" t="s">
@@ -2849,11 +2873,11 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="45" t="s">
+      <c r="A220" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="B220" s="46"/>
-      <c r="C220" s="47"/>
+      <c r="B220" s="47"/>
+      <c r="C220" s="48"/>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="34" t="s">
@@ -2867,11 +2891,11 @@
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="225" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A225" s="45" t="s">
+      <c r="A225" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="B225" s="46"/>
-      <c r="C225" s="47"/>
+      <c r="B225" s="47"/>
+      <c r="C225" s="48"/>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="34" t="s">
@@ -2890,11 +2914,11 @@
     </row>
     <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A231" s="45" t="s">
+      <c r="A231" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="B231" s="46"/>
-      <c r="C231" s="47"/>
+      <c r="B231" s="47"/>
+      <c r="C231" s="48"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="34" t="s">
@@ -2927,11 +2951,11 @@
       </c>
     </row>
     <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="45" t="s">
+      <c r="A237" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="B237" s="46"/>
-      <c r="C237" s="47"/>
+      <c r="B237" s="47"/>
+      <c r="C237" s="48"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="34" t="s">
@@ -2946,11 +2970,11 @@
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="45" t="s">
+      <c r="A241" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="B241" s="46"/>
-      <c r="C241" s="47"/>
+      <c r="B241" s="47"/>
+      <c r="C241" s="48"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="34" t="s">
@@ -2982,11 +3006,11 @@
     </row>
     <row r="246" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A247" s="45" t="s">
+      <c r="A247" s="46" t="s">
         <v>252</v>
       </c>
-      <c r="B247" s="46"/>
-      <c r="C247" s="47"/>
+      <c r="B247" s="47"/>
+      <c r="C247" s="48"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="34" t="s">
@@ -2999,11 +3023,11 @@
       </c>
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="45" t="s">
+      <c r="A250" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="B250" s="46"/>
-      <c r="C250" s="47"/>
+      <c r="B250" s="47"/>
+      <c r="C250" s="48"/>
     </row>
     <row r="251" spans="1:3" ht="30">
       <c r="A251" s="34" t="s">
@@ -3025,11 +3049,11 @@
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="255" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A255" s="45" t="s">
+      <c r="A255" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="B255" s="46"/>
-      <c r="C255" s="47"/>
+      <c r="B255" s="47"/>
+      <c r="C255" s="48"/>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="34" t="s">
@@ -3041,11 +3065,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="45" t="s">
+      <c r="A259" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B259" s="46"/>
-      <c r="C259" s="47"/>
+      <c r="B259" s="47"/>
+      <c r="C259" s="48"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="49" t="s">
@@ -3066,11 +3090,11 @@
     </row>
     <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="263" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A263" s="45" t="s">
+      <c r="A263" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="B263" s="46"/>
-      <c r="C263" s="47"/>
+      <c r="B263" s="47"/>
+      <c r="C263" s="48"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="34" t="s">
@@ -3104,11 +3128,11 @@
     </row>
     <row r="270" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="271" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A271" s="45" t="s">
+      <c r="A271" s="46" t="s">
         <v>291</v>
       </c>
-      <c r="B271" s="46"/>
-      <c r="C271" s="47"/>
+      <c r="B271" s="47"/>
+      <c r="C271" s="48"/>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="41" t="s">
@@ -3118,13 +3142,69 @@
         <v>286</v>
       </c>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:3">
       <c r="A273" s="43" t="s">
         <v>290</v>
       </c>
     </row>
+    <row r="274" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="275" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A275" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="B275" s="47"/>
+      <c r="C275" s="48"/>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="45" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="45" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="45" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="45" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="45" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="45" t="s">
+        <v>299</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A263:C263"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A271:C271"/>
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A260:A261"/>
     <mergeCell ref="B244:C244"/>
@@ -3138,23 +3218,6 @@
     <mergeCell ref="A237:C237"/>
     <mergeCell ref="A241:C241"/>
     <mergeCell ref="A247:C247"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="A263:C263"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A271:C271"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
Cloud computing introduction course completed
Cloud computing introduction course completedz
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1182,7 +1182,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1195,6 +1194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1493,8 +1493,8 @@
   <dimension ref="A1:D284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A285" sqref="A285"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2592,14 +2592,14 @@
       <c r="B165" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C165" s="50"/>
+      <c r="C165" s="54"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A166" s="34"/>
       <c r="B166" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C166" s="50"/>
+      <c r="C166" s="54"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="43" t="s">
@@ -2997,10 +2997,10 @@
       <c r="A244" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B244" s="53" t="s">
+      <c r="B244" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C244" s="54"/>
+      <c r="C244" s="53"/>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="34" t="s">
@@ -3076,7 +3076,7 @@
       <c r="C259" s="49"/>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" s="51" t="s">
+      <c r="A260" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B260" s="2" t="s">
@@ -3087,7 +3087,7 @@
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="52"/>
+      <c r="A261" s="51"/>
       <c r="B261" s="32" t="s">
         <v>263</v>
       </c>
@@ -3204,6 +3204,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A271:C271"/>
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A283:C283"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A260:A261"/>
@@ -3218,24 +3234,8 @@
     <mergeCell ref="A237:C237"/>
     <mergeCell ref="A241:C241"/>
     <mergeCell ref="A247:C247"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A263:C263"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A271:C271"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
Spring, Web Services, Node JS
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="304">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t>p_Definitions_Mule.xlsx</t>
+  </si>
+  <si>
+    <t>q_Definitions_Node_JS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1176,6 +1179,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1185,7 +1189,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1198,6 +1201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1496,8 +1500,8 @@
   <dimension ref="A1:D284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2248,6 +2252,9 @@
       <c r="A112" s="33" t="s">
         <v>172</v>
       </c>
+      <c r="C112" s="47" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="33" t="s">
@@ -2326,11 +2333,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="47" t="s">
+      <c r="A124" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="B124" s="48"/>
-      <c r="C124" s="49"/>
+      <c r="B124" s="49"/>
+      <c r="C124" s="50"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2368,11 +2375,11 @@
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="47" t="s">
+      <c r="A131" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="B131" s="48"/>
-      <c r="C131" s="49"/>
+      <c r="B131" s="49"/>
+      <c r="C131" s="50"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2428,11 +2435,11 @@
       <c r="B138" s="33"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="47" t="s">
+      <c r="A139" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="B139" s="48"/>
-      <c r="C139" s="49"/>
+      <c r="B139" s="49"/>
+      <c r="C139" s="50"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="33" t="s">
@@ -2477,11 +2484,11 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="47" t="s">
+      <c r="A145" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="B145" s="48"/>
-      <c r="C145" s="49"/>
+      <c r="B145" s="49"/>
+      <c r="C145" s="50"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="33" t="s">
@@ -2520,11 +2527,11 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="47" t="s">
+      <c r="A153" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="B153" s="48"/>
-      <c r="C153" s="49"/>
+      <c r="B153" s="49"/>
+      <c r="C153" s="50"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="33" t="s">
@@ -2577,11 +2584,11 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="47" t="s">
+      <c r="A163" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="48"/>
-      <c r="C163" s="49"/>
+      <c r="B163" s="49"/>
+      <c r="C163" s="50"/>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="33" t="s">
@@ -2598,14 +2605,14 @@
       <c r="B165" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C165" s="50"/>
+      <c r="C165" s="55"/>
     </row>
     <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A166" s="33"/>
       <c r="B166" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C166" s="50"/>
+      <c r="C166" s="55"/>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="42" t="s">
@@ -2614,11 +2621,11 @@
     </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="47" t="s">
+      <c r="A170" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="B170" s="48"/>
-      <c r="C170" s="49"/>
+      <c r="B170" s="49"/>
+      <c r="C170" s="50"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="33" t="s">
@@ -2653,11 +2660,11 @@
       <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="47" t="s">
+      <c r="A178" s="48" t="s">
         <v>277</v>
       </c>
-      <c r="B178" s="48"/>
-      <c r="C178" s="49"/>
+      <c r="B178" s="49"/>
+      <c r="C178" s="50"/>
     </row>
     <row r="179" spans="1:3" s="37" customFormat="1">
       <c r="A179" s="36" t="s">
@@ -2682,11 +2689,11 @@
       <c r="B182" s="36"/>
     </row>
     <row r="183" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="47" t="s">
+      <c r="A183" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="B183" s="48"/>
-      <c r="C183" s="49"/>
+      <c r="B183" s="49"/>
+      <c r="C183" s="50"/>
     </row>
     <row r="184" spans="1:3" s="37" customFormat="1">
       <c r="A184" s="36" t="s">
@@ -2711,11 +2718,11 @@
       <c r="B187" s="36"/>
     </row>
     <row r="188" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="47" t="s">
+      <c r="A188" s="48" t="s">
         <v>282</v>
       </c>
-      <c r="B188" s="48"/>
-      <c r="C188" s="49"/>
+      <c r="B188" s="49"/>
+      <c r="C188" s="50"/>
     </row>
     <row r="189" spans="1:3" s="37" customFormat="1">
       <c r="A189" s="36" t="s">
@@ -2732,11 +2739,11 @@
       <c r="B191" s="36"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="47" t="s">
+      <c r="A192" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="B192" s="48"/>
-      <c r="C192" s="49"/>
+      <c r="B192" s="49"/>
+      <c r="C192" s="50"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="33" t="s">
@@ -2752,11 +2759,11 @@
     </row>
     <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="47" t="s">
+      <c r="A197" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="B197" s="48"/>
-      <c r="C197" s="49"/>
+      <c r="B197" s="49"/>
+      <c r="C197" s="50"/>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="33" t="s">
@@ -2782,11 +2789,11 @@
       <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A202" s="47" t="s">
+      <c r="A202" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="B202" s="48"/>
-      <c r="C202" s="49"/>
+      <c r="B202" s="49"/>
+      <c r="C202" s="50"/>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="33" t="s">
@@ -2811,22 +2818,22 @@
       <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A207" s="47" t="s">
+      <c r="A207" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="B207" s="48"/>
-      <c r="C207" s="49"/>
+      <c r="B207" s="49"/>
+      <c r="C207" s="50"/>
     </row>
     <row r="208" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
       <c r="A208" s="35"/>
       <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A209" s="47" t="s">
+      <c r="A209" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="B209" s="48"/>
-      <c r="C209" s="49"/>
+      <c r="B209" s="49"/>
+      <c r="C209" s="50"/>
     </row>
     <row r="210" spans="1:3" s="25" customFormat="1">
       <c r="A210" s="33" t="s">
@@ -2863,11 +2870,11 @@
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="217" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A217" s="47" t="s">
+      <c r="A217" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="B217" s="48"/>
-      <c r="C217" s="49"/>
+      <c r="B217" s="49"/>
+      <c r="C217" s="50"/>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="33" t="s">
@@ -2883,11 +2890,11 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="47" t="s">
+      <c r="A220" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="B220" s="48"/>
-      <c r="C220" s="49"/>
+      <c r="B220" s="49"/>
+      <c r="C220" s="50"/>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="33" t="s">
@@ -2901,11 +2908,11 @@
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="225" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A225" s="47" t="s">
+      <c r="A225" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="B225" s="48"/>
-      <c r="C225" s="49"/>
+      <c r="B225" s="49"/>
+      <c r="C225" s="50"/>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="33" t="s">
@@ -2924,11 +2931,11 @@
     </row>
     <row r="230" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A231" s="47" t="s">
+      <c r="A231" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="B231" s="48"/>
-      <c r="C231" s="49"/>
+      <c r="B231" s="49"/>
+      <c r="C231" s="50"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="33" t="s">
@@ -2961,11 +2968,11 @@
       </c>
     </row>
     <row r="237" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A237" s="47" t="s">
+      <c r="A237" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="B237" s="48"/>
-      <c r="C237" s="49"/>
+      <c r="B237" s="49"/>
+      <c r="C237" s="50"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="33" t="s">
@@ -2980,11 +2987,11 @@
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="47" t="s">
+      <c r="A241" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="B241" s="48"/>
-      <c r="C241" s="49"/>
+      <c r="B241" s="49"/>
+      <c r="C241" s="50"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
@@ -3016,11 +3023,11 @@
     </row>
     <row r="246" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A247" s="47" t="s">
+      <c r="A247" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="B247" s="48"/>
-      <c r="C247" s="49"/>
+      <c r="B247" s="49"/>
+      <c r="C247" s="50"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="33" t="s">
@@ -3033,11 +3040,11 @@
       </c>
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="47" t="s">
+      <c r="A250" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="B250" s="48"/>
-      <c r="C250" s="49"/>
+      <c r="B250" s="49"/>
+      <c r="C250" s="50"/>
     </row>
     <row r="251" spans="1:3" ht="30">
       <c r="A251" s="33" t="s">
@@ -3059,11 +3066,11 @@
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="255" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A255" s="47" t="s">
+      <c r="A255" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="B255" s="48"/>
-      <c r="C255" s="49"/>
+      <c r="B255" s="49"/>
+      <c r="C255" s="50"/>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="33" t="s">
@@ -3075,11 +3082,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="47" t="s">
+      <c r="A259" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B259" s="48"/>
-      <c r="C259" s="49"/>
+      <c r="B259" s="49"/>
+      <c r="C259" s="50"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="51" t="s">
@@ -3100,11 +3107,11 @@
     </row>
     <row r="262" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="263" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A263" s="47" t="s">
+      <c r="A263" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="B263" s="48"/>
-      <c r="C263" s="49"/>
+      <c r="B263" s="49"/>
+      <c r="C263" s="50"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="33" t="s">
@@ -3138,11 +3145,11 @@
     </row>
     <row r="270" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="271" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A271" s="47" t="s">
+      <c r="A271" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="B271" s="48"/>
-      <c r="C271" s="49"/>
+      <c r="B271" s="49"/>
+      <c r="C271" s="50"/>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="40" t="s">
@@ -3159,11 +3166,11 @@
     </row>
     <row r="274" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="275" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A275" s="47" t="s">
+      <c r="A275" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="B275" s="48"/>
-      <c r="C275" s="49"/>
+      <c r="B275" s="49"/>
+      <c r="C275" s="50"/>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="44" t="s">
@@ -3197,11 +3204,11 @@
     </row>
     <row r="282" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="283" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A283" s="47" t="s">
+      <c r="A283" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="B283" s="48"/>
-      <c r="C283" s="49"/>
+      <c r="B283" s="49"/>
+      <c r="C283" s="50"/>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="45" t="s">
@@ -3210,11 +3217,14 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A263:C263"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="C165:C166"/>
     <mergeCell ref="A283:C283"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A260:A261"/>
@@ -3228,17 +3238,14 @@
     <mergeCell ref="A231:C231"/>
     <mergeCell ref="A237:C237"/>
     <mergeCell ref="A241:C241"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
     <mergeCell ref="A259:C259"/>
     <mergeCell ref="A255:C255"/>
     <mergeCell ref="A250:C250"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A263:C263"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A188:C188"/>
     <mergeCell ref="A271:C271"/>
     <mergeCell ref="A192:C192"/>
     <mergeCell ref="A247:C247"/>

</xml_diff>

<commit_message>
Todo, Angular JS, Redis, Hygieia, Node JS, Core Java Collections
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -1533,8 +1533,8 @@
   <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C294" sqref="C294"/>
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A289" sqref="A289:C289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3304,13 +3304,16 @@
     <mergeCell ref="A289:C289"/>
     <mergeCell ref="A278:C278"/>
     <mergeCell ref="A266:C266"/>
+    <mergeCell ref="A286:C286"/>
+    <mergeCell ref="A223:C223"/>
+    <mergeCell ref="A228:C228"/>
+    <mergeCell ref="A234:C234"/>
     <mergeCell ref="A178:C178"/>
     <mergeCell ref="A183:C183"/>
     <mergeCell ref="A188:C188"/>
     <mergeCell ref="A274:C274"/>
     <mergeCell ref="A192:C192"/>
     <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A286:C286"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A263:A264"/>
     <mergeCell ref="B247:C247"/>
@@ -3320,6 +3323,7 @@
     <mergeCell ref="A262:C262"/>
     <mergeCell ref="A258:C258"/>
     <mergeCell ref="A253:C253"/>
+    <mergeCell ref="A220:C220"/>
     <mergeCell ref="A124:C124"/>
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="A170:C170"/>
@@ -3328,10 +3332,6 @@
     <mergeCell ref="A153:C153"/>
     <mergeCell ref="A163:C163"/>
     <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A220:C220"/>
-    <mergeCell ref="A223:C223"/>
-    <mergeCell ref="A228:C228"/>
-    <mergeCell ref="A234:C234"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
Restructured, Eclipselink material added
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -10,14 +10,14 @@
     <sheet name="All Topics" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="A">'All Topics'!$A$245</definedName>
+    <definedName name="A">'All Topics'!$A$246</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="314">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -694,9 +694,6 @@
     <t>JVM and JDK Tools - c_Definitions_JVM.xlsx</t>
   </si>
   <si>
-    <t>Docker Hub</t>
-  </si>
-  <si>
     <t>APIGEE</t>
   </si>
   <si>
@@ -965,6 +962,15 @@
   </si>
   <si>
     <t>t-Definitions-UI.xlsx</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>ORM - u-Definitions-ORM.xlsx</t>
+  </si>
+  <si>
+    <t>Eclipselink</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1227,6 +1233,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1236,6 +1249,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1248,7 +1262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1544,11 +1557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D297"/>
+  <dimension ref="A1:D303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C262" sqref="C262"/>
+      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,11 +1807,6 @@
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="33" t="s">
-        <v>221</v>
-      </c>
-    </row>
     <row r="31" spans="1:3">
       <c r="A31" s="33" t="s">
         <v>51</v>
@@ -2114,7 +2122,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2161,7 +2169,7 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1">
@@ -2175,7 +2183,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2217,7 +2225,7 @@
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2289,10 +2297,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C111" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2300,7 +2308,7 @@
         <v>172</v>
       </c>
       <c r="C112" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2380,11 +2388,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="59" t="s">
+      <c r="A124" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="B124" s="60"/>
-      <c r="C124" s="61"/>
+      <c r="B124" s="63"/>
+      <c r="C124" s="64"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2412,21 +2420,21 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="29" customFormat="1" ht="15.75" thickBot="1">
       <c r="A130" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="59" t="s">
+      <c r="A131" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="B131" s="60"/>
-      <c r="C131" s="61"/>
+      <c r="B131" s="63"/>
+      <c r="C131" s="64"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2453,7 +2461,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>132</v>
@@ -2461,7 +2469,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>132</v>
@@ -2469,525 +2477,518 @@
     </row>
     <row r="137" spans="1:3" s="28" customFormat="1">
       <c r="A137" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="32" customFormat="1" ht="15.75" thickBot="1">
+    <row r="138" spans="1:3" s="32" customFormat="1">
       <c r="A138" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B138" s="33"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A139" s="59" t="s">
+    <row r="139" spans="1:3" s="59" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A139" s="60" t="s">
+        <v>311</v>
+      </c>
+      <c r="B139" s="60"/>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A140" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="B139" s="60"/>
-      <c r="C139" s="61"/>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C140" s="19" t="s">
-        <v>194</v>
-      </c>
+      <c r="B140" s="63"/>
+      <c r="C140" s="64"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B141" s="2"/>
+        <v>22</v>
+      </c>
       <c r="C141" s="19" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="C142" s="22" t="s">
-        <v>206</v>
+        <v>52</v>
+      </c>
+      <c r="B142" s="2"/>
+      <c r="C142" s="19" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="C143" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="C144" s="32" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="1:3" s="39" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A144" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="B144" s="38"/>
-      <c r="C144" s="39" t="s">
+    <row r="145" spans="1:3" s="39" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A145" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="B145" s="38"/>
+      <c r="C145" s="39" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A145" s="59" t="s">
+    <row r="146" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A146" s="62" t="s">
         <v>207</v>
       </c>
-      <c r="B145" s="60"/>
-      <c r="C145" s="61"/>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C146" t="s">
-        <v>168</v>
-      </c>
+      <c r="B146" s="63"/>
+      <c r="C146" s="64"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C147" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C148" t="s">
-        <v>168</v>
-      </c>
-    </row>
     <row r="149" spans="1:3">
       <c r="A149" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="51" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="153" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A153" s="59" t="s">
+    <row r="151" spans="1:3">
+      <c r="A151" s="51" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="154" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A154" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="B153" s="60"/>
-      <c r="C153" s="61"/>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C154" s="22"/>
+      <c r="B154" s="63"/>
+      <c r="C154" s="64"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="33" t="s">
-        <v>141</v>
+        <v>23</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C155" s="22"/>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C156" s="22"/>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="B157" s="2"/>
+        <v>142</v>
+      </c>
       <c r="C157" s="22"/>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="22"/>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="22"/>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="22"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="163" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A163" s="59" t="s">
+    <row r="161" spans="1:3">
+      <c r="A161" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B161" s="2"/>
+      <c r="C161" s="22"/>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="164" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A164" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="60"/>
-      <c r="C163" s="61"/>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="33" t="s">
+      <c r="B164" s="63"/>
+      <c r="C164" s="64"/>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="30">
-      <c r="A165" s="33" t="s">
+    <row r="166" spans="1:3" ht="30">
+      <c r="A166" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B166" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C165" s="66"/>
-    </row>
-    <row r="166" spans="1:3" s="22" customFormat="1" ht="30">
-      <c r="A166" s="33"/>
-      <c r="B166" s="2" t="s">
+      <c r="C166" s="65"/>
+    </row>
+    <row r="167" spans="1:3" s="22" customFormat="1" ht="30">
+      <c r="A167" s="33"/>
+      <c r="B167" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C166" s="66"/>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="42" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="170" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A170" s="59" t="s">
+      <c r="C167" s="65"/>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="42" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="171" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A171" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="B170" s="60"/>
-      <c r="C170" s="61"/>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="C171" s="22"/>
+      <c r="B171" s="63"/>
+      <c r="C171" s="64"/>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C172" s="22"/>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="33" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" s="24" customFormat="1">
-      <c r="A173" s="33" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="174" spans="1:3" s="24" customFormat="1">
       <c r="A174" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="B174" s="1"/>
-      <c r="C174" s="22"/>
+        <v>222</v>
+      </c>
     </row>
     <row r="175" spans="1:3" s="24" customFormat="1">
       <c r="A175" s="33" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B175" s="1"/>
-    </row>
-    <row r="177" spans="1:3" s="27" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B177" s="1"/>
-    </row>
-    <row r="178" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A178" s="59" t="s">
-        <v>277</v>
-      </c>
-      <c r="B178" s="60"/>
-      <c r="C178" s="61"/>
-    </row>
-    <row r="179" spans="1:3" s="37" customFormat="1">
-      <c r="A179" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="B179" s="36"/>
+      <c r="C175" s="22"/>
+    </row>
+    <row r="176" spans="1:3" s="24" customFormat="1">
+      <c r="A176" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B176" s="1"/>
+    </row>
+    <row r="178" spans="1:3" s="27" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A179" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="B179" s="63"/>
+      <c r="C179" s="64"/>
     </row>
     <row r="180" spans="1:3" s="37" customFormat="1">
       <c r="A180" s="36" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B180" s="36"/>
     </row>
     <row r="181" spans="1:3" s="37" customFormat="1">
       <c r="A181" s="36" t="s">
-        <v>276</v>
+        <v>200</v>
       </c>
       <c r="B181" s="36"/>
     </row>
-    <row r="182" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A182" s="36"/>
+    <row r="182" spans="1:3" s="37" customFormat="1">
+      <c r="A182" s="36" t="s">
+        <v>275</v>
+      </c>
       <c r="B182" s="36"/>
     </row>
     <row r="183" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A183" s="59" t="s">
-        <v>278</v>
-      </c>
-      <c r="B183" s="60"/>
-      <c r="C183" s="61"/>
-    </row>
-    <row r="184" spans="1:3" s="37" customFormat="1">
-      <c r="A184" s="36" t="s">
-        <v>279</v>
-      </c>
-      <c r="B184" s="36"/>
+      <c r="A183" s="36"/>
+      <c r="B183" s="36"/>
+    </row>
+    <row r="184" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A184" s="62" t="s">
+        <v>277</v>
+      </c>
+      <c r="B184" s="63"/>
+      <c r="C184" s="64"/>
     </row>
     <row r="185" spans="1:3" s="37" customFormat="1">
       <c r="A185" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B185" s="36"/>
+    </row>
+    <row r="186" spans="1:3" s="37" customFormat="1">
+      <c r="A186" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="B186" s="36"/>
+    </row>
+    <row r="187" spans="1:3" s="27" customFormat="1">
+      <c r="A187" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="B185" s="36"/>
-    </row>
-    <row r="186" spans="1:3" s="27" customFormat="1">
-      <c r="A186" s="36" t="s">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A188" s="36"/>
+      <c r="B188" s="36"/>
+    </row>
+    <row r="189" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A189" s="62" t="s">
         <v>281</v>
       </c>
-      <c r="B186" s="1"/>
-    </row>
-    <row r="187" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A187" s="36"/>
-      <c r="B187" s="36"/>
-    </row>
-    <row r="188" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A188" s="59" t="s">
+      <c r="B189" s="63"/>
+      <c r="C189" s="64"/>
+    </row>
+    <row r="190" spans="1:3" s="37" customFormat="1">
+      <c r="A190" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="B188" s="60"/>
-      <c r="C188" s="61"/>
-    </row>
-    <row r="189" spans="1:3" s="37" customFormat="1">
-      <c r="A189" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="B189" s="36"/>
-    </row>
-    <row r="190" spans="1:3" s="37" customFormat="1">
-      <c r="A190" s="36"/>
       <c r="B190" s="36"/>
     </row>
-    <row r="191" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+    <row r="191" spans="1:3" s="37" customFormat="1">
       <c r="A191" s="36"/>
       <c r="B191" s="36"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A192" s="59" t="s">
+    <row r="192" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A192" s="36"/>
+      <c r="B192" s="36"/>
+    </row>
+    <row r="193" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A193" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="B192" s="60"/>
-      <c r="C192" s="61"/>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C193" s="22"/>
+      <c r="B193" s="63"/>
+      <c r="C193" s="64"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C194" s="22"/>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="C194" s="20"/>
-    </row>
-    <row r="196" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="197" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A197" s="59" t="s">
+      <c r="C195" s="20"/>
+    </row>
+    <row r="197" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="198" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A198" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="B197" s="60"/>
-      <c r="C197" s="61"/>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="B198" s="2"/>
+      <c r="B198" s="63"/>
+      <c r="C198" s="64"/>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="33" t="s">
-        <v>38</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="B199" s="2"/>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="B200" s="2"/>
-    </row>
-    <row r="201" spans="1:3" s="32" customFormat="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
       <c r="A201" s="33" t="s">
         <v>272</v>
       </c>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" spans="1:3" s="52" customFormat="1">
-      <c r="A202" s="53" t="s">
-        <v>306</v>
+    <row r="202" spans="1:3" s="32" customFormat="1">
+      <c r="A202" s="33" t="s">
+        <v>271</v>
       </c>
       <c r="B202" s="2"/>
     </row>
     <row r="203" spans="1:3" s="52" customFormat="1">
-      <c r="A203" s="53"/>
+      <c r="A203" s="53" t="s">
+        <v>305</v>
+      </c>
       <c r="B203" s="2"/>
     </row>
-    <row r="204" spans="1:3" s="52" customFormat="1" ht="15.75" thickBot="1">
+    <row r="204" spans="1:3" s="52" customFormat="1">
       <c r="A204" s="53"/>
       <c r="B204" s="2"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A205" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="B205" s="60"/>
-      <c r="C205" s="61"/>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" s="33" t="s">
+    <row r="205" spans="1:3" s="52" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A205" s="53"/>
+      <c r="B205" s="2"/>
+    </row>
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A206" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="B206" s="63"/>
+      <c r="C206" s="64"/>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="C206" s="10"/>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="A207" s="35" t="s">
-        <v>219</v>
-      </c>
+      <c r="C207" s="10"/>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="35" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A209" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="B209" s="1"/>
-    </row>
     <row r="210" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A210" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="B210" s="60"/>
-      <c r="C210" s="61"/>
+      <c r="A210" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A211" s="35"/>
-      <c r="B211" s="1"/>
-    </row>
-    <row r="212" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A212" s="59" t="s">
-        <v>233</v>
-      </c>
-      <c r="B212" s="60"/>
-      <c r="C212" s="61"/>
-    </row>
-    <row r="213" spans="1:3" s="25" customFormat="1">
-      <c r="A213" s="33" t="s">
+      <c r="A211" s="62" t="s">
+        <v>224</v>
+      </c>
+      <c r="B211" s="63"/>
+      <c r="C211" s="64"/>
+    </row>
+    <row r="212" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A212" s="35"/>
+      <c r="B212" s="1"/>
+    </row>
+    <row r="213" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A213" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="B213" s="63"/>
+      <c r="C213" s="64"/>
+    </row>
+    <row r="214" spans="1:3" s="25" customFormat="1">
+      <c r="A214" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B214" s="26" t="s">
         <v>231</v>
-      </c>
-      <c r="B213" s="26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="A214" s="33" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="33" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="220" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A220" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="B220" s="60"/>
-      <c r="C220" s="61"/>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" s="33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="33" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="221" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A221" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B221" s="63"/>
+      <c r="C221" s="64"/>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B221" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A222" s="33" t="s">
-        <v>253</v>
-      </c>
     </row>
     <row r="223" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A223" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="B223" s="60"/>
-      <c r="C223" s="61"/>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="33" t="s">
-        <v>239</v>
-      </c>
+      <c r="A223" s="33" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A224" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="B224" s="63"/>
+      <c r="C224" s="64"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="33" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="228" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A228" s="59" t="s">
-        <v>243</v>
-      </c>
-      <c r="B228" s="60"/>
-      <c r="C228" s="61"/>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="33" t="s">
-        <v>211</v>
-      </c>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="229" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A229" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="B229" s="63"/>
+      <c r="C229" s="64"/>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="33" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -2995,376 +2996,400 @@
         <v>241</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A234" s="59" t="s">
-        <v>244</v>
-      </c>
-      <c r="B234" s="60"/>
-      <c r="C234" s="61"/>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C235" s="15"/>
+    <row r="232" spans="1:3">
+      <c r="A232" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A235" s="62" t="s">
+        <v>243</v>
+      </c>
+      <c r="B235" s="63"/>
+      <c r="C235" s="64"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="C236" s="16"/>
+        <v>79</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C236" s="15"/>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="33" t="s">
-        <v>245</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C237" s="16"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="33" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A239" s="43" t="s">
-        <v>292</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="33" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A240" s="59" t="s">
-        <v>275</v>
-      </c>
-      <c r="B240" s="60"/>
-      <c r="C240" s="61"/>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241" s="33" t="s">
-        <v>70</v>
-      </c>
+      <c r="A240" s="43" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A241" s="62" t="s">
+        <v>274</v>
+      </c>
+      <c r="B241" s="63"/>
+      <c r="C241" s="64"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B242" s="2"/>
-    </row>
-    <row r="243" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="244" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A244" s="59" t="s">
-        <v>251</v>
-      </c>
-      <c r="B244" s="60"/>
-      <c r="C244" s="61"/>
-    </row>
-    <row r="245" spans="1:3">
-      <c r="A245" s="33" t="s">
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="245" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A245" s="62" t="s">
         <v>250</v>
       </c>
+      <c r="B245" s="63"/>
+      <c r="C245" s="64"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>1</v>
+        <v>249</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B247" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C247" s="65"/>
+        <v>0</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B248" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C248" s="69"/>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C248" s="13"/>
-    </row>
-    <row r="249" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="250" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A250" s="59" t="s">
-        <v>252</v>
-      </c>
-      <c r="B250" s="60"/>
-      <c r="C250" s="61"/>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251" s="33" t="s">
+      <c r="C249" s="13"/>
+    </row>
+    <row r="250" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="251" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A251" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="B251" s="63"/>
+      <c r="C251" s="64"/>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A253" s="33" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A252" s="33" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A253" s="59" t="s">
-        <v>262</v>
-      </c>
-      <c r="B253" s="60"/>
-      <c r="C253" s="61"/>
-    </row>
-    <row r="254" spans="1:3" ht="30">
-      <c r="A254" s="33" t="s">
+    <row r="254" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A254" s="62" t="s">
+        <v>261</v>
+      </c>
+      <c r="B254" s="63"/>
+      <c r="C254" s="64"/>
+    </row>
+    <row r="255" spans="1:3" ht="30">
+      <c r="A255" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B254" s="2" t="s">
+      <c r="B255" s="2" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" s="33" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="259" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A259" s="62" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="258" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A258" s="59" t="s">
-        <v>261</v>
-      </c>
-      <c r="B258" s="60"/>
-      <c r="C258" s="61"/>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259" s="33" t="s">
+      <c r="B259" s="63"/>
+      <c r="C259" s="64"/>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="C259" s="18" t="s">
+      <c r="C260" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
-      <c r="A260" s="55" t="s">
+    <row r="261" spans="1:3">
+      <c r="A261" s="55" t="s">
+        <v>309</v>
+      </c>
+      <c r="C261" s="56" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C262" s="57" t="s">
         <v>310</v>
       </c>
-      <c r="C260" s="56" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
-      <c r="A261" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C261" s="57" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" s="57" customFormat="1">
-      <c r="A262" s="58"/>
-      <c r="B262" s="58"/>
     </row>
     <row r="263" spans="1:3" s="57" customFormat="1">
       <c r="A263" s="58"/>
       <c r="B263" s="58"/>
     </row>
-    <row r="264" spans="1:3" s="57" customFormat="1" ht="15.75" thickBot="1">
+    <row r="264" spans="1:3" s="57" customFormat="1">
       <c r="A264" s="58"/>
       <c r="B264" s="58"/>
     </row>
-    <row r="265" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A265" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B265" s="60"/>
-      <c r="C265" s="61"/>
-    </row>
-    <row r="266" spans="1:3">
+    <row r="265" spans="1:3" s="57" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A265" s="58"/>
+      <c r="B265" s="58"/>
+    </row>
+    <row r="266" spans="1:3" ht="15.75" thickBot="1">
       <c r="A266" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="B266" s="2" t="s">
+      <c r="B266" s="63"/>
+      <c r="C266" s="64"/>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B267" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C267" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
-      <c r="A267" s="63"/>
-      <c r="B267" s="31" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="269" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A269" s="59" t="s">
-        <v>269</v>
-      </c>
-      <c r="B269" s="60"/>
-      <c r="C269" s="61"/>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" s="33" t="s">
-        <v>264</v>
-      </c>
+    <row r="268" spans="1:3">
+      <c r="A268" s="67"/>
+      <c r="B268" s="31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="270" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A270" s="62" t="s">
+        <v>268</v>
+      </c>
+      <c r="B270" s="63"/>
+      <c r="C270" s="64"/>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="33" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="33" t="s">
-        <v>138</v>
+        <v>265</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="33" t="s">
-        <v>267</v>
+        <v>138</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="33" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="277" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A277" s="59" t="s">
-        <v>291</v>
-      </c>
-      <c r="B277" s="60"/>
-      <c r="C277" s="61"/>
-    </row>
-    <row r="278" spans="1:3">
-      <c r="A278" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="33" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="278" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A278" s="62" t="s">
+        <v>290</v>
+      </c>
+      <c r="B278" s="63"/>
+      <c r="C278" s="64"/>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B279" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B278" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
-      <c r="A279" s="42" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="281" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A281" s="59" t="s">
-        <v>293</v>
-      </c>
-      <c r="B281" s="60"/>
-      <c r="C281" s="61"/>
-    </row>
-    <row r="282" spans="1:3">
-      <c r="A282" s="44" t="s">
-        <v>294</v>
-      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="282" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A282" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="B282" s="63"/>
+      <c r="C282" s="64"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="44" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="44" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="44" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="44" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="290" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A290" s="62" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="289" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A289" s="59" t="s">
+      <c r="B290" s="63"/>
+      <c r="C290" s="64"/>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="B289" s="60"/>
-      <c r="C289" s="61"/>
-    </row>
-    <row r="290" spans="1:3">
-      <c r="A290" s="45" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="292" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A292" s="59" t="s">
-        <v>309</v>
-      </c>
-      <c r="B292" s="60"/>
-      <c r="C292" s="61"/>
-    </row>
-    <row r="295" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="296" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A296" s="59" t="s">
+    </row>
+    <row r="292" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="293" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A293" s="62" t="s">
         <v>308</v>
       </c>
-      <c r="B296" s="60"/>
-      <c r="C296" s="61"/>
-    </row>
-    <row r="297" spans="1:3">
-      <c r="A297" s="54" t="s">
+      <c r="B293" s="63"/>
+      <c r="C293" s="64"/>
+    </row>
+    <row r="296" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="297" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A297" s="62" t="s">
         <v>307</v>
       </c>
+      <c r="B297" s="63"/>
+      <c r="C297" s="64"/>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="54" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="301" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A301" s="62" t="s">
+        <v>312</v>
+      </c>
+      <c r="B301" s="63"/>
+      <c r="C301" s="64"/>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" s="61" t="s">
+        <v>313</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="A301:C301"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A297:C297"/>
+    <mergeCell ref="A241:C241"/>
+    <mergeCell ref="A293:C293"/>
+    <mergeCell ref="A282:C282"/>
+    <mergeCell ref="A270:C270"/>
+    <mergeCell ref="A290:C290"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A229:C229"/>
+    <mergeCell ref="A235:C235"/>
+    <mergeCell ref="A179:C179"/>
+    <mergeCell ref="A184:C184"/>
+    <mergeCell ref="A189:C189"/>
+    <mergeCell ref="A278:C278"/>
+    <mergeCell ref="A193:C193"/>
+    <mergeCell ref="A251:C251"/>
+    <mergeCell ref="A198:C198"/>
+    <mergeCell ref="A267:A268"/>
+    <mergeCell ref="B248:C248"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A266:C266"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A254:C254"/>
+    <mergeCell ref="A221:C221"/>
     <mergeCell ref="A124:C124"/>
     <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A170:C170"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="A277:C277"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A250:C250"/>
-    <mergeCell ref="A197:C197"/>
-    <mergeCell ref="A266:A267"/>
-    <mergeCell ref="B247:C247"/>
-    <mergeCell ref="A205:C205"/>
-    <mergeCell ref="A210:C210"/>
-    <mergeCell ref="A244:C244"/>
-    <mergeCell ref="A265:C265"/>
-    <mergeCell ref="A258:C258"/>
-    <mergeCell ref="A253:C253"/>
-    <mergeCell ref="A220:C220"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A240:C240"/>
-    <mergeCell ref="A292:C292"/>
-    <mergeCell ref="A281:C281"/>
-    <mergeCell ref="A269:C269"/>
-    <mergeCell ref="A289:C289"/>
-    <mergeCell ref="A223:C223"/>
-    <mergeCell ref="A228:C228"/>
-    <mergeCell ref="A234:C234"/>
+    <mergeCell ref="A171:C171"/>
+    <mergeCell ref="A140:C140"/>
+    <mergeCell ref="A146:C146"/>
+    <mergeCell ref="A154:C154"/>
+    <mergeCell ref="A164:C164"/>
+    <mergeCell ref="C166:C167"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
@@ -3376,20 +3401,20 @@
     <hyperlink ref="B77" r:id="rId7"/>
     <hyperlink ref="B53" r:id="rId8"/>
     <hyperlink ref="B63" r:id="rId9"/>
-    <hyperlink ref="B235" r:id="rId10"/>
-    <hyperlink ref="B149" r:id="rId11"/>
+    <hyperlink ref="B236" r:id="rId10"/>
+    <hyperlink ref="B150" r:id="rId11"/>
     <hyperlink ref="B45" r:id="rId12"/>
     <hyperlink ref="B78" r:id="rId13"/>
     <hyperlink ref="B72" r:id="rId14"/>
     <hyperlink ref="B66" r:id="rId15"/>
-    <hyperlink ref="B266" r:id="rId16"/>
+    <hyperlink ref="B267" r:id="rId16"/>
     <hyperlink ref="B42" r:id="rId17" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
     <hyperlink ref="B41" r:id="rId18"/>
     <hyperlink ref="B94" r:id="rId19"/>
     <hyperlink ref="B95" r:id="rId20"/>
     <hyperlink ref="B35" r:id="rId21"/>
-    <hyperlink ref="B141" r:id="rId22" display="http://www.tutorialspoint.com/restful/index.htm"/>
-    <hyperlink ref="B254" r:id="rId23"/>
+    <hyperlink ref="B142" r:id="rId22" display="http://www.tutorialspoint.com/restful/index.htm"/>
+    <hyperlink ref="B255" r:id="rId23"/>
     <hyperlink ref="B62" r:id="rId24"/>
     <hyperlink ref="B107" r:id="rId25"/>
     <hyperlink ref="B108" r:id="rId26" location="commandLine"/>
@@ -3398,9 +3423,9 @@
     <hyperlink ref="B133" r:id="rId29"/>
     <hyperlink ref="B119" r:id="rId30"/>
     <hyperlink ref="D1" location="'All Topics'!A2" display="Up"/>
-    <hyperlink ref="B166" r:id="rId31"/>
-    <hyperlink ref="B213" r:id="rId32"/>
-    <hyperlink ref="B278" r:id="rId33"/>
+    <hyperlink ref="B167" r:id="rId31"/>
+    <hyperlink ref="B214" r:id="rId32"/>
+    <hyperlink ref="B279" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>

</xml_diff>

<commit_message>
github, active mq, yaml, cassandra, camel
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="334">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -1025,6 +1025,12 @@
   </si>
   <si>
     <t>Machine Learning - x-Defnitions-machine-learning.xlsx</t>
+  </si>
+  <si>
+    <t>SourceTree</t>
+  </si>
+  <si>
+    <t>Git Extensions</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1317,6 +1323,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1634,11 +1644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D325"/>
+  <dimension ref="A1:D326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A325" sqref="A325:C325"/>
+      <pane ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2452,11 +2462,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="71" t="s">
+      <c r="A124" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="72"/>
-      <c r="C124" s="73"/>
+      <c r="B124" s="74"/>
+      <c r="C124" s="75"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2494,11 +2504,11 @@
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="71" t="s">
+      <c r="A131" s="73" t="s">
         <v>215</v>
       </c>
-      <c r="B131" s="72"/>
-      <c r="C131" s="73"/>
+      <c r="B131" s="74"/>
+      <c r="C131" s="75"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2560,11 +2570,11 @@
       <c r="B139" s="60"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A140" s="71" t="s">
+      <c r="A140" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="B140" s="72"/>
-      <c r="C140" s="73"/>
+      <c r="B140" s="74"/>
+      <c r="C140" s="75"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="33" t="s">
@@ -2609,11 +2619,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A146" s="71" t="s">
+      <c r="A146" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="B146" s="72"/>
-      <c r="C146" s="73"/>
+      <c r="B146" s="74"/>
+      <c r="C146" s="75"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="33" t="s">
@@ -2625,11 +2635,11 @@
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="154" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A154" s="71" t="s">
+      <c r="A154" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="B154" s="72"/>
-      <c r="C154" s="73"/>
+      <c r="B154" s="74"/>
+      <c r="C154" s="75"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="33" t="s">
@@ -2682,11 +2692,11 @@
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="164" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A164" s="71" t="s">
+      <c r="A164" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="72"/>
-      <c r="C164" s="73"/>
+      <c r="B164" s="74"/>
+      <c r="C164" s="75"/>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="33" t="s">
@@ -2703,14 +2713,14 @@
       <c r="B166" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C166" s="74"/>
+      <c r="C166" s="76"/>
     </row>
     <row r="167" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C167" s="74"/>
+      <c r="C167" s="76"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="42" t="s">
@@ -2719,11 +2729,11 @@
     </row>
     <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="171" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A171" s="71" t="s">
+      <c r="A171" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="B171" s="72"/>
-      <c r="C171" s="73"/>
+      <c r="B171" s="74"/>
+      <c r="C171" s="75"/>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="33" t="s">
@@ -2758,11 +2768,11 @@
       <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A179" s="71" t="s">
+      <c r="A179" s="73" t="s">
         <v>275</v>
       </c>
-      <c r="B179" s="72"/>
-      <c r="C179" s="73"/>
+      <c r="B179" s="74"/>
+      <c r="C179" s="75"/>
     </row>
     <row r="180" spans="1:3" s="37" customFormat="1">
       <c r="A180" s="36" t="s">
@@ -2787,11 +2797,11 @@
       <c r="B183" s="36"/>
     </row>
     <row r="184" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A184" s="71" t="s">
+      <c r="A184" s="73" t="s">
         <v>276</v>
       </c>
-      <c r="B184" s="72"/>
-      <c r="C184" s="73"/>
+      <c r="B184" s="74"/>
+      <c r="C184" s="75"/>
     </row>
     <row r="185" spans="1:3" s="37" customFormat="1">
       <c r="A185" s="36" t="s">
@@ -2816,11 +2826,11 @@
       <c r="B188" s="36"/>
     </row>
     <row r="189" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A189" s="71" t="s">
+      <c r="A189" s="73" t="s">
         <v>280</v>
       </c>
-      <c r="B189" s="72"/>
-      <c r="C189" s="73"/>
+      <c r="B189" s="74"/>
+      <c r="C189" s="75"/>
     </row>
     <row r="190" spans="1:3" s="37" customFormat="1">
       <c r="A190" s="36" t="s">
@@ -2837,11 +2847,11 @@
       <c r="B192" s="36"/>
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A193" s="71" t="s">
+      <c r="A193" s="73" t="s">
         <v>212</v>
       </c>
-      <c r="B193" s="72"/>
-      <c r="C193" s="73"/>
+      <c r="B193" s="74"/>
+      <c r="C193" s="75"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="33" t="s">
@@ -2857,11 +2867,11 @@
     </row>
     <row r="197" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="198" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A198" s="71" t="s">
+      <c r="A198" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="B198" s="72"/>
-      <c r="C198" s="73"/>
+      <c r="B198" s="74"/>
+      <c r="C198" s="75"/>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="33" t="s">
@@ -2901,11 +2911,11 @@
       <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A206" s="71" t="s">
+      <c r="A206" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="B206" s="72"/>
-      <c r="C206" s="73"/>
+      <c r="B206" s="74"/>
+      <c r="C206" s="75"/>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="33" t="s">
@@ -2930,22 +2940,22 @@
       <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A211" s="71" t="s">
+      <c r="A211" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="B211" s="72"/>
-      <c r="C211" s="73"/>
+      <c r="B211" s="74"/>
+      <c r="C211" s="75"/>
     </row>
     <row r="212" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
       <c r="A212" s="35"/>
       <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A213" s="71" t="s">
+      <c r="A213" s="73" t="s">
         <v>231</v>
       </c>
-      <c r="B213" s="72"/>
-      <c r="C213" s="73"/>
+      <c r="B213" s="74"/>
+      <c r="C213" s="75"/>
     </row>
     <row r="214" spans="1:3" s="25" customFormat="1">
       <c r="A214" s="33" t="s">
@@ -2982,11 +2992,11 @@
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="71" t="s">
+      <c r="A221" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="B221" s="72"/>
-      <c r="C221" s="73"/>
+      <c r="B221" s="74"/>
+      <c r="C221" s="75"/>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="33" t="s">
@@ -3002,11 +3012,11 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A224" s="71" t="s">
+      <c r="A224" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="B224" s="72"/>
-      <c r="C224" s="73"/>
+      <c r="B224" s="74"/>
+      <c r="C224" s="75"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="33" t="s">
@@ -3020,11 +3030,11 @@
     </row>
     <row r="228" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="229" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A229" s="71" t="s">
+      <c r="A229" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="B229" s="72"/>
-      <c r="C229" s="73"/>
+      <c r="B229" s="74"/>
+      <c r="C229" s="75"/>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="33" t="s">
@@ -3043,11 +3053,11 @@
     </row>
     <row r="234" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="235" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A235" s="71" t="s">
+      <c r="A235" s="73" t="s">
         <v>242</v>
       </c>
-      <c r="B235" s="72"/>
-      <c r="C235" s="73"/>
+      <c r="B235" s="74"/>
+      <c r="C235" s="75"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="33" t="s">
@@ -3080,11 +3090,11 @@
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="71" t="s">
+      <c r="A241" s="73" t="s">
         <v>273</v>
       </c>
-      <c r="B241" s="72"/>
-      <c r="C241" s="73"/>
+      <c r="B241" s="74"/>
+      <c r="C241" s="75"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
@@ -3099,11 +3109,11 @@
     </row>
     <row r="244" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="245" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A245" s="71" t="s">
+      <c r="A245" s="73" t="s">
         <v>249</v>
       </c>
-      <c r="B245" s="72"/>
-      <c r="C245" s="73"/>
+      <c r="B245" s="74"/>
+      <c r="C245" s="75"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="33" t="s">
@@ -3122,10 +3132,10 @@
       <c r="A248" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B248" s="77" t="s">
+      <c r="B248" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C248" s="78"/>
+      <c r="C248" s="80"/>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="33" t="s">
@@ -3135,11 +3145,11 @@
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="251" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A251" s="71" t="s">
+      <c r="A251" s="73" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="72"/>
-      <c r="C251" s="73"/>
+      <c r="B251" s="74"/>
+      <c r="C251" s="75"/>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="33" t="s">
@@ -3152,11 +3162,11 @@
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A254" s="71" t="s">
+      <c r="A254" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="B254" s="72"/>
-      <c r="C254" s="73"/>
+      <c r="B254" s="74"/>
+      <c r="C254" s="75"/>
     </row>
     <row r="255" spans="1:3" ht="30">
       <c r="A255" s="33" t="s">
@@ -3178,11 +3188,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="71" t="s">
+      <c r="A259" s="73" t="s">
         <v>259</v>
       </c>
-      <c r="B259" s="72"/>
-      <c r="C259" s="73"/>
+      <c r="B259" s="74"/>
+      <c r="C259" s="75"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="33" t="s">
@@ -3221,14 +3231,14 @@
       <c r="B265" s="58"/>
     </row>
     <row r="266" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A266" s="71" t="s">
+      <c r="A266" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B266" s="72"/>
-      <c r="C266" s="73"/>
+      <c r="B266" s="74"/>
+      <c r="C266" s="75"/>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" s="75" t="s">
+      <c r="A267" s="77" t="s">
         <v>40</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -3239,18 +3249,18 @@
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="76"/>
+      <c r="A268" s="78"/>
       <c r="B268" s="31" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="270" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A270" s="71" t="s">
+      <c r="A270" s="73" t="s">
         <v>267</v>
       </c>
-      <c r="B270" s="72"/>
-      <c r="C270" s="73"/>
+      <c r="B270" s="74"/>
+      <c r="C270" s="75"/>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="33" t="s">
@@ -3284,11 +3294,11 @@
     </row>
     <row r="277" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="278" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A278" s="71" t="s">
+      <c r="A278" s="73" t="s">
         <v>289</v>
       </c>
-      <c r="B278" s="72"/>
-      <c r="C278" s="73"/>
+      <c r="B278" s="74"/>
+      <c r="C278" s="75"/>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="40" t="s">
@@ -3305,11 +3315,11 @@
     </row>
     <row r="281" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A282" s="71" t="s">
+      <c r="A282" s="73" t="s">
         <v>291</v>
       </c>
-      <c r="B282" s="72"/>
-      <c r="C282" s="73"/>
+      <c r="B282" s="74"/>
+      <c r="C282" s="75"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="44" t="s">
@@ -3343,11 +3353,11 @@
     </row>
     <row r="289" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="290" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A290" s="71" t="s">
+      <c r="A290" s="73" t="s">
         <v>298</v>
       </c>
-      <c r="B290" s="72"/>
-      <c r="C290" s="73"/>
+      <c r="B290" s="74"/>
+      <c r="C290" s="75"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="45" t="s">
@@ -3356,11 +3366,11 @@
     </row>
     <row r="292" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="293" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A293" s="71" t="s">
+      <c r="A293" s="73" t="s">
         <v>314</v>
       </c>
-      <c r="B293" s="72"/>
-      <c r="C293" s="73"/>
+      <c r="B293" s="74"/>
+      <c r="C293" s="75"/>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="63" t="s">
@@ -3370,11 +3380,11 @@
     </row>
     <row r="296" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="297" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A297" s="71" t="s">
+      <c r="A297" s="73" t="s">
         <v>306</v>
       </c>
-      <c r="B297" s="72"/>
-      <c r="C297" s="73"/>
+      <c r="B297" s="74"/>
+      <c r="C297" s="75"/>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="54" t="s">
@@ -3383,11 +3393,11 @@
     </row>
     <row r="300" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="301" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A301" s="71" t="s">
+      <c r="A301" s="73" t="s">
         <v>310</v>
       </c>
-      <c r="B301" s="72"/>
-      <c r="C301" s="73"/>
+      <c r="B301" s="74"/>
+      <c r="C301" s="75"/>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="61" t="s">
@@ -3442,11 +3452,11 @@
     </row>
     <row r="311" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="312" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A312" s="71" t="s">
+      <c r="A312" s="73" t="s">
         <v>317</v>
       </c>
-      <c r="B312" s="72"/>
-      <c r="C312" s="73"/>
+      <c r="B312" s="74"/>
+      <c r="C312" s="75"/>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="33" t="s">
@@ -3469,58 +3479,68 @@
         <v>319</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="317" spans="1:3" s="72" customFormat="1">
+      <c r="A317" s="71" t="s">
+        <v>333</v>
+      </c>
+      <c r="B317" s="71"/>
+    </row>
     <row r="318" spans="1:3" ht="15.75" thickBot="1">
       <c r="A318" s="71" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A319" s="73" t="s">
         <v>320</v>
       </c>
-      <c r="B318" s="72"/>
-      <c r="C318" s="73"/>
-    </row>
-    <row r="319" spans="1:3">
-      <c r="A319" s="68" t="s">
-        <v>321</v>
-      </c>
-      <c r="B319" s="68" t="s">
-        <v>322</v>
-      </c>
+      <c r="B319" s="74"/>
+      <c r="C319" s="75"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="68" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B320" s="68" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="68" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B321" s="68" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="B322" s="68" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" s="68" t="s">
         <v>327</v>
       </c>
-      <c r="B322" s="68" t="s">
+      <c r="B323" s="68" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
-      <c r="A323" s="69" t="s">
+    <row r="324" spans="1:3">
+      <c r="A324" s="69" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="325" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A325" s="71" t="s">
+    <row r="325" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="326" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A326" s="73" t="s">
         <v>331</v>
       </c>
-      <c r="B325" s="72"/>
-      <c r="C325" s="73"/>
+      <c r="B326" s="74"/>
+      <c r="C326" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -3546,8 +3566,8 @@
     <mergeCell ref="A259:C259"/>
     <mergeCell ref="A254:C254"/>
     <mergeCell ref="A221:C221"/>
-    <mergeCell ref="A325:C325"/>
-    <mergeCell ref="A318:C318"/>
+    <mergeCell ref="A326:C326"/>
+    <mergeCell ref="A319:C319"/>
     <mergeCell ref="A124:C124"/>
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="A171:C171"/>

</xml_diff>

<commit_message>
Kafka, Spring Integration, ActiveMQ
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="335">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -1031,6 +1031,9 @@
   </si>
   <si>
     <t>Git Extensions</t>
+  </si>
+  <si>
+    <t>Spring Integration</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1327,6 +1330,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1647,8 +1653,8 @@
   <dimension ref="A1:D326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A317" sqref="A317"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2462,11 +2468,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="73" t="s">
+      <c r="A124" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="74"/>
-      <c r="C124" s="75"/>
+      <c r="B124" s="75"/>
+      <c r="C124" s="76"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2504,11 +2510,11 @@
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="73" t="s">
+      <c r="A131" s="74" t="s">
         <v>215</v>
       </c>
-      <c r="B131" s="74"/>
-      <c r="C131" s="75"/>
+      <c r="B131" s="75"/>
+      <c r="C131" s="76"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2570,11 +2576,11 @@
       <c r="B139" s="60"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A140" s="73" t="s">
+      <c r="A140" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="B140" s="74"/>
-      <c r="C140" s="75"/>
+      <c r="B140" s="75"/>
+      <c r="C140" s="76"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="33" t="s">
@@ -2619,11 +2625,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A146" s="73" t="s">
+      <c r="A146" s="74" t="s">
         <v>206</v>
       </c>
-      <c r="B146" s="74"/>
-      <c r="C146" s="75"/>
+      <c r="B146" s="75"/>
+      <c r="C146" s="76"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="33" t="s">
@@ -2635,11 +2641,11 @@
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="154" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A154" s="73" t="s">
+      <c r="A154" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="B154" s="74"/>
-      <c r="C154" s="75"/>
+      <c r="B154" s="75"/>
+      <c r="C154" s="76"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="33" t="s">
@@ -2690,13 +2696,18 @@
       <c r="B161" s="2"/>
       <c r="C161" s="22"/>
     </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="73" t="s">
+        <v>334</v>
+      </c>
+    </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="164" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A164" s="73" t="s">
+      <c r="A164" s="74" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="74"/>
-      <c r="C164" s="75"/>
+      <c r="B164" s="75"/>
+      <c r="C164" s="76"/>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="33" t="s">
@@ -2713,14 +2724,14 @@
       <c r="B166" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C166" s="76"/>
+      <c r="C166" s="77"/>
     </row>
     <row r="167" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C167" s="76"/>
+      <c r="C167" s="77"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="42" t="s">
@@ -2729,11 +2740,11 @@
     </row>
     <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="171" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A171" s="73" t="s">
+      <c r="A171" s="74" t="s">
         <v>211</v>
       </c>
-      <c r="B171" s="74"/>
-      <c r="C171" s="75"/>
+      <c r="B171" s="75"/>
+      <c r="C171" s="76"/>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="33" t="s">
@@ -2768,11 +2779,11 @@
       <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A179" s="73" t="s">
+      <c r="A179" s="74" t="s">
         <v>275</v>
       </c>
-      <c r="B179" s="74"/>
-      <c r="C179" s="75"/>
+      <c r="B179" s="75"/>
+      <c r="C179" s="76"/>
     </row>
     <row r="180" spans="1:3" s="37" customFormat="1">
       <c r="A180" s="36" t="s">
@@ -2797,11 +2808,11 @@
       <c r="B183" s="36"/>
     </row>
     <row r="184" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A184" s="73" t="s">
+      <c r="A184" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="B184" s="74"/>
-      <c r="C184" s="75"/>
+      <c r="B184" s="75"/>
+      <c r="C184" s="76"/>
     </row>
     <row r="185" spans="1:3" s="37" customFormat="1">
       <c r="A185" s="36" t="s">
@@ -2826,11 +2837,11 @@
       <c r="B188" s="36"/>
     </row>
     <row r="189" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A189" s="73" t="s">
+      <c r="A189" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="B189" s="74"/>
-      <c r="C189" s="75"/>
+      <c r="B189" s="75"/>
+      <c r="C189" s="76"/>
     </row>
     <row r="190" spans="1:3" s="37" customFormat="1">
       <c r="A190" s="36" t="s">
@@ -2847,11 +2858,11 @@
       <c r="B192" s="36"/>
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A193" s="73" t="s">
+      <c r="A193" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="B193" s="74"/>
-      <c r="C193" s="75"/>
+      <c r="B193" s="75"/>
+      <c r="C193" s="76"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="33" t="s">
@@ -2867,11 +2878,11 @@
     </row>
     <row r="197" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="198" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A198" s="73" t="s">
+      <c r="A198" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="B198" s="74"/>
-      <c r="C198" s="75"/>
+      <c r="B198" s="75"/>
+      <c r="C198" s="76"/>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="33" t="s">
@@ -2911,11 +2922,11 @@
       <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A206" s="73" t="s">
+      <c r="A206" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="B206" s="74"/>
-      <c r="C206" s="75"/>
+      <c r="B206" s="75"/>
+      <c r="C206" s="76"/>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="33" t="s">
@@ -2940,22 +2951,22 @@
       <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A211" s="73" t="s">
+      <c r="A211" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="B211" s="74"/>
-      <c r="C211" s="75"/>
+      <c r="B211" s="75"/>
+      <c r="C211" s="76"/>
     </row>
     <row r="212" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
       <c r="A212" s="35"/>
       <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A213" s="73" t="s">
+      <c r="A213" s="74" t="s">
         <v>231</v>
       </c>
-      <c r="B213" s="74"/>
-      <c r="C213" s="75"/>
+      <c r="B213" s="75"/>
+      <c r="C213" s="76"/>
     </row>
     <row r="214" spans="1:3" s="25" customFormat="1">
       <c r="A214" s="33" t="s">
@@ -2992,11 +3003,11 @@
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="73" t="s">
+      <c r="A221" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="B221" s="74"/>
-      <c r="C221" s="75"/>
+      <c r="B221" s="75"/>
+      <c r="C221" s="76"/>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="33" t="s">
@@ -3012,11 +3023,11 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A224" s="73" t="s">
+      <c r="A224" s="74" t="s">
         <v>236</v>
       </c>
-      <c r="B224" s="74"/>
-      <c r="C224" s="75"/>
+      <c r="B224" s="75"/>
+      <c r="C224" s="76"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="33" t="s">
@@ -3030,11 +3041,11 @@
     </row>
     <row r="228" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="229" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A229" s="73" t="s">
+      <c r="A229" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="B229" s="74"/>
-      <c r="C229" s="75"/>
+      <c r="B229" s="75"/>
+      <c r="C229" s="76"/>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="33" t="s">
@@ -3053,11 +3064,11 @@
     </row>
     <row r="234" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="235" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A235" s="73" t="s">
+      <c r="A235" s="74" t="s">
         <v>242</v>
       </c>
-      <c r="B235" s="74"/>
-      <c r="C235" s="75"/>
+      <c r="B235" s="75"/>
+      <c r="C235" s="76"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="33" t="s">
@@ -3090,11 +3101,11 @@
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="73" t="s">
+      <c r="A241" s="74" t="s">
         <v>273</v>
       </c>
-      <c r="B241" s="74"/>
-      <c r="C241" s="75"/>
+      <c r="B241" s="75"/>
+      <c r="C241" s="76"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
@@ -3109,11 +3120,11 @@
     </row>
     <row r="244" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="245" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A245" s="73" t="s">
+      <c r="A245" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="B245" s="74"/>
-      <c r="C245" s="75"/>
+      <c r="B245" s="75"/>
+      <c r="C245" s="76"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="33" t="s">
@@ -3132,10 +3143,10 @@
       <c r="A248" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B248" s="79" t="s">
+      <c r="B248" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C248" s="80"/>
+      <c r="C248" s="81"/>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="33" t="s">
@@ -3145,11 +3156,11 @@
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="251" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A251" s="73" t="s">
+      <c r="A251" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="74"/>
-      <c r="C251" s="75"/>
+      <c r="B251" s="75"/>
+      <c r="C251" s="76"/>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="33" t="s">
@@ -3162,11 +3173,11 @@
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A254" s="73" t="s">
+      <c r="A254" s="74" t="s">
         <v>260</v>
       </c>
-      <c r="B254" s="74"/>
-      <c r="C254" s="75"/>
+      <c r="B254" s="75"/>
+      <c r="C254" s="76"/>
     </row>
     <row r="255" spans="1:3" ht="30">
       <c r="A255" s="33" t="s">
@@ -3188,11 +3199,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="73" t="s">
+      <c r="A259" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="B259" s="74"/>
-      <c r="C259" s="75"/>
+      <c r="B259" s="75"/>
+      <c r="C259" s="76"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="33" t="s">
@@ -3231,14 +3242,14 @@
       <c r="B265" s="58"/>
     </row>
     <row r="266" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A266" s="73" t="s">
+      <c r="A266" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="B266" s="74"/>
-      <c r="C266" s="75"/>
+      <c r="B266" s="75"/>
+      <c r="C266" s="76"/>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" s="77" t="s">
+      <c r="A267" s="78" t="s">
         <v>40</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -3249,18 +3260,18 @@
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="78"/>
+      <c r="A268" s="79"/>
       <c r="B268" s="31" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="270" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A270" s="73" t="s">
+      <c r="A270" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="B270" s="74"/>
-      <c r="C270" s="75"/>
+      <c r="B270" s="75"/>
+      <c r="C270" s="76"/>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="33" t="s">
@@ -3294,11 +3305,11 @@
     </row>
     <row r="277" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="278" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A278" s="73" t="s">
+      <c r="A278" s="74" t="s">
         <v>289</v>
       </c>
-      <c r="B278" s="74"/>
-      <c r="C278" s="75"/>
+      <c r="B278" s="75"/>
+      <c r="C278" s="76"/>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="40" t="s">
@@ -3315,11 +3326,11 @@
     </row>
     <row r="281" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A282" s="73" t="s">
+      <c r="A282" s="74" t="s">
         <v>291</v>
       </c>
-      <c r="B282" s="74"/>
-      <c r="C282" s="75"/>
+      <c r="B282" s="75"/>
+      <c r="C282" s="76"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="44" t="s">
@@ -3353,11 +3364,11 @@
     </row>
     <row r="289" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="290" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A290" s="73" t="s">
+      <c r="A290" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="B290" s="74"/>
-      <c r="C290" s="75"/>
+      <c r="B290" s="75"/>
+      <c r="C290" s="76"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="45" t="s">
@@ -3366,11 +3377,11 @@
     </row>
     <row r="292" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="293" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A293" s="73" t="s">
+      <c r="A293" s="74" t="s">
         <v>314</v>
       </c>
-      <c r="B293" s="74"/>
-      <c r="C293" s="75"/>
+      <c r="B293" s="75"/>
+      <c r="C293" s="76"/>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="63" t="s">
@@ -3380,11 +3391,11 @@
     </row>
     <row r="296" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="297" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A297" s="73" t="s">
+      <c r="A297" s="74" t="s">
         <v>306</v>
       </c>
-      <c r="B297" s="74"/>
-      <c r="C297" s="75"/>
+      <c r="B297" s="75"/>
+      <c r="C297" s="76"/>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="54" t="s">
@@ -3393,11 +3404,11 @@
     </row>
     <row r="300" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="301" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A301" s="73" t="s">
+      <c r="A301" s="74" t="s">
         <v>310</v>
       </c>
-      <c r="B301" s="74"/>
-      <c r="C301" s="75"/>
+      <c r="B301" s="75"/>
+      <c r="C301" s="76"/>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="61" t="s">
@@ -3452,11 +3463,11 @@
     </row>
     <row r="311" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="312" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A312" s="73" t="s">
+      <c r="A312" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="B312" s="74"/>
-      <c r="C312" s="75"/>
+      <c r="B312" s="75"/>
+      <c r="C312" s="76"/>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="33" t="s">
@@ -3491,11 +3502,11 @@
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A319" s="73" t="s">
+      <c r="A319" s="74" t="s">
         <v>320</v>
       </c>
-      <c r="B319" s="74"/>
-      <c r="C319" s="75"/>
+      <c r="B319" s="75"/>
+      <c r="C319" s="76"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="68" t="s">
@@ -3536,11 +3547,11 @@
     </row>
     <row r="325" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="326" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A326" s="73" t="s">
+      <c r="A326" s="74" t="s">
         <v>331</v>
       </c>
-      <c r="B326" s="74"/>
-      <c r="C326" s="75"/>
+      <c r="B326" s="75"/>
+      <c r="C326" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="38">

</xml_diff>

<commit_message>
1. Eclipselink 2. ReactJS
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="337">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -1034,6 +1034,12 @@
   </si>
   <si>
     <t>Spring Integration</t>
+  </si>
+  <si>
+    <t>ReactJS/React JS</t>
+  </si>
+  <si>
+    <t>y_Definitions_React_JS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1333,6 +1339,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1342,6 +1352,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1354,7 +1365,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1654,7 +1664,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A260" sqref="A260"/>
+      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2468,11 +2478,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="74" t="s">
+      <c r="A124" s="76" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="75"/>
-      <c r="C124" s="76"/>
+      <c r="B124" s="77"/>
+      <c r="C124" s="78"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2510,11 +2520,11 @@
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="74" t="s">
+      <c r="A131" s="76" t="s">
         <v>215</v>
       </c>
-      <c r="B131" s="75"/>
-      <c r="C131" s="76"/>
+      <c r="B131" s="77"/>
+      <c r="C131" s="78"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2576,11 +2586,11 @@
       <c r="B139" s="60"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A140" s="74" t="s">
+      <c r="A140" s="76" t="s">
         <v>204</v>
       </c>
-      <c r="B140" s="75"/>
-      <c r="C140" s="76"/>
+      <c r="B140" s="77"/>
+      <c r="C140" s="78"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="33" t="s">
@@ -2625,11 +2635,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A146" s="74" t="s">
+      <c r="A146" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B146" s="75"/>
-      <c r="C146" s="76"/>
+      <c r="B146" s="77"/>
+      <c r="C146" s="78"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="33" t="s">
@@ -2641,11 +2651,11 @@
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="154" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A154" s="74" t="s">
+      <c r="A154" s="76" t="s">
         <v>213</v>
       </c>
-      <c r="B154" s="75"/>
-      <c r="C154" s="76"/>
+      <c r="B154" s="77"/>
+      <c r="C154" s="78"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="33" t="s">
@@ -2703,11 +2713,11 @@
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="164" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A164" s="74" t="s">
+      <c r="A164" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="75"/>
-      <c r="C164" s="76"/>
+      <c r="B164" s="77"/>
+      <c r="C164" s="78"/>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="33" t="s">
@@ -2724,14 +2734,14 @@
       <c r="B166" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C166" s="81"/>
+      <c r="C166" s="79"/>
     </row>
     <row r="167" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C167" s="81"/>
+      <c r="C167" s="79"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="42" t="s">
@@ -2740,11 +2750,11 @@
     </row>
     <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="171" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A171" s="74" t="s">
+      <c r="A171" s="76" t="s">
         <v>211</v>
       </c>
-      <c r="B171" s="75"/>
-      <c r="C171" s="76"/>
+      <c r="B171" s="77"/>
+      <c r="C171" s="78"/>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="33" t="s">
@@ -2779,11 +2789,11 @@
       <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A179" s="74" t="s">
+      <c r="A179" s="76" t="s">
         <v>275</v>
       </c>
-      <c r="B179" s="75"/>
-      <c r="C179" s="76"/>
+      <c r="B179" s="77"/>
+      <c r="C179" s="78"/>
     </row>
     <row r="180" spans="1:3" s="37" customFormat="1">
       <c r="A180" s="36" t="s">
@@ -2808,11 +2818,11 @@
       <c r="B183" s="36"/>
     </row>
     <row r="184" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A184" s="74" t="s">
+      <c r="A184" s="76" t="s">
         <v>276</v>
       </c>
-      <c r="B184" s="75"/>
-      <c r="C184" s="76"/>
+      <c r="B184" s="77"/>
+      <c r="C184" s="78"/>
     </row>
     <row r="185" spans="1:3" s="37" customFormat="1">
       <c r="A185" s="36" t="s">
@@ -2837,11 +2847,11 @@
       <c r="B188" s="36"/>
     </row>
     <row r="189" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A189" s="74" t="s">
+      <c r="A189" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="B189" s="75"/>
-      <c r="C189" s="76"/>
+      <c r="B189" s="77"/>
+      <c r="C189" s="78"/>
     </row>
     <row r="190" spans="1:3" s="37" customFormat="1">
       <c r="A190" s="36" t="s">
@@ -2858,11 +2868,11 @@
       <c r="B192" s="36"/>
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A193" s="74" t="s">
+      <c r="A193" s="76" t="s">
         <v>212</v>
       </c>
-      <c r="B193" s="75"/>
-      <c r="C193" s="76"/>
+      <c r="B193" s="77"/>
+      <c r="C193" s="78"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="33" t="s">
@@ -2878,11 +2888,11 @@
     </row>
     <row r="197" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="198" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A198" s="74" t="s">
+      <c r="A198" s="76" t="s">
         <v>219</v>
       </c>
-      <c r="B198" s="75"/>
-      <c r="C198" s="76"/>
+      <c r="B198" s="77"/>
+      <c r="C198" s="78"/>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="33" t="s">
@@ -2922,11 +2932,11 @@
       <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A206" s="74" t="s">
+      <c r="A206" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="B206" s="75"/>
-      <c r="C206" s="76"/>
+      <c r="B206" s="77"/>
+      <c r="C206" s="78"/>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="33" t="s">
@@ -2951,22 +2961,22 @@
       <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A211" s="74" t="s">
+      <c r="A211" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="B211" s="75"/>
-      <c r="C211" s="76"/>
+      <c r="B211" s="77"/>
+      <c r="C211" s="78"/>
     </row>
     <row r="212" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
       <c r="A212" s="35"/>
       <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A213" s="74" t="s">
+      <c r="A213" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="B213" s="75"/>
-      <c r="C213" s="76"/>
+      <c r="B213" s="77"/>
+      <c r="C213" s="78"/>
     </row>
     <row r="214" spans="1:3" s="25" customFormat="1">
       <c r="A214" s="33" t="s">
@@ -3003,11 +3013,11 @@
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="74" t="s">
+      <c r="A221" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="B221" s="75"/>
-      <c r="C221" s="76"/>
+      <c r="B221" s="77"/>
+      <c r="C221" s="78"/>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="33" t="s">
@@ -3023,11 +3033,11 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A224" s="74" t="s">
+      <c r="A224" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="B224" s="75"/>
-      <c r="C224" s="76"/>
+      <c r="B224" s="77"/>
+      <c r="C224" s="78"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="33" t="s">
@@ -3041,11 +3051,11 @@
     </row>
     <row r="228" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="229" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A229" s="74" t="s">
+      <c r="A229" s="76" t="s">
         <v>241</v>
       </c>
-      <c r="B229" s="75"/>
-      <c r="C229" s="76"/>
+      <c r="B229" s="77"/>
+      <c r="C229" s="78"/>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="33" t="s">
@@ -3064,11 +3074,11 @@
     </row>
     <row r="234" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="235" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A235" s="74" t="s">
+      <c r="A235" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="B235" s="75"/>
-      <c r="C235" s="76"/>
+      <c r="B235" s="77"/>
+      <c r="C235" s="78"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="33" t="s">
@@ -3101,11 +3111,11 @@
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="74" t="s">
+      <c r="A241" s="76" t="s">
         <v>273</v>
       </c>
-      <c r="B241" s="75"/>
-      <c r="C241" s="76"/>
+      <c r="B241" s="77"/>
+      <c r="C241" s="78"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
@@ -3120,11 +3130,11 @@
     </row>
     <row r="244" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="245" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A245" s="74" t="s">
+      <c r="A245" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="B245" s="75"/>
-      <c r="C245" s="76"/>
+      <c r="B245" s="77"/>
+      <c r="C245" s="78"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="33" t="s">
@@ -3143,10 +3153,10 @@
       <c r="A248" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B248" s="79" t="s">
+      <c r="B248" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C248" s="80"/>
+      <c r="C248" s="83"/>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="33" t="s">
@@ -3156,11 +3166,11 @@
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="251" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A251" s="74" t="s">
+      <c r="A251" s="76" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="75"/>
-      <c r="C251" s="76"/>
+      <c r="B251" s="77"/>
+      <c r="C251" s="78"/>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="33" t="s">
@@ -3173,11 +3183,11 @@
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A254" s="74" t="s">
+      <c r="A254" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="B254" s="75"/>
-      <c r="C254" s="76"/>
+      <c r="B254" s="77"/>
+      <c r="C254" s="78"/>
     </row>
     <row r="255" spans="1:3" ht="30">
       <c r="A255" s="33" t="s">
@@ -3199,11 +3209,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="74" t="s">
+      <c r="A259" s="76" t="s">
         <v>259</v>
       </c>
-      <c r="B259" s="75"/>
-      <c r="C259" s="76"/>
+      <c r="B259" s="77"/>
+      <c r="C259" s="78"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="33" t="s">
@@ -3230,8 +3240,13 @@
       </c>
     </row>
     <row r="263" spans="1:3" s="57" customFormat="1">
-      <c r="A263" s="58"/>
+      <c r="A263" s="74" t="s">
+        <v>335</v>
+      </c>
       <c r="B263" s="58"/>
+      <c r="C263" s="75" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="264" spans="1:3" s="57" customFormat="1">
       <c r="A264" s="58"/>
@@ -3242,14 +3257,14 @@
       <c r="B265" s="58"/>
     </row>
     <row r="266" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A266" s="74" t="s">
+      <c r="A266" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B266" s="75"/>
-      <c r="C266" s="76"/>
+      <c r="B266" s="77"/>
+      <c r="C266" s="78"/>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" s="77" t="s">
+      <c r="A267" s="80" t="s">
         <v>40</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -3260,18 +3275,18 @@
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="78"/>
+      <c r="A268" s="81"/>
       <c r="B268" s="31" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="270" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A270" s="74" t="s">
+      <c r="A270" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="B270" s="75"/>
-      <c r="C270" s="76"/>
+      <c r="B270" s="77"/>
+      <c r="C270" s="78"/>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="33" t="s">
@@ -3305,11 +3320,11 @@
     </row>
     <row r="277" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="278" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A278" s="74" t="s">
+      <c r="A278" s="76" t="s">
         <v>289</v>
       </c>
-      <c r="B278" s="75"/>
-      <c r="C278" s="76"/>
+      <c r="B278" s="77"/>
+      <c r="C278" s="78"/>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="40" t="s">
@@ -3326,11 +3341,11 @@
     </row>
     <row r="281" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A282" s="74" t="s">
+      <c r="A282" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="B282" s="75"/>
-      <c r="C282" s="76"/>
+      <c r="B282" s="77"/>
+      <c r="C282" s="78"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="44" t="s">
@@ -3364,11 +3379,11 @@
     </row>
     <row r="289" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="290" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A290" s="74" t="s">
+      <c r="A290" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="B290" s="75"/>
-      <c r="C290" s="76"/>
+      <c r="B290" s="77"/>
+      <c r="C290" s="78"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="45" t="s">
@@ -3377,11 +3392,11 @@
     </row>
     <row r="292" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="293" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A293" s="74" t="s">
+      <c r="A293" s="76" t="s">
         <v>314</v>
       </c>
-      <c r="B293" s="75"/>
-      <c r="C293" s="76"/>
+      <c r="B293" s="77"/>
+      <c r="C293" s="78"/>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="63" t="s">
@@ -3391,11 +3406,11 @@
     </row>
     <row r="296" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="297" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A297" s="74" t="s">
+      <c r="A297" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="B297" s="75"/>
-      <c r="C297" s="76"/>
+      <c r="B297" s="77"/>
+      <c r="C297" s="78"/>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="54" t="s">
@@ -3404,11 +3419,11 @@
     </row>
     <row r="300" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="301" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A301" s="74" t="s">
+      <c r="A301" s="76" t="s">
         <v>310</v>
       </c>
-      <c r="B301" s="75"/>
-      <c r="C301" s="76"/>
+      <c r="B301" s="77"/>
+      <c r="C301" s="78"/>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="61" t="s">
@@ -3463,11 +3478,11 @@
     </row>
     <row r="311" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="312" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A312" s="74" t="s">
+      <c r="A312" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="B312" s="75"/>
-      <c r="C312" s="76"/>
+      <c r="B312" s="77"/>
+      <c r="C312" s="78"/>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="33" t="s">
@@ -3502,11 +3517,11 @@
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A319" s="74" t="s">
+      <c r="A319" s="76" t="s">
         <v>320</v>
       </c>
-      <c r="B319" s="75"/>
-      <c r="C319" s="76"/>
+      <c r="B319" s="77"/>
+      <c r="C319" s="78"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="68" t="s">
@@ -3547,14 +3562,36 @@
     </row>
     <row r="325" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="326" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A326" s="74" t="s">
+      <c r="A326" s="76" t="s">
         <v>331</v>
       </c>
-      <c r="B326" s="75"/>
-      <c r="C326" s="76"/>
+      <c r="B326" s="77"/>
+      <c r="C326" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A312:C312"/>
+    <mergeCell ref="A301:C301"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A297:C297"/>
+    <mergeCell ref="A241:C241"/>
+    <mergeCell ref="A293:C293"/>
+    <mergeCell ref="A282:C282"/>
+    <mergeCell ref="A270:C270"/>
+    <mergeCell ref="A290:C290"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A229:C229"/>
+    <mergeCell ref="A235:C235"/>
+    <mergeCell ref="A267:A268"/>
+    <mergeCell ref="B248:C248"/>
+    <mergeCell ref="A198:C198"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A266:C266"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A254:C254"/>
+    <mergeCell ref="A221:C221"/>
     <mergeCell ref="A326:C326"/>
     <mergeCell ref="A319:C319"/>
     <mergeCell ref="A124:C124"/>
@@ -3571,28 +3608,6 @@
     <mergeCell ref="A278:C278"/>
     <mergeCell ref="A193:C193"/>
     <mergeCell ref="A251:C251"/>
-    <mergeCell ref="A198:C198"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="A211:C211"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A266:C266"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A254:C254"/>
-    <mergeCell ref="A221:C221"/>
-    <mergeCell ref="A312:C312"/>
-    <mergeCell ref="A301:C301"/>
-    <mergeCell ref="A213:C213"/>
-    <mergeCell ref="A297:C297"/>
-    <mergeCell ref="A241:C241"/>
-    <mergeCell ref="A293:C293"/>
-    <mergeCell ref="A282:C282"/>
-    <mergeCell ref="A270:C270"/>
-    <mergeCell ref="A290:C290"/>
-    <mergeCell ref="A224:C224"/>
-    <mergeCell ref="A229:C229"/>
-    <mergeCell ref="A235:C235"/>
-    <mergeCell ref="A267:A268"/>
-    <mergeCell ref="B248:C248"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>

<commit_message>
TypeScript, Spring, Angular, React
</commit_message>
<xml_diff>
--- a/Definitions/1_Grand_Definitions.xlsx
+++ b/Definitions/1_Grand_Definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="338">
   <si>
     <t>OOPS concepts</t>
   </si>
@@ -1040,6 +1040,9 @@
   </si>
   <si>
     <t>y_Definitions_React_JS.xlsx</t>
+  </si>
+  <si>
+    <t>Typescript</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1343,6 +1346,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1352,7 +1359,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1365,6 +1371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1663,8 +1670,8 @@
   <dimension ref="A1:D326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2478,11 +2485,11 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A124" s="76" t="s">
+      <c r="A124" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="77"/>
-      <c r="C124" s="78"/>
+      <c r="B124" s="79"/>
+      <c r="C124" s="80"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
@@ -2520,11 +2527,11 @@
       <c r="B130" s="30"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A131" s="76" t="s">
+      <c r="A131" s="78" t="s">
         <v>215</v>
       </c>
-      <c r="B131" s="77"/>
-      <c r="C131" s="78"/>
+      <c r="B131" s="79"/>
+      <c r="C131" s="80"/>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="33" t="s">
@@ -2586,11 +2593,11 @@
       <c r="B139" s="60"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A140" s="76" t="s">
+      <c r="A140" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="B140" s="77"/>
-      <c r="C140" s="78"/>
+      <c r="B140" s="79"/>
+      <c r="C140" s="80"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="33" t="s">
@@ -2635,11 +2642,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A146" s="76" t="s">
+      <c r="A146" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="B146" s="77"/>
-      <c r="C146" s="78"/>
+      <c r="B146" s="79"/>
+      <c r="C146" s="80"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="33" t="s">
@@ -2651,11 +2658,11 @@
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="154" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A154" s="76" t="s">
+      <c r="A154" s="78" t="s">
         <v>213</v>
       </c>
-      <c r="B154" s="77"/>
-      <c r="C154" s="78"/>
+      <c r="B154" s="79"/>
+      <c r="C154" s="80"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="33" t="s">
@@ -2713,11 +2720,11 @@
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="164" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A164" s="76" t="s">
+      <c r="A164" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="77"/>
-      <c r="C164" s="78"/>
+      <c r="B164" s="79"/>
+      <c r="C164" s="80"/>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="33" t="s">
@@ -2734,14 +2741,14 @@
       <c r="B166" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C166" s="79"/>
+      <c r="C166" s="85"/>
     </row>
     <row r="167" spans="1:3" s="22" customFormat="1" ht="30">
       <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C167" s="79"/>
+      <c r="C167" s="85"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="42" t="s">
@@ -2750,11 +2757,11 @@
     </row>
     <row r="170" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="171" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A171" s="76" t="s">
+      <c r="A171" s="78" t="s">
         <v>211</v>
       </c>
-      <c r="B171" s="77"/>
-      <c r="C171" s="78"/>
+      <c r="B171" s="79"/>
+      <c r="C171" s="80"/>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="33" t="s">
@@ -2789,11 +2796,11 @@
       <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A179" s="76" t="s">
+      <c r="A179" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="B179" s="77"/>
-      <c r="C179" s="78"/>
+      <c r="B179" s="79"/>
+      <c r="C179" s="80"/>
     </row>
     <row r="180" spans="1:3" s="37" customFormat="1">
       <c r="A180" s="36" t="s">
@@ -2818,11 +2825,11 @@
       <c r="B183" s="36"/>
     </row>
     <row r="184" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A184" s="76" t="s">
+      <c r="A184" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="B184" s="77"/>
-      <c r="C184" s="78"/>
+      <c r="B184" s="79"/>
+      <c r="C184" s="80"/>
     </row>
     <row r="185" spans="1:3" s="37" customFormat="1">
       <c r="A185" s="36" t="s">
@@ -2847,11 +2854,11 @@
       <c r="B188" s="36"/>
     </row>
     <row r="189" spans="1:3" s="37" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A189" s="76" t="s">
+      <c r="A189" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="B189" s="77"/>
-      <c r="C189" s="78"/>
+      <c r="B189" s="79"/>
+      <c r="C189" s="80"/>
     </row>
     <row r="190" spans="1:3" s="37" customFormat="1">
       <c r="A190" s="36" t="s">
@@ -2868,11 +2875,11 @@
       <c r="B192" s="36"/>
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A193" s="76" t="s">
+      <c r="A193" s="78" t="s">
         <v>212</v>
       </c>
-      <c r="B193" s="77"/>
-      <c r="C193" s="78"/>
+      <c r="B193" s="79"/>
+      <c r="C193" s="80"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="33" t="s">
@@ -2888,11 +2895,11 @@
     </row>
     <row r="197" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="198" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A198" s="76" t="s">
+      <c r="A198" s="78" t="s">
         <v>219</v>
       </c>
-      <c r="B198" s="77"/>
-      <c r="C198" s="78"/>
+      <c r="B198" s="79"/>
+      <c r="C198" s="80"/>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="33" t="s">
@@ -2932,11 +2939,11 @@
       <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A206" s="76" t="s">
+      <c r="A206" s="78" t="s">
         <v>222</v>
       </c>
-      <c r="B206" s="77"/>
-      <c r="C206" s="78"/>
+      <c r="B206" s="79"/>
+      <c r="C206" s="80"/>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="33" t="s">
@@ -2961,22 +2968,22 @@
       <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A211" s="76" t="s">
+      <c r="A211" s="78" t="s">
         <v>223</v>
       </c>
-      <c r="B211" s="77"/>
-      <c r="C211" s="78"/>
+      <c r="B211" s="79"/>
+      <c r="C211" s="80"/>
     </row>
     <row r="212" spans="1:3" s="25" customFormat="1" ht="15.75" thickBot="1">
       <c r="A212" s="35"/>
       <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A213" s="76" t="s">
+      <c r="A213" s="78" t="s">
         <v>231</v>
       </c>
-      <c r="B213" s="77"/>
-      <c r="C213" s="78"/>
+      <c r="B213" s="79"/>
+      <c r="C213" s="80"/>
     </row>
     <row r="214" spans="1:3" s="25" customFormat="1">
       <c r="A214" s="33" t="s">
@@ -3013,11 +3020,11 @@
     </row>
     <row r="220" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="221" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A221" s="76" t="s">
+      <c r="A221" s="78" t="s">
         <v>234</v>
       </c>
-      <c r="B221" s="77"/>
-      <c r="C221" s="78"/>
+      <c r="B221" s="79"/>
+      <c r="C221" s="80"/>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="33" t="s">
@@ -3033,11 +3040,11 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A224" s="76" t="s">
+      <c r="A224" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="B224" s="77"/>
-      <c r="C224" s="78"/>
+      <c r="B224" s="79"/>
+      <c r="C224" s="80"/>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="33" t="s">
@@ -3051,11 +3058,11 @@
     </row>
     <row r="228" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="229" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A229" s="76" t="s">
+      <c r="A229" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="B229" s="77"/>
-      <c r="C229" s="78"/>
+      <c r="B229" s="79"/>
+      <c r="C229" s="80"/>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="33" t="s">
@@ -3074,11 +3081,11 @@
     </row>
     <row r="234" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="235" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A235" s="76" t="s">
+      <c r="A235" s="78" t="s">
         <v>242</v>
       </c>
-      <c r="B235" s="77"/>
-      <c r="C235" s="78"/>
+      <c r="B235" s="79"/>
+      <c r="C235" s="80"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="33" t="s">
@@ -3111,11 +3118,11 @@
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A241" s="76" t="s">
+      <c r="A241" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="B241" s="77"/>
-      <c r="C241" s="78"/>
+      <c r="B241" s="79"/>
+      <c r="C241" s="80"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="33" t="s">
@@ -3130,11 +3137,11 @@
     </row>
     <row r="244" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="245" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A245" s="76" t="s">
+      <c r="A245" s="78" t="s">
         <v>249</v>
       </c>
-      <c r="B245" s="77"/>
-      <c r="C245" s="78"/>
+      <c r="B245" s="79"/>
+      <c r="C245" s="80"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="33" t="s">
@@ -3153,10 +3160,10 @@
       <c r="A248" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B248" s="82" t="s">
+      <c r="B248" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C248" s="83"/>
+      <c r="C248" s="84"/>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="33" t="s">
@@ -3166,11 +3173,11 @@
     </row>
     <row r="250" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="251" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A251" s="76" t="s">
+      <c r="A251" s="78" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="77"/>
-      <c r="C251" s="78"/>
+      <c r="B251" s="79"/>
+      <c r="C251" s="80"/>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="33" t="s">
@@ -3183,11 +3190,11 @@
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A254" s="76" t="s">
+      <c r="A254" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="B254" s="77"/>
-      <c r="C254" s="78"/>
+      <c r="B254" s="79"/>
+      <c r="C254" s="80"/>
     </row>
     <row r="255" spans="1:3" ht="30">
       <c r="A255" s="33" t="s">
@@ -3209,11 +3216,11 @@
     </row>
     <row r="258" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="259" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A259" s="76" t="s">
+      <c r="A259" s="78" t="s">
         <v>259</v>
       </c>
-      <c r="B259" s="77"/>
-      <c r="C259" s="78"/>
+      <c r="B259" s="79"/>
+      <c r="C259" s="80"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="33" t="s">
@@ -3249,22 +3256,27 @@
       </c>
     </row>
     <row r="264" spans="1:3" s="57" customFormat="1">
-      <c r="A264" s="58"/>
+      <c r="A264" s="77" t="s">
+        <v>337</v>
+      </c>
       <c r="B264" s="58"/>
+      <c r="C264" s="76" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="265" spans="1:3" s="57" customFormat="1" ht="15.75" thickBot="1">
       <c r="A265" s="58"/>
       <c r="B265" s="58"/>
     </row>
     <row r="266" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A266" s="76" t="s">
+      <c r="A266" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="B266" s="77"/>
-      <c r="C266" s="78"/>
+      <c r="B266" s="79"/>
+      <c r="C266" s="80"/>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" s="80" t="s">
+      <c r="A267" s="81" t="s">
         <v>40</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -3275,18 +3287,18 @@
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="81"/>
+      <c r="A268" s="82"/>
       <c r="B268" s="31" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="270" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A270" s="76" t="s">
+      <c r="A270" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="B270" s="77"/>
-      <c r="C270" s="78"/>
+      <c r="B270" s="79"/>
+      <c r="C270" s="80"/>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="33" t="s">
@@ -3320,11 +3332,11 @@
     </row>
     <row r="277" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="278" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A278" s="76" t="s">
+      <c r="A278" s="78" t="s">
         <v>289</v>
       </c>
-      <c r="B278" s="77"/>
-      <c r="C278" s="78"/>
+      <c r="B278" s="79"/>
+      <c r="C278" s="80"/>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="40" t="s">
@@ -3341,11 +3353,11 @@
     </row>
     <row r="281" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A282" s="76" t="s">
+      <c r="A282" s="78" t="s">
         <v>291</v>
       </c>
-      <c r="B282" s="77"/>
-      <c r="C282" s="78"/>
+      <c r="B282" s="79"/>
+      <c r="C282" s="80"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="44" t="s">
@@ -3379,11 +3391,11 @@
     </row>
     <row r="289" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="290" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A290" s="76" t="s">
+      <c r="A290" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="B290" s="77"/>
-      <c r="C290" s="78"/>
+      <c r="B290" s="79"/>
+      <c r="C290" s="80"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="45" t="s">
@@ -3392,11 +3404,11 @@
     </row>
     <row r="292" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="293" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A293" s="76" t="s">
+      <c r="A293" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="B293" s="77"/>
-      <c r="C293" s="78"/>
+      <c r="B293" s="79"/>
+      <c r="C293" s="80"/>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="63" t="s">
@@ -3406,11 +3418,11 @@
     </row>
     <row r="296" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="297" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A297" s="76" t="s">
+      <c r="A297" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="B297" s="77"/>
-      <c r="C297" s="78"/>
+      <c r="B297" s="79"/>
+      <c r="C297" s="80"/>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="54" t="s">
@@ -3419,11 +3431,11 @@
     </row>
     <row r="300" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="301" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A301" s="76" t="s">
+      <c r="A301" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="B301" s="77"/>
-      <c r="C301" s="78"/>
+      <c r="B301" s="79"/>
+      <c r="C301" s="80"/>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="61" t="s">
@@ -3478,11 +3490,11 @@
     </row>
     <row r="311" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="312" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A312" s="76" t="s">
+      <c r="A312" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="B312" s="77"/>
-      <c r="C312" s="78"/>
+      <c r="B312" s="79"/>
+      <c r="C312" s="80"/>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="33" t="s">
@@ -3517,11 +3529,11 @@
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A319" s="76" t="s">
+      <c r="A319" s="78" t="s">
         <v>320</v>
       </c>
-      <c r="B319" s="77"/>
-      <c r="C319" s="78"/>
+      <c r="B319" s="79"/>
+      <c r="C319" s="80"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="68" t="s">
@@ -3562,36 +3574,14 @@
     </row>
     <row r="325" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="326" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A326" s="76" t="s">
+      <c r="A326" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="B326" s="77"/>
-      <c r="C326" s="78"/>
+      <c r="B326" s="79"/>
+      <c r="C326" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A312:C312"/>
-    <mergeCell ref="A301:C301"/>
-    <mergeCell ref="A213:C213"/>
-    <mergeCell ref="A297:C297"/>
-    <mergeCell ref="A241:C241"/>
-    <mergeCell ref="A293:C293"/>
-    <mergeCell ref="A282:C282"/>
-    <mergeCell ref="A270:C270"/>
-    <mergeCell ref="A290:C290"/>
-    <mergeCell ref="A224:C224"/>
-    <mergeCell ref="A229:C229"/>
-    <mergeCell ref="A235:C235"/>
-    <mergeCell ref="A267:A268"/>
-    <mergeCell ref="B248:C248"/>
-    <mergeCell ref="A198:C198"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="A211:C211"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A266:C266"/>
-    <mergeCell ref="A259:C259"/>
-    <mergeCell ref="A254:C254"/>
-    <mergeCell ref="A221:C221"/>
     <mergeCell ref="A326:C326"/>
     <mergeCell ref="A319:C319"/>
     <mergeCell ref="A124:C124"/>
@@ -3608,6 +3598,28 @@
     <mergeCell ref="A278:C278"/>
     <mergeCell ref="A193:C193"/>
     <mergeCell ref="A251:C251"/>
+    <mergeCell ref="A198:C198"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A266:C266"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A254:C254"/>
+    <mergeCell ref="A221:C221"/>
+    <mergeCell ref="A312:C312"/>
+    <mergeCell ref="A301:C301"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A297:C297"/>
+    <mergeCell ref="A241:C241"/>
+    <mergeCell ref="A293:C293"/>
+    <mergeCell ref="A282:C282"/>
+    <mergeCell ref="A270:C270"/>
+    <mergeCell ref="A290:C290"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A229:C229"/>
+    <mergeCell ref="A235:C235"/>
+    <mergeCell ref="A267:A268"/>
+    <mergeCell ref="B248:C248"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>

</xml_diff>